<commit_message>
Updated for ReducePred4 - Attempt to fix crashing fish groups
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Group Condition" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group Condition'!$A$1:$G$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recruitment_Log!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recruitment_Log!$A$1:$K$68</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="202">
   <si>
     <t>Too High</t>
   </si>
@@ -626,6 +626,15 @@
   </si>
   <si>
     <t>RemovePred3_NewKDENR</t>
+  </si>
+  <si>
+    <t>RemovePred4_KDENR</t>
+  </si>
+  <si>
+    <t>RemovePred4_Changed</t>
+  </si>
+  <si>
+    <t>RemovePred3_FinalKDENR</t>
   </si>
 </sst>
 </file>
@@ -661,7 +670,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -714,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -723,24 +732,29 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,11 +1035,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,62 +1077,59 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="G4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E6" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
       <c r="F6" t="s">
         <v>181</v>
@@ -1125,19 +1137,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1148,24 +1157,18 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>113</v>
       </c>
-      <c r="C9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E9" t="s">
-        <v>181</v>
-      </c>
       <c r="F9" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1179,23 +1182,23 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
-      </c>
-      <c r="G11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="F11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="F12" t="s">
         <v>181</v>
@@ -1203,43 +1206,49 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>177</v>
-      </c>
-      <c r="G13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="G14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="D15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>107</v>
+      </c>
+      <c r="E16" t="s">
+        <v>181</v>
       </c>
       <c r="F16" t="s">
         <v>181</v>
@@ -1247,302 +1256,293 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" t="s">
-        <v>181</v>
-      </c>
-      <c r="F18" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
         <v>181</v>
       </c>
-      <c r="E19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>165</v>
+      </c>
+      <c r="G22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+      <c r="G23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>171</v>
       </c>
-      <c r="G20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" t="s">
-        <v>178</v>
-      </c>
-      <c r="D21" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>179</v>
-      </c>
-      <c r="G23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
-      </c>
-      <c r="G25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="C25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="G26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
-      </c>
-      <c r="E27" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="F27" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="G28" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="F29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>53</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>142</v>
       </c>
-      <c r="C30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="F33" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
-      </c>
-      <c r="G34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="F34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
-      </c>
-      <c r="G35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="D35" t="s">
+        <v>181</v>
+      </c>
+      <c r="F35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>169</v>
-      </c>
-      <c r="F36" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>177</v>
+      </c>
+      <c r="G38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B42" t="s">
         <v>131</v>
       </c>
-      <c r="C37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" t="s">
-        <v>166</v>
-      </c>
-      <c r="D39" t="s">
-        <v>183</v>
-      </c>
-      <c r="E39" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" t="s">
-        <v>159</v>
-      </c>
-      <c r="F40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" t="s">
-        <v>93</v>
-      </c>
-      <c r="F41" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" t="s">
-        <v>108</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="F42" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1560,92 +1560,89 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>143</v>
       </c>
-      <c r="C44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" t="s">
+        <v>162</v>
+      </c>
+      <c r="G45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>35</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>124</v>
       </c>
-      <c r="C45" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" t="s">
-        <v>163</v>
-      </c>
-      <c r="G46" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
-      </c>
-      <c r="G47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="F47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
-      </c>
-      <c r="G48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>170</v>
-      </c>
-      <c r="G49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="F49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="F50" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
-      </c>
-      <c r="E51" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="G51" t="s">
         <v>181</v>
@@ -1653,237 +1650,231 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
-      </c>
-      <c r="G52" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="C52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="G53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" t="s">
+        <v>163</v>
+      </c>
+      <c r="G54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="G55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" t="s">
+        <v>175</v>
+      </c>
+      <c r="G56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>83</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B57" t="s">
         <v>172</v>
       </c>
-      <c r="G53" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" t="s">
-        <v>140</v>
-      </c>
-      <c r="G54" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" t="s">
-        <v>162</v>
-      </c>
-      <c r="G55" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" t="s">
-        <v>123</v>
-      </c>
       <c r="G57" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>160</v>
-      </c>
-      <c r="C58" t="s">
-        <v>181</v>
-      </c>
-      <c r="E58" t="s">
+        <v>145</v>
+      </c>
+      <c r="G58" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
-      </c>
-      <c r="E59" t="s">
-        <v>181</v>
-      </c>
-      <c r="G59" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="C59" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
-      </c>
-      <c r="C60" t="s">
+        <v>139</v>
+      </c>
+      <c r="G60" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>155</v>
-      </c>
-      <c r="F61" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="C61" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="G62" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>157</v>
-      </c>
-      <c r="F63" t="s">
+        <v>179</v>
+      </c>
+      <c r="G63" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
-      </c>
-      <c r="F64" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>154</v>
-      </c>
-      <c r="F65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C66" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
-      </c>
-      <c r="E67" t="s">
-        <v>181</v>
-      </c>
-      <c r="G67" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="F67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>167</v>
-      </c>
-      <c r="C68" t="s">
+        <v>144</v>
+      </c>
+      <c r="G68" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
-      </c>
-      <c r="C70" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="G70" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>27</v>
       </c>
       <c r="B71" t="s">
         <v>114</v>
       </c>
-      <c r="E71" t="s">
-        <v>181</v>
-      </c>
       <c r="F71" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -1894,45 +1885,51 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" t="s">
+        <v>116</v>
+      </c>
+      <c r="F73" t="s">
+        <v>181</v>
+      </c>
+      <c r="G73" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>60</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>149</v>
       </c>
-      <c r="G73" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>39</v>
-      </c>
-      <c r="B74" t="s">
-        <v>128</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="G74" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
-      </c>
-      <c r="G75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>134</v>
+      </c>
+      <c r="C76" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -1951,74 +1948,68 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>181</v>
-      </c>
-      <c r="G78" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="C79" t="s">
+        <v>181</v>
+      </c>
+      <c r="F79" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B80" t="s">
-        <v>129</v>
-      </c>
-      <c r="E80" t="s">
-        <v>181</v>
-      </c>
-      <c r="G80" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="C80" t="s">
+        <v>181</v>
+      </c>
+      <c r="F80" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B82" t="s">
-        <v>98</v>
-      </c>
-      <c r="C82" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="F82" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F83" t="s">
         <v>181</v>
@@ -2026,52 +2017,46 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="C84" t="s">
-        <v>181</v>
-      </c>
-      <c r="F84" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" t="s">
+        <v>141</v>
+      </c>
+      <c r="C85" t="s">
+        <v>181</v>
+      </c>
+      <c r="F85" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>17</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>100</v>
       </c>
-      <c r="F85" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>44</v>
-      </c>
-      <c r="B86" t="s">
-        <v>133</v>
-      </c>
-      <c r="C86" t="s">
-        <v>181</v>
-      </c>
-      <c r="E86" t="s">
-        <v>181</v>
-      </c>
       <c r="F86" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="G87" t="s">
         <v>181</v>
@@ -2079,18 +2064,26 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
-      </c>
-      <c r="G88" t="s">
+        <v>133</v>
+      </c>
+      <c r="C88" t="s">
+        <v>181</v>
+      </c>
+      <c r="F88" t="s">
         <v>181</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G88">
-    <sortState ref="A6:G86">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <sortState ref="A2:G88">
       <sortCondition ref="B1:B88"/>
     </sortState>
   </autoFilter>
@@ -2100,13 +2093,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2116,1808 +2110,2449 @@
     <col min="3" max="3" width="27.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="20" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="4" t="s">
         <v>194</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="I1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="7">
         <v>1001094433</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>15</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>66739628.866666667</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="11">
         <v>66739628</v>
       </c>
-      <c r="G2" s="9"/>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H33" si="0">IF(ISBLANK(G2),F2,F2/G2)</f>
+        <f>IF(ISBLANK(G2),F2,F2/G2)</f>
         <v>66739628</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="I2" s="3">
+        <v>45700000</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3">
+        <v>45700000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="7">
         <v>20527442.649999999</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>10</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>2052744.2649999999</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="11">
         <v>2052744.2649999999</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="4">
         <v>4</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G3),F3,F3/G3)</f>
         <v>513186.06624999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="I3" s="3">
+        <v>22700000</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3">
+        <v>22700000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="7">
         <v>114181041.2</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="D4" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="11">
         <v>19030173</v>
       </c>
-      <c r="G4" s="9"/>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G4),F4,F4/G4)</f>
         <v>19030173</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="I4" s="3">
+        <v>19030173</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f t="shared" ref="J3:J66" si="0">IF(H4=I4,"",1)</f>
+        <v/>
+      </c>
+      <c r="K4" s="3">
+        <v>19030173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="7">
         <v>15816.31169</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="D5" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" s="11">
         <v>15816.31169</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="4">
         <v>0.25</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G5),F5,F5/G5)</f>
         <v>63265.246760000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="I5" s="3">
+        <v>63265</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>63265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="7">
         <v>16477555.609999999</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>7</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>2353936.5157142854</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="11">
         <v>2353936.5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="4">
         <v>5</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G6),F6,F6/G6)</f>
         <v>470787.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="I6" s="3">
+        <v>470787</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="11">
+        <v>2353936.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="7">
         <v>254421.22440000001</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>150</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>1696.141496</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="11">
         <v>1696.14</v>
       </c>
-      <c r="G7" s="9"/>
       <c r="H7" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G7),F7,F7/G7)</f>
         <v>1696.14</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="I7" s="3">
+        <v>1696.14</v>
+      </c>
+      <c r="J7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K7" s="3">
+        <v>1696.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="8">
         <v>229000000000</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="D8" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8" s="11">
         <v>500000000000</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="4">
         <v>0.5</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G8),F8,F8/G8)</f>
         <v>1000000000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="I8" s="3">
+        <v>1000000000000</v>
+      </c>
+      <c r="J8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K8" s="3">
+        <v>1000000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="7">
         <v>32122718.550000001</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="D9" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F9" s="11">
         <v>3212271805.0500002</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="4">
         <v>15</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G9),F9,F9/G9)</f>
         <v>214151453.67000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="I9" s="3">
+        <v>214151453</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>3212271805.0500002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="7">
         <v>2123.8950410000002</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="D10" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F10" s="11">
         <v>2123.8950410000002</v>
       </c>
-      <c r="G10" s="9"/>
       <c r="H10" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G10),F10,F10/G10)</f>
         <v>2123.8950410000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="I10" s="3">
+        <v>2123.8950410000002</v>
+      </c>
+      <c r="J10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K10" s="3">
+        <v>2123.8950410000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="7">
         <v>74822.192989999996</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="D11" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F11" s="11">
         <v>74822.192989999996</v>
       </c>
-      <c r="G11" s="9"/>
       <c r="H11" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G11),F11,F11/G11)</f>
         <v>74822.192989999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="I11" s="3">
+        <v>74822.192989999996</v>
+      </c>
+      <c r="J11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K11" s="11">
+        <v>74822.192989999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="7">
         <v>235.45910710000001</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="D12" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F12" s="11">
         <v>235.45910710000001</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="4">
         <v>10</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G12),F12,F12/G12)</f>
         <v>23.545910710000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="I12" s="3">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <v>23.545910710000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="7">
         <v>25797.24295</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>100</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>257.97242949999998</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="11">
         <v>257.97000000000003</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="4">
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G13),F13,F13/G13)</f>
         <v>51.594000000000008</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="I13" s="3">
+        <v>51</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="7">
         <v>1718757.3940000001</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="D14" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" s="11">
         <v>1718757.3940000001</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="4">
         <v>75</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G14),F14,F14/G14)</f>
         <v>22916.765253333335</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="I14" s="3">
+        <v>36100000000</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>36100000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="7">
         <v>15874.27808</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="D15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F15" s="11">
         <v>15874.27808</v>
       </c>
-      <c r="G15" s="9"/>
       <c r="H15" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G15),F15,F15/G15)</f>
         <v>15874.27808</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="I15" s="3">
+        <v>15874.27808</v>
+      </c>
+      <c r="J15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K15" s="3">
+        <v>15874.27808</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="7">
         <v>2124041.1490000002</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="D16" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F16" s="11">
         <v>2124041.1490000002</v>
       </c>
-      <c r="G16" s="9"/>
       <c r="H16" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G16),F16,F16/G16)</f>
         <v>2124041.1490000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="I16" s="3">
+        <v>46100000</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="5">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="7">
         <v>21996106.07</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="D17" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F17" s="11">
         <v>21996106.07</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="4">
         <v>10</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G17),F17,F17/G17)</f>
         <v>2199610.6069999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="I17" s="3">
+        <v>8700000</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="5">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="7">
         <v>129309.07709999999</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="D18" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F18" s="11">
         <v>129309</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="4">
         <v>10</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G18),F18,F18/G18)</f>
         <v>12930.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="I18" s="3">
+        <v>12930</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>12930.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="7">
         <v>13236869.029999999</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>10</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>1323686.9029999999</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="11">
         <v>1323686.8999999999</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="4">
         <v>7</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G19),F19,F19/G19)</f>
         <v>189098.12857142856</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="I19" s="3">
+        <v>189098</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>189098.12857142856</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="7">
         <v>172649603.19999999</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>34529920.600000001</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="11">
         <v>34529920</v>
       </c>
-      <c r="G20" s="9"/>
       <c r="H20" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G20),F20,F20/G20)</f>
         <v>34529920</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="I20" s="3">
+        <v>104000000</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3">
+        <v>104000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="7">
         <v>0.05</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="D21" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" s="11">
         <v>3.3300000000000001E-3</v>
       </c>
-      <c r="G21" s="9"/>
       <c r="H21" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G21),F21,F21/G21)</f>
         <v>3.3300000000000001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="I21" s="3">
+        <v>3.3300000000000001E-3</v>
+      </c>
+      <c r="J21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K21" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="7">
         <v>0.05</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="D22" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="11">
         <v>3.3300000000000001E-3</v>
       </c>
-      <c r="G22" s="9"/>
       <c r="H22" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G22),F22,F22/G22)</f>
         <v>3.3300000000000001E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="I22" s="3">
+        <v>3.3300000000000001E-3</v>
+      </c>
+      <c r="J22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K22" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="7">
         <v>747577.53830000001</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>149515.50766</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="11">
         <v>149515.5</v>
       </c>
-      <c r="G23" s="9"/>
       <c r="H23" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G23),F23,F23/G23)</f>
         <v>149515.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="I23" s="3">
+        <v>149515.5</v>
+      </c>
+      <c r="J23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K23" s="3">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="7">
         <v>15150975.09</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>8</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>1893871.875</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="11">
         <v>1893871.875</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="4">
         <v>10</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G24),F24,F24/G24)</f>
         <v>189387.1875</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="I24" s="3">
+        <v>189387</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="3">
+        <v>378774.375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="7">
         <v>0.05</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="D25" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F25" s="11">
         <v>0.01</v>
       </c>
-      <c r="G25" s="9"/>
       <c r="H25" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G25),F25,F25/G25)</f>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="I25" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="J25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K25" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="7">
         <v>0.05</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F26" s="8">
+      <c r="D26" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F26" s="11">
         <v>0.01</v>
       </c>
-      <c r="G26" s="9"/>
       <c r="H26" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G26),F26,F26/G26)</f>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="I26" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="J26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K26" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="7">
         <v>932233758.39999998</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F27" s="8">
+      <c r="D27" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F27" s="11">
         <v>100000000</v>
       </c>
-      <c r="G27" s="9"/>
       <c r="H27" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G27),F27,F27/G27)</f>
         <v>100000000</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="I27" s="3">
+        <v>181000000</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2</v>
+      </c>
+      <c r="K27" s="3">
+        <v>181000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="7">
         <v>749.83099549999997</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F28" s="8">
+      <c r="D28" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F28" s="11">
         <v>749.83099549999997</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="4">
         <v>2</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G28),F28,F28/G28)</f>
         <v>374.91549774999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="I28" s="3">
+        <v>375</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="7">
         <v>4986608.142</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F29" s="8">
+      <c r="D29" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F29" s="11">
         <v>4986608.142</v>
       </c>
-      <c r="G29" s="9"/>
       <c r="H29" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G29),F29,F29/G29)</f>
         <v>4986608.142</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="I29" s="3">
+        <v>4986608.142</v>
+      </c>
+      <c r="J29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K29" s="3">
+        <v>4986608.142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="7">
         <v>174418341.5</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>5</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>34883668.299999997</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="11">
         <v>34883668.299999997</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="4">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G30),F30,F30/G30)</f>
         <v>6976733.6599999992</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="I30" s="3">
+        <v>6976733</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K30" s="3">
+        <v>13953467.319999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="7">
         <v>432544359.30000001</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>20</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>21627217.965</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="11">
         <v>21627217</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="4">
         <v>10</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G31),F31,F31/G31)</f>
         <v>2162721.7000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
+      <c r="I31" s="3">
+        <v>2162721</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
+        <v>4325443.4000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="7">
         <v>4108787.665</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>5</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>821757.53300000005</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="11">
         <v>821757.5</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="4">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G32),F32,F32/G32)</f>
         <v>164351.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+      <c r="I32" s="3">
+        <v>164351</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="3">
+        <v>328703</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="7">
         <v>0.05</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="D33" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F33" s="11">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G33" s="9"/>
       <c r="H33" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(G33),F33,F33/G33)</f>
         <v>1.2500000000000001E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
+      <c r="I33" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="J33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K33" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="7">
         <v>0.05</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F34" s="8">
+      <c r="D34" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F34" s="11">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G34" s="9"/>
       <c r="H34" s="3">
-        <f t="shared" ref="H34:H65" si="1">IF(ISBLANK(G34),F34,F34/G34)</f>
+        <f>IF(ISBLANK(G34),F34,F34/G34)</f>
         <v>1.2500000000000001E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
+      <c r="I34" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="J34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K34" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="7">
         <v>22940055.34</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>5</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>4588011.068</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="11">
         <v>4588011.068</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="4">
         <v>7.5</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G35),F35,F35/G35)</f>
         <v>611734.80906666664</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
+      <c r="I35" s="3">
+        <v>611734</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1411695.7132307691</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="7">
         <v>19201175.25</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>150</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>128007.83500000001</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="11">
         <v>128007.8</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="4">
         <v>6</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G36),F36,F36/G36)</f>
         <v>21334.633333333335</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
+      <c r="I36" s="3">
+        <v>21334</v>
+      </c>
+      <c r="J36" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="3">
+        <v>42669.26666666667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="7">
         <v>34847060.600000001</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>10</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>3484706.06</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="11">
         <v>3484706</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="4">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G37),F37,F37/G37)</f>
         <v>696941.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
+      <c r="I37" s="3">
+        <v>696941</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="3">
+        <v>1393882.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="7">
         <v>554.64984700000002</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>5</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
         <v>110.9298</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="11">
         <v>110.9</v>
       </c>
-      <c r="G38" s="9"/>
       <c r="H38" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G38),F38,F38/G38)</f>
         <v>110.9</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
+      <c r="I38" s="3">
+        <v>110.9</v>
+      </c>
+      <c r="J38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K38" s="3">
+        <v>110.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="7">
         <v>17230050.359999999</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="6">
         <v>20</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="6">
         <v>861502.51799999992</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="11">
         <v>861502.5</v>
       </c>
-      <c r="G39" s="9"/>
       <c r="H39" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G39),F39,F39/G39)</f>
         <v>861502.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+      <c r="I39" s="3">
+        <v>861502.5</v>
+      </c>
+      <c r="J39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K39" s="3">
+        <v>861502.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="7">
         <v>4273.9050960000004</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F40" s="8">
+      <c r="D40" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F40" s="11">
         <v>4273.9050960000004</v>
       </c>
-      <c r="G40" s="9"/>
       <c r="H40" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G40),F40,F40/G40)</f>
         <v>4273.9050960000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+      <c r="I40" s="3">
+        <v>4273.9050960000004</v>
+      </c>
+      <c r="J40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K40" s="3">
+        <v>4273.9050960000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="7">
         <v>0.05</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F41" s="8">
+      <c r="D41" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F41" s="11">
         <v>0.05</v>
       </c>
-      <c r="G41" s="9"/>
       <c r="H41" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G41),F41,F41/G41)</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+      <c r="I41" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="J41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K41" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="7">
         <v>0.05</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F42" s="8">
+      <c r="D42" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F42" s="11">
         <v>0.05</v>
       </c>
-      <c r="G42" s="9"/>
       <c r="H42" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G42),F42,F42/G42)</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+      <c r="I42" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="J42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K42" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="7">
         <v>401050.08909999998</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="6">
         <v>5</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="6">
         <v>80210</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="11">
         <v>80210</v>
       </c>
-      <c r="G43" s="9"/>
       <c r="H43" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G43),F43,F43/G43)</f>
         <v>80210</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
+      <c r="I43" s="3">
+        <v>80210</v>
+      </c>
+      <c r="J43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K43" s="3">
+        <v>80210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="7">
         <v>28898.867849999999</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F44" s="8">
+      <c r="D44" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F44" s="11">
         <v>28898.867849999999</v>
       </c>
-      <c r="G44" s="9"/>
       <c r="H44" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G44),F44,F44/G44)</f>
         <v>28898.867849999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
+      <c r="I44" s="3">
+        <v>28898.867849999999</v>
+      </c>
+      <c r="J44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K44" s="3">
+        <v>28898.867849999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="7">
         <v>15779070.359999999</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>12</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
         <v>1314922.53</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="11">
         <v>1314922.53</v>
       </c>
-      <c r="G45" s="9"/>
       <c r="H45" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G45),F45,F45/G45)</f>
         <v>1314922.53</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
+      <c r="I45" s="3">
+        <v>27400000</v>
+      </c>
+      <c r="J45" s="3">
+        <v>2</v>
+      </c>
+      <c r="K45" s="3">
+        <v>27400000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="7">
         <v>6221.5131609999999</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F46" s="8">
+      <c r="D46" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F46" s="11">
         <v>6221.5131609999999</v>
       </c>
-      <c r="G46" s="9"/>
       <c r="H46" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G46),F46,F46/G46)</f>
         <v>6221.5131609999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
+      <c r="I46" s="3">
+        <v>6221.5131609999999</v>
+      </c>
+      <c r="J46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K46" s="3">
+        <v>6221.5131609999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="7">
         <v>24854569.199999999</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>6</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="6">
         <v>4142428.1666666665</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="11">
         <v>4142428.1669999999</v>
       </c>
-      <c r="G47" s="9"/>
       <c r="H47" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G47),F47,F47/G47)</f>
         <v>4142428.1669999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
+      <c r="I47" s="3">
+        <v>4142428.1669999999</v>
+      </c>
+      <c r="J47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K47" s="3">
+        <v>4142428.1669999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="7">
         <v>53.609603989999997</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F48" s="8">
+      <c r="D48" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F48" s="11">
         <v>53.609603989999997</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="4">
         <v>2</v>
       </c>
       <c r="H48" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G48),F48,F48/G48)</f>
         <v>26.804801994999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
+      <c r="I48" s="3">
+        <v>26</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K48" s="3">
+        <v>26.804801994999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="7">
         <v>16705.027440000002</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="D49" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F49" s="11">
         <v>16705.027440000002</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="4">
         <v>15</v>
       </c>
       <c r="H49" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G49),F49,F49/G49)</f>
         <v>1113.668496</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
+      <c r="I49" s="3">
+        <v>438000</v>
+      </c>
+      <c r="J49" s="3">
+        <v>1</v>
+      </c>
+      <c r="K49" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="7">
         <v>5700290.8640000001</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F50" s="8">
+      <c r="D50" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F50" s="11">
         <v>5700290.8640000001</v>
       </c>
-      <c r="G50" s="9"/>
       <c r="H50" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G50),F50,F50/G50)</f>
         <v>5700290.8640000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
+      <c r="I50" s="3">
+        <v>134000000</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2</v>
+      </c>
+      <c r="K50" s="3">
+        <v>134000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="7">
         <v>10723808.939999999</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="6">
         <v>30</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="6">
         <v>357460.29800000001</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F51" s="11">
         <v>357460.29800000001</v>
       </c>
-      <c r="G51" s="9"/>
       <c r="H51" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G51),F51,F51/G51)</f>
         <v>357460.29800000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
+      <c r="I51" s="3">
+        <v>357460.29800000001</v>
+      </c>
+      <c r="J51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K51" s="3">
+        <v>357460.29800000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="7">
         <v>2957397.3650000002</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F52" s="8">
+      <c r="D52" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F52" s="11">
         <v>2957397.3650000002</v>
       </c>
-      <c r="G52" s="9"/>
       <c r="H52" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G52),F52,F52/G52)</f>
         <v>2957397.3650000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="4" t="s">
+      <c r="I52" s="3">
+        <v>2957397.3650000002</v>
+      </c>
+      <c r="J52" s="3" t="str">
+        <f>IF(H52=I52,"",1)</f>
+        <v/>
+      </c>
+      <c r="K52" s="3">
+        <v>3943196.4866666668</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="7">
         <v>361154520.60000002</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="6">
         <v>5</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="6">
         <v>72230904.120000005</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="11">
         <v>72230904</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="4">
         <v>1.5</v>
       </c>
       <c r="H53" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G53),F53,F53/G53)</f>
         <v>48153936</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
+      <c r="I53" s="3">
+        <v>48153936</v>
+      </c>
+      <c r="J53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K53" s="3">
+        <v>57784723.200000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="7">
         <v>7496.955054</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F54" s="8">
+      <c r="D54" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F54" s="11">
         <v>7496.955054</v>
       </c>
-      <c r="G54" s="9"/>
       <c r="H54" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G54),F54,F54/G54)</f>
         <v>7496.955054</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
+      <c r="I54" s="3">
+        <v>7496.955054</v>
+      </c>
+      <c r="J54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K54" s="3">
+        <v>7496.955054</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="7">
         <v>358999.37920000002</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="6">
         <v>12</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55" s="6">
         <v>29916.614166666666</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F55" s="11">
         <v>29916.6</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G55" s="9">
         <v>10</v>
       </c>
       <c r="H55" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G55),F55,F55/G55)</f>
         <v>2991.66</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="4" t="s">
+      <c r="I55" s="3">
+        <v>2991</v>
+      </c>
+      <c r="J55" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K55" s="3">
+        <v>2991.66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C56" s="7">
         <v>352590040.69999999</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="6">
         <v>7</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="6">
         <v>50370005.81428571</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="11">
         <v>50370005.799999997</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="4">
         <v>6</v>
       </c>
       <c r="H56" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G56),F56,F56/G56)</f>
         <v>8395000.9666666668</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
+      <c r="I56" s="3">
+        <v>6330000</v>
+      </c>
+      <c r="J56" s="3">
+        <v>1</v>
+      </c>
+      <c r="K56" s="3">
+        <f>I56/2</f>
+        <v>3165000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="7">
         <v>233447.39780000001</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F57" s="8">
+      <c r="D57" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="11">
         <v>233447.39780000001</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="4">
         <v>8</v>
       </c>
       <c r="H57" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G57),F57,F57/G57)</f>
         <v>29180.924725000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="4" t="s">
+      <c r="I57" s="3">
+        <v>29180</v>
+      </c>
+      <c r="J57" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K57" s="3">
+        <v>58361.849450000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="7">
         <v>1053704.304</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F58" s="8">
+      <c r="D58" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F58" s="11">
         <v>210740.4</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="4">
         <v>7.5</v>
       </c>
       <c r="H58" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G58),F58,F58/G58)</f>
         <v>28098.719999999998</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
+      <c r="I58" s="3">
+        <v>53400000</v>
+      </c>
+      <c r="J58" s="3">
+        <v>1</v>
+      </c>
+      <c r="K58" s="3">
+        <f>I58/10</f>
+        <v>5340000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="7">
         <v>177129.4045</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F59" s="8">
+      <c r="D59" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F59" s="11">
         <v>177129.4045</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="4">
         <v>10</v>
       </c>
       <c r="H59" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G59),F59,F59/G59)</f>
         <v>17712.940450000002</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4" t="s">
+      <c r="I59" s="3">
+        <v>17712</v>
+      </c>
+      <c r="J59" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K59" s="3">
+        <v>35425.880900000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="7">
         <v>40960.04507</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="6">
         <v>1000</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="6">
         <v>4096.0045070000006</v>
       </c>
-      <c r="F60" s="8">
+      <c r="F60" s="11">
         <v>4096</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="4">
         <v>0.2</v>
       </c>
       <c r="H60" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G60),F60,F60/G60)</f>
         <v>20480</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="4" t="s">
+      <c r="I60" s="3">
+        <v>1420000</v>
+      </c>
+      <c r="J60" s="3">
+        <v>1</v>
+      </c>
+      <c r="K60" s="3">
+        <f>I60/10</f>
+        <v>142000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61" s="7">
         <v>71.004761549999998</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F61" s="8">
+      <c r="D61" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F61" s="11">
         <v>71.004761549999998</v>
       </c>
-      <c r="G61" s="9"/>
       <c r="H61" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G61),F61,F61/G61)</f>
         <v>71.004761549999998</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="4" t="s">
+      <c r="I61" s="3">
+        <v>71.004761549999998</v>
+      </c>
+      <c r="J61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K61" s="3">
+        <v>71.004761549999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C62" s="7">
         <v>52020187.369999997</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F62" s="8">
+      <c r="D62" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F62" s="11">
         <v>52020187.369999997</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G62" s="4">
         <v>10</v>
       </c>
       <c r="H62" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G62),F62,F62/G62)</f>
         <v>5202018.7369999997</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
+      <c r="I62" s="3">
+        <v>5020000</v>
+      </c>
+      <c r="J62" s="3">
+        <v>1</v>
+      </c>
+      <c r="K62" s="3">
+        <f>I62*1.5</f>
+        <v>7530000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63" s="7">
         <v>14975339.800000001</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="6">
         <v>250</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E63" s="6">
         <v>2199013.5920000002</v>
       </c>
-      <c r="F63" s="8">
+      <c r="F63" s="11">
         <v>2199013</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="4">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G63),F63,F63/G63)</f>
         <v>439802.6</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="4" t="s">
+      <c r="I63" s="3">
+        <v>439802</v>
+      </c>
+      <c r="J63" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K63" s="3">
+        <v>879605.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64" s="7">
         <v>3738776.034</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F64" s="8">
+      <c r="D64" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F64" s="11">
         <v>3738776.034</v>
       </c>
-      <c r="G64" s="9">
+      <c r="G64" s="4">
         <v>15</v>
       </c>
       <c r="H64" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G64),F64,F64/G64)</f>
         <v>249251.73559999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="4" t="s">
+      <c r="I64" s="3">
+        <v>32400000</v>
+      </c>
+      <c r="J64" s="3">
+        <v>1</v>
+      </c>
+      <c r="K64" s="3">
+        <f>I64/1.5</f>
+        <v>21600000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="7">
         <v>97071048.260000005</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="6">
         <v>150</v>
       </c>
-      <c r="E65" s="7">
+      <c r="E65" s="6">
         <v>647140.3217333334</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F65" s="11">
         <v>300000</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G65" s="4">
         <v>7</v>
       </c>
       <c r="H65" s="3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G65),F65,F65/G65)</f>
         <v>42857.142857142855</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="4" t="s">
+      <c r="I65" s="3">
+        <v>42857</v>
+      </c>
+      <c r="J65" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K65" s="3">
+        <v>42857.142857142855</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="7">
         <v>20265685.109999999</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="7">
+      <c r="E66" s="6">
         <v>2026568.5109999999</v>
       </c>
-      <c r="F66" s="8">
+      <c r="F66" s="11">
         <v>2026568.5109999999</v>
       </c>
-      <c r="G66" s="9"/>
       <c r="H66" s="3">
-        <f t="shared" ref="H66:H68" si="2">IF(ISBLANK(G66),F66,F66/G66)</f>
+        <f>IF(ISBLANK(G66),F66,F66/G66)</f>
         <v>2026568.5109999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="4" t="s">
+      <c r="I66" s="3">
+        <v>2026568.5109999999</v>
+      </c>
+      <c r="J66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K66" s="3">
+        <v>2026568.5109999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="7">
         <v>2983706.8709999998</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F67" s="8">
+      <c r="D67" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F67" s="11">
         <v>2983706.8709999998</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="4">
         <v>10</v>
       </c>
       <c r="H67" s="3">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(G67),F67,F67/G67)</f>
         <v>298370.68709999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="4" t="s">
+      <c r="I67" s="3">
+        <v>491000</v>
+      </c>
+      <c r="J67" s="3">
+        <v>2</v>
+      </c>
+      <c r="K67" s="3">
+        <v>491000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="7">
         <v>204805160.5</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="7">
+      <c r="E68" s="6">
         <v>20480516.050000001</v>
       </c>
-      <c r="F68" s="8">
+      <c r="F68" s="11">
         <v>20480516</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="4">
         <v>7</v>
       </c>
       <c r="H68" s="3">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(G68),F68,F68/G68)</f>
         <v>2925788</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I68" s="3">
+        <v>29500000</v>
+      </c>
+      <c r="J68" s="3">
+        <v>1</v>
+      </c>
+      <c r="K68" s="3">
+        <v>2925788</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
       <c r="E71"/>
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F71" s="12"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B72"/>
       <c r="C72"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1">
-    <sortState ref="A2:H68">
-      <sortCondition ref="B1"/>
-    </sortState>
+  <autoFilter ref="A1:K68">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
RemovePred6 - Last try to reduce beginning groups - Any groups that don't change in first 15 yrs, deem not a recruitment issue - Increase Zoo and RCB growth
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Group Condition" sheetId="1" r:id="rId1"/>
     <sheet name="Recruitment_Log" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group Condition'!$A$1:$G$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recruitment_Log!$A$1:$K$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group Condition'!$A$1:$I$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recruitment_Log!$A$1:$O$68</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="212">
   <si>
     <t>Too High</t>
   </si>
@@ -635,6 +635,36 @@
   </si>
   <si>
     <t>RemovePred3_FinalKDENR</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Too High Early</t>
+  </si>
+  <si>
+    <t>RemovePred5_tochange</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>RemovePred5_KDENR</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>RemovePred6_KDENR</t>
+  </si>
+  <si>
+    <t>RemovePred6_Change</t>
   </si>
 </sst>
 </file>
@@ -723,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -755,6 +785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1036,25 +1067,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -1062,33 +1095,39 @@
         <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>123</v>
       </c>
-      <c r="F2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1098,8 +1137,14 @@
       <c r="C3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1110,32 +1155,35 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>105</v>
       </c>
-      <c r="E5" t="s">
-        <v>181</v>
-      </c>
       <c r="F5" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>115</v>
       </c>
-      <c r="F6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1145,116 +1193,119 @@
       <c r="C7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>94</v>
       </c>
-      <c r="F8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>113</v>
       </c>
-      <c r="F9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>125</v>
       </c>
-      <c r="E10" t="s">
-        <v>181</v>
-      </c>
       <c r="F10" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>130</v>
       </c>
-      <c r="F11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>156</v>
       </c>
-      <c r="F12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>148</v>
       </c>
-      <c r="C13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>79</v>
       </c>
       <c r="B14" t="s">
         <v>168</v>
       </c>
-      <c r="G14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
       <c r="B15" t="s">
         <v>158</v>
       </c>
-      <c r="D15" t="s">
-        <v>181</v>
-      </c>
-      <c r="F15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>107</v>
       </c>
-      <c r="E16" t="s">
-        <v>181</v>
-      </c>
       <c r="F16" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1264,19 +1315,25 @@
       <c r="C17" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>181</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>49</v>
       </c>
       <c r="B18" t="s">
         <v>138</v>
       </c>
-      <c r="G18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1286,63 +1343,69 @@
       <c r="C19" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>181</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>109</v>
       </c>
-      <c r="F20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>75</v>
       </c>
       <c r="B21" t="s">
         <v>164</v>
       </c>
-      <c r="F21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>76</v>
       </c>
       <c r="B22" t="s">
         <v>165</v>
       </c>
-      <c r="G22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>81</v>
       </c>
       <c r="B23" t="s">
         <v>170</v>
       </c>
-      <c r="G23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>82</v>
       </c>
       <c r="B24" t="s">
         <v>171</v>
       </c>
-      <c r="G24" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1352,201 +1415,228 @@
       <c r="C25" t="s">
         <v>181</v>
       </c>
-      <c r="F25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G25" t="s">
+        <v>181</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
       <c r="B26" t="s">
         <v>101</v>
       </c>
-      <c r="G26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>181</v>
+      </c>
+      <c r="H26" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>80</v>
       </c>
       <c r="B27" t="s">
         <v>169</v>
       </c>
-      <c r="F27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
       <c r="B28" t="s">
         <v>132</v>
       </c>
-      <c r="G28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H28" t="s">
+        <v>181</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>64</v>
       </c>
       <c r="B29" t="s">
         <v>153</v>
       </c>
-      <c r="F29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
       <c r="B30" t="s">
         <v>151</v>
       </c>
-      <c r="F30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>89</v>
       </c>
       <c r="B31" t="s">
         <v>178</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>53</v>
       </c>
       <c r="B32" t="s">
         <v>142</v>
       </c>
-      <c r="F32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>181</v>
+      </c>
+      <c r="G32" t="s">
+        <v>181</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
       <c r="B33" t="s">
         <v>159</v>
       </c>
-      <c r="F33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
       <c r="B34" t="s">
         <v>152</v>
       </c>
-      <c r="F34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>181</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
       <c r="B35" t="s">
         <v>93</v>
       </c>
-      <c r="D35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>181</v>
+      </c>
+      <c r="G35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>77</v>
       </c>
       <c r="B36" t="s">
         <v>166</v>
       </c>
-      <c r="G36" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>57</v>
       </c>
       <c r="B37" t="s">
         <v>146</v>
       </c>
-      <c r="C37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>88</v>
       </c>
       <c r="B38" t="s">
         <v>177</v>
       </c>
-      <c r="G38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>84</v>
       </c>
       <c r="B39" t="s">
         <v>173</v>
       </c>
-      <c r="F39" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>85</v>
       </c>
       <c r="B40" t="s">
         <v>174</v>
       </c>
-      <c r="G40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>22</v>
       </c>
       <c r="B41" t="s">
         <v>108</v>
       </c>
-      <c r="D41" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>131</v>
       </c>
-      <c r="F42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -1556,99 +1646,108 @@
       <c r="C43" t="s">
         <v>181</v>
       </c>
-      <c r="F43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>181</v>
+      </c>
+      <c r="G43" t="s">
+        <v>181</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>143</v>
       </c>
-      <c r="F44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>162</v>
       </c>
-      <c r="G45" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>35</v>
       </c>
       <c r="B46" t="s">
         <v>124</v>
       </c>
-      <c r="F46" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>181</v>
+      </c>
+      <c r="G46" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>66</v>
       </c>
       <c r="B47" t="s">
         <v>155</v>
       </c>
-      <c r="F47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>29</v>
       </c>
       <c r="B48" t="s">
         <v>117</v>
       </c>
-      <c r="D48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>68</v>
       </c>
       <c r="B49" t="s">
         <v>157</v>
       </c>
-      <c r="F49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="B50" t="s">
         <v>110</v>
       </c>
-      <c r="F50" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>48</v>
       </c>
       <c r="B51" t="s">
         <v>137</v>
       </c>
-      <c r="G51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -1658,74 +1757,80 @@
       <c r="C52" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>181</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>140</v>
       </c>
-      <c r="G53" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>74</v>
       </c>
       <c r="B54" t="s">
         <v>163</v>
       </c>
-      <c r="G54" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
       <c r="B55" t="s">
         <v>106</v>
       </c>
-      <c r="G55" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>86</v>
       </c>
       <c r="B56" t="s">
         <v>175</v>
       </c>
-      <c r="G56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>83</v>
       </c>
       <c r="B57" t="s">
         <v>172</v>
       </c>
-      <c r="G57" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H57" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>145</v>
       </c>
-      <c r="G58" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -1735,77 +1840,86 @@
       <c r="C59" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>181</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>50</v>
       </c>
       <c r="B60" t="s">
         <v>139</v>
       </c>
-      <c r="G60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>71</v>
       </c>
       <c r="B61" t="s">
         <v>160</v>
       </c>
-      <c r="C61" t="s">
-        <v>181</v>
-      </c>
       <c r="E61" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I61" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>31</v>
       </c>
       <c r="B62" t="s">
         <v>119</v>
       </c>
-      <c r="G62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>181</v>
+      </c>
+      <c r="H62" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>90</v>
       </c>
       <c r="B63" t="s">
         <v>179</v>
       </c>
-      <c r="G63" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>58</v>
       </c>
       <c r="B64" t="s">
         <v>147</v>
       </c>
-      <c r="C64" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>47</v>
       </c>
       <c r="B65" t="s">
         <v>136</v>
       </c>
-      <c r="C65" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>33</v>
       </c>
@@ -1815,102 +1929,105 @@
       <c r="C66" t="s">
         <v>181</v>
       </c>
-      <c r="F66" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>181</v>
+      </c>
+      <c r="G66" t="s">
+        <v>181</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>154</v>
       </c>
-      <c r="F67" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>55</v>
       </c>
       <c r="B68" t="s">
         <v>144</v>
       </c>
-      <c r="G68" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>78</v>
       </c>
       <c r="B69" t="s">
         <v>167</v>
       </c>
-      <c r="C69" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>87</v>
       </c>
       <c r="B70" t="s">
         <v>176</v>
       </c>
-      <c r="G70" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H70" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>27</v>
       </c>
       <c r="B71" t="s">
         <v>114</v>
       </c>
-      <c r="F71" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G71" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" t="s">
         <v>161</v>
       </c>
-      <c r="F72" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>28</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
       </c>
-      <c r="F73" t="s">
-        <v>181</v>
-      </c>
       <c r="G73" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>60</v>
       </c>
       <c r="B74" t="s">
         <v>149</v>
       </c>
-      <c r="G74" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>46</v>
       </c>
@@ -1920,8 +2037,14 @@
       <c r="C75" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D75" t="s">
+        <v>181</v>
+      </c>
+      <c r="I75" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -1931,22 +2054,25 @@
       <c r="C76" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D76" t="s">
+        <v>181</v>
+      </c>
+      <c r="I76" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77" t="s">
         <v>127</v>
       </c>
-      <c r="C77" t="s">
-        <v>181</v>
-      </c>
-      <c r="F77" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G77" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -1956,8 +2082,17 @@
       <c r="C78" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>181</v>
+      </c>
+      <c r="G78" t="s">
+        <v>181</v>
+      </c>
+      <c r="I78" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -1967,55 +2102,70 @@
       <c r="C79" t="s">
         <v>181</v>
       </c>
-      <c r="F79" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>181</v>
+      </c>
+      <c r="G79" t="s">
+        <v>181</v>
+      </c>
+      <c r="I79" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>34</v>
       </c>
       <c r="B80" t="s">
         <v>122</v>
       </c>
-      <c r="C80" t="s">
-        <v>181</v>
-      </c>
-      <c r="F80" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G80" t="s">
+        <v>181</v>
+      </c>
+      <c r="I80" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>61</v>
       </c>
       <c r="B81" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H81" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>12</v>
       </c>
       <c r="B82" t="s">
         <v>95</v>
       </c>
-      <c r="F82" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>181</v>
+      </c>
+      <c r="G82" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
       <c r="B83" t="s">
         <v>97</v>
       </c>
-      <c r="F83" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>181</v>
+      </c>
+      <c r="H83" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -2025,8 +2175,14 @@
       <c r="C84" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>181</v>
+      </c>
+      <c r="I84" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>52</v>
       </c>
@@ -2036,33 +2192,45 @@
       <c r="C85" t="s">
         <v>181</v>
       </c>
-      <c r="F85" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>181</v>
+      </c>
+      <c r="G85" t="s">
+        <v>181</v>
+      </c>
+      <c r="I85" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>17</v>
       </c>
       <c r="B86" t="s">
         <v>100</v>
       </c>
-      <c r="F86" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>181</v>
+      </c>
+      <c r="G86" t="s">
+        <v>181</v>
+      </c>
+      <c r="I86" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>40</v>
       </c>
       <c r="B87" t="s">
         <v>129</v>
       </c>
-      <c r="G87" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H87" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -2072,20 +2240,28 @@
       <c r="C88" t="s">
         <v>181</v>
       </c>
-      <c r="F88" t="s">
-        <v>181</v>
+      <c r="D88" t="s">
+        <v>181</v>
+      </c>
+      <c r="G88" t="s">
+        <v>181</v>
+      </c>
+      <c r="I88" s="13" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G88">
+  <autoFilter ref="A1:I88">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <sortState ref="A2:G88">
-      <sortCondition ref="B1:B88"/>
-    </sortState>
+    <filterColumn colId="8">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2094,13 +2270,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2116,10 +2292,15 @@
     <col min="9" max="9" width="26" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="3"/>
+    <col min="12" max="12" width="10.88671875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="3"/>
+    <col min="15" max="15" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>91</v>
       </c>
@@ -2153,8 +2334,23 @@
       <c r="K1" s="3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2370,7 @@
         <v>66739628</v>
       </c>
       <c r="H2" s="3">
-        <f>IF(ISBLANK(G2),F2,F2/G2)</f>
+        <f t="shared" ref="H2:H33" si="0">IF(ISBLANK(G2),F2,F2/G2)</f>
         <v>66739628</v>
       </c>
       <c r="I2" s="3">
@@ -2186,44 +2382,76 @@
       <c r="K2" s="3">
         <v>45700000</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L2" s="3">
+        <f>VLOOKUP(A2,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>45700000</v>
+      </c>
+      <c r="N2" s="3">
+        <f>VLOOKUP(A2,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>45700000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C3" s="7">
-        <v>20527442.649999999</v>
-      </c>
-      <c r="D3" s="6">
-        <v>10</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2052744.2649999999</v>
+        <v>2124041.1490000002</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>193</v>
       </c>
       <c r="F3" s="11">
-        <v>2052744.2649999999</v>
-      </c>
-      <c r="G3" s="4">
-        <v>4</v>
+        <v>2124041.1490000002</v>
       </c>
       <c r="H3" s="3">
         <f>IF(ISBLANK(G3),F3,F3/G3)</f>
-        <v>513186.06624999997</v>
+        <v>2124041.1490000002</v>
       </c>
       <c r="I3" s="3">
-        <v>22700000</v>
+        <v>46100000</v>
       </c>
       <c r="J3" s="3">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3">
-        <v>22700000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <f>IF(H3=I3,"",1)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="5">
+        <v>10000000</v>
+      </c>
+      <c r="L3" s="3">
+        <f>IF(K3=M3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <f>K3*0.75</f>
+        <v>7500000</v>
+      </c>
+      <c r="N3" s="3" t="str">
+        <f>VLOOKUP(A3,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O3" s="5">
+        <f>M3*0.75</f>
+        <v>5625000</v>
+      </c>
+      <c r="P3" s="3">
+        <f>O3*0.5</f>
+        <v>2812500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2250,14 +2478,29 @@
         <v>19030173</v>
       </c>
       <c r="J4" s="3" t="str">
-        <f t="shared" ref="J3:J66" si="0">IF(H4=I4,"",1)</f>
+        <f>IF(H4=I4,"",1)</f>
         <v/>
       </c>
       <c r="K4" s="3">
         <v>19030173</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L4" s="3">
+        <f>IF(K4=M4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <f>K4+1.25</f>
+        <v>19030174.25</v>
+      </c>
+      <c r="N4" s="3">
+        <f>VLOOKUP(A4,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>19030174.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -2287,85 +2530,141 @@
         <v>63265</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H5=I5,"",1)</f>
         <v>1</v>
       </c>
       <c r="K5" s="3">
         <v>63265</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L5" s="3">
+        <f>IF(K5=M5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <v>63265</v>
+      </c>
+      <c r="N5" s="3">
+        <f>VLOOKUP(A5,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>63265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C6" s="7">
-        <v>16477555.609999999</v>
-      </c>
-      <c r="D6" s="6">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2353936.5157142854</v>
+        <v>1718757.3940000001</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>193</v>
       </c>
       <c r="F6" s="11">
-        <v>2353936.5</v>
+        <v>1718757.3940000001</v>
       </c>
       <c r="G6" s="4">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="H6" s="3">
         <f>IF(ISBLANK(G6),F6,F6/G6)</f>
-        <v>470787.3</v>
+        <v>22916.765253333335</v>
       </c>
       <c r="I6" s="3">
-        <v>470787</v>
+        <v>36100000000</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="11">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>36100000000</v>
+      </c>
+      <c r="L6" s="3">
+        <f>IF(K6=M6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <f>K6/100</f>
+        <v>361000000</v>
+      </c>
+      <c r="N6" s="3" t="str">
+        <f>VLOOKUP(A6,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>---</v>
+      </c>
+      <c r="O6" s="3">
+        <f>M6/5</f>
+        <v>72200000</v>
+      </c>
+      <c r="P6" s="3">
+        <f>O6*0.75</f>
+        <v>54150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="7">
+        <v>16477555.609999999</v>
+      </c>
+      <c r="D7" s="6">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2353936.5157142854</v>
+      </c>
+      <c r="F7" s="11">
         <v>2353936.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="7">
-        <v>254421.22440000001</v>
-      </c>
-      <c r="D7" s="6">
-        <v>150</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1696.141496</v>
-      </c>
-      <c r="F7" s="11">
-        <v>1696.14</v>
+      <c r="G7" s="4">
+        <v>5</v>
       </c>
       <c r="H7" s="3">
         <f>IF(ISBLANK(G7),F7,F7/G7)</f>
-        <v>1696.14</v>
+        <v>470787.3</v>
       </c>
       <c r="I7" s="3">
-        <v>1696.14</v>
-      </c>
-      <c r="J7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="K7" s="3">
-        <v>1696.14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>470787</v>
+      </c>
+      <c r="J7" s="3">
+        <f>IF(H7=I7,"",1)</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="11">
+        <v>2353936.5</v>
+      </c>
+      <c r="L7" s="3">
+        <f>IF(K7=M7,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="11">
+        <f>K7*0.75</f>
+        <v>1765452.375</v>
+      </c>
+      <c r="N7" s="3" t="str">
+        <f>VLOOKUP(A7,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O7" s="3">
+        <f>M7*0.75</f>
+        <v>1324089.28125</v>
+      </c>
+      <c r="P7" s="3">
+        <f>O7*0.75</f>
+        <v>993066.9609375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -2395,14 +2694,28 @@
         <v>1000000000000</v>
       </c>
       <c r="J8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H8=I8,"",1)</f>
         <v/>
       </c>
       <c r="K8" s="3">
         <v>1000000000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L8" s="3">
+        <f>IF(K8=M8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>2000000000000</v>
+      </c>
+      <c r="N8" s="3">
+        <f>VLOOKUP(A8,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>2000000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -2432,14 +2745,29 @@
         <v>214151453</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H9=I9,"",1)</f>
         <v>1</v>
       </c>
       <c r="K9" s="11">
         <v>3212271805.0500002</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="3">
+        <f>IF(K9=M9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="11">
+        <f>K9*1.25</f>
+        <v>4015339756.3125</v>
+      </c>
+      <c r="N9" s="3">
+        <f>VLOOKUP(A9,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="11">
+        <v>4015339756.3125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
@@ -2466,14 +2794,28 @@
         <v>2123.8950410000002</v>
       </c>
       <c r="J10" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H10=I10,"",1)</f>
         <v/>
       </c>
       <c r="K10" s="3">
         <v>2123.8950410000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L10" s="3">
+        <f>IF(K10=M10,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2123.8950410000002</v>
+      </c>
+      <c r="N10" s="3">
+        <f>VLOOKUP(A10,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>2123.8950410000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
@@ -2500,14 +2842,28 @@
         <v>74822.192989999996</v>
       </c>
       <c r="J11" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H11=I11,"",1)</f>
         <v/>
       </c>
       <c r="K11" s="11">
         <v>74822.192989999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="3">
+        <f>IF(K11=M11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M11" s="11">
+        <v>74822.192989999996</v>
+      </c>
+      <c r="N11" s="3">
+        <f>VLOOKUP(A11,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="11">
+        <v>74822.192989999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>59</v>
       </c>
@@ -2537,14 +2893,28 @@
         <v>23</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H12=I12,"",1)</f>
         <v>1</v>
       </c>
       <c r="K12" s="3">
         <v>23.545910710000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="3">
+        <f>IF(K12=M12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>10</v>
+      </c>
+      <c r="N12" s="3">
+        <f>VLOOKUP(A12,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
@@ -2574,50 +2944,85 @@
         <v>51</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H13=I13,"",1)</f>
         <v>1</v>
       </c>
       <c r="K13" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L13" s="3">
+        <f>IF(K13=M13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>100</v>
+      </c>
+      <c r="N13" s="3">
+        <f>VLOOKUP(A13,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="C14" s="7">
-        <v>1718757.3940000001</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>193</v>
+        <v>352590040.69999999</v>
+      </c>
+      <c r="D14" s="6">
+        <v>7</v>
+      </c>
+      <c r="E14" s="6">
+        <v>50370005.81428571</v>
       </c>
       <c r="F14" s="11">
-        <v>1718757.3940000001</v>
+        <v>50370005.799999997</v>
       </c>
       <c r="G14" s="4">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="H14" s="3">
         <f>IF(ISBLANK(G14),F14,F14/G14)</f>
-        <v>22916.765253333335</v>
+        <v>8395000.9666666668</v>
       </c>
       <c r="I14" s="3">
-        <v>36100000000</v>
+        <v>6330000</v>
       </c>
       <c r="J14" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" s="3">
-        <v>36100000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <f>I14/2</f>
+        <v>3165000</v>
+      </c>
+      <c r="L14" s="3">
+        <f>IF(K14=M14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <f>K14*0.75</f>
+        <v>2373750</v>
+      </c>
+      <c r="N14" s="3" t="str">
+        <f>VLOOKUP(A14,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O14" s="3">
+        <f>M14*0.75</f>
+        <v>1780312.5</v>
+      </c>
+      <c r="P14" s="3">
+        <f>C14</f>
+        <v>352590040.69999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
@@ -2644,22 +3049,36 @@
         <v>15874.27808</v>
       </c>
       <c r="J15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H15=I15,"",1)</f>
         <v/>
       </c>
       <c r="K15" s="3">
         <v>15874.27808</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L15" s="3">
+        <f>IF(K15=M15,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>15874.27808</v>
+      </c>
+      <c r="N15" s="3">
+        <f>VLOOKUP(A15,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>15874.27808</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="C16" s="7">
-        <v>2124041.1490000002</v>
+        <v>129309.07709999999</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>193</v>
@@ -2668,24 +3087,47 @@
         <v>193</v>
       </c>
       <c r="F16" s="11">
-        <v>2124041.1490000002</v>
+        <v>129309</v>
+      </c>
+      <c r="G16" s="4">
+        <v>10</v>
       </c>
       <c r="H16" s="3">
         <f>IF(ISBLANK(G16),F16,F16/G16)</f>
-        <v>2124041.1490000002</v>
+        <v>12930.9</v>
       </c>
       <c r="I16" s="3">
-        <v>46100000</v>
+        <v>12930</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H16=I16,"",1)</f>
         <v>1</v>
       </c>
-      <c r="K16" s="5">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K16" s="3">
+        <v>12930.9</v>
+      </c>
+      <c r="L16" s="3">
+        <f>IF(K16=M16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <f>K16*0.75</f>
+        <v>9698.1749999999993</v>
+      </c>
+      <c r="N16" s="3" t="str">
+        <f>VLOOKUP(A16,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O16" s="5">
+        <f>M16*0.75</f>
+        <v>7273.6312499999995</v>
+      </c>
+      <c r="P16" s="5">
+        <f>O16*0.75</f>
+        <v>5455.2234374999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
@@ -2715,51 +3157,82 @@
         <v>8700000</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H17=I17,"",1)</f>
         <v>1</v>
       </c>
       <c r="K17" s="5">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L17" s="3">
+        <f>IF(K17=M17,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M17" s="5">
+        <v>4000000</v>
+      </c>
+      <c r="N17" s="3">
+        <f>VLOOKUP(A17,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C18" s="7">
-        <v>129309.07709999999</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>193</v>
+        <v>17230050.359999999</v>
+      </c>
+      <c r="D18" s="6">
+        <v>20</v>
+      </c>
+      <c r="E18" s="6">
+        <v>861502.51799999992</v>
       </c>
       <c r="F18" s="11">
-        <v>129309</v>
-      </c>
-      <c r="G18" s="4">
-        <v>10</v>
+        <v>861502.5</v>
       </c>
       <c r="H18" s="3">
         <f>IF(ISBLANK(G18),F18,F18/G18)</f>
-        <v>12930.9</v>
+        <v>861502.5</v>
       </c>
       <c r="I18" s="3">
-        <v>12930</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>861502.5</v>
+      </c>
+      <c r="J18" s="3" t="str">
+        <f>IF(H18=I18,"",1)</f>
+        <v/>
       </c>
       <c r="K18" s="3">
-        <v>12930.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>861502.5</v>
+      </c>
+      <c r="L18" s="3">
+        <f>IF(K18=M18,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <f>K18*0.85</f>
+        <v>732277.125</v>
+      </c>
+      <c r="N18" s="3" t="str">
+        <f>VLOOKUP(A18,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O18" s="5">
+        <f>M18*0.75</f>
+        <v>549207.84375</v>
+      </c>
+      <c r="P18" s="5">
+        <f t="shared" ref="P18:P20" si="1">O18*0.75</f>
+        <v>411905.8828125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2789,47 +3262,91 @@
         <v>189098</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H19=I19,"",1)</f>
         <v>1</v>
       </c>
       <c r="K19" s="3">
         <v>189098.12857142856</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="3">
+        <f>IF(K19=M19,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <f>K19*0.75</f>
+        <v>141823.59642857141</v>
+      </c>
+      <c r="N19" s="3" t="str">
+        <f>VLOOKUP(A19,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O19" s="5">
+        <f>M19*0.75</f>
+        <v>106367.69732142857</v>
+      </c>
+      <c r="P19" s="5">
+        <f t="shared" si="1"/>
+        <v>79775.772991071426</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C20" s="7">
-        <v>172649603.19999999</v>
+        <v>432544359.30000001</v>
       </c>
       <c r="D20" s="6">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E20" s="6">
-        <v>34529920.600000001</v>
+        <v>21627217.965</v>
       </c>
       <c r="F20" s="11">
-        <v>34529920</v>
+        <v>21627217</v>
+      </c>
+      <c r="G20" s="4">
+        <v>10</v>
       </c>
       <c r="H20" s="3">
         <f>IF(ISBLANK(G20),F20,F20/G20)</f>
-        <v>34529920</v>
+        <v>2162721.7000000002</v>
       </c>
       <c r="I20" s="3">
-        <v>104000000</v>
+        <v>2162721</v>
       </c>
       <c r="J20" s="3">
-        <v>2</v>
+        <f>IF(H20=I20,"",1)</f>
+        <v>1</v>
       </c>
       <c r="K20" s="3">
-        <v>104000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4325443.4000000004</v>
+      </c>
+      <c r="L20" s="3">
+        <f>IF(K20=M20,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="3">
+        <f>K20*0.75</f>
+        <v>3244082.5500000003</v>
+      </c>
+      <c r="N20" s="3" t="str">
+        <f>VLOOKUP(A20,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O20" s="5">
+        <f>M20*0.75</f>
+        <v>2433061.9125000001</v>
+      </c>
+      <c r="P20" s="5">
+        <f t="shared" si="1"/>
+        <v>1824796.4343750002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>187</v>
       </c>
@@ -2856,14 +3373,28 @@
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="J21" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H21=I21,"",1)</f>
         <v/>
       </c>
       <c r="K21" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L21" s="3">
+        <f>IF(K21=M21,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N21" s="3" t="e">
+        <f>VLOOKUP(A21,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O21" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>186</v>
       </c>
@@ -2890,14 +3421,28 @@
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H22=I22,"",1)</f>
         <v/>
       </c>
       <c r="K22" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L22" s="3">
+        <f>IF(K22=M22,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N22" s="3" t="e">
+        <f>VLOOKUP(A22,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O22" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>62</v>
       </c>
@@ -2924,51 +3469,83 @@
         <v>149515.5</v>
       </c>
       <c r="J23" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H23=I23,"",1)</f>
         <v/>
       </c>
       <c r="K23" s="3">
         <v>350000</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L23" s="3">
+        <f>IF(K23=M23,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <f>K23*0.75</f>
+        <v>262500</v>
+      </c>
+      <c r="N23" s="3">
+        <f>VLOOKUP(A23,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="5">
+        <f>M23*0.75</f>
+        <v>196875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C24" s="7">
-        <v>15150975.09</v>
+        <v>172649603.19999999</v>
       </c>
       <c r="D24" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E24" s="6">
-        <v>1893871.875</v>
+        <v>34529920.600000001</v>
       </c>
       <c r="F24" s="11">
-        <v>1893871.875</v>
-      </c>
-      <c r="G24" s="4">
-        <v>10</v>
+        <v>34529920</v>
       </c>
       <c r="H24" s="3">
         <f>IF(ISBLANK(G24),F24,F24/G24)</f>
-        <v>189387.1875</v>
+        <v>34529920</v>
       </c>
       <c r="I24" s="3">
-        <v>189387</v>
+        <v>104000000</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" s="3">
-        <v>378774.375</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>104000000</v>
+      </c>
+      <c r="L24" s="3">
+        <f>IF(K24=M24,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
+        <f>K24*0.85</f>
+        <v>88400000</v>
+      </c>
+      <c r="N24" s="3" t="str">
+        <f>VLOOKUP(A24,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O24" s="5">
+        <f>M24*0.75</f>
+        <v>66300000</v>
+      </c>
+      <c r="P24" s="5">
+        <f>O24*0.75</f>
+        <v>49725000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>185</v>
       </c>
@@ -2995,14 +3572,28 @@
         <v>0.01</v>
       </c>
       <c r="J25" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H25=I25,"",1)</f>
         <v/>
       </c>
       <c r="K25" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L25" s="3">
+        <f>IF(K25=M25,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M25" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N25" s="3" t="e">
+        <f>VLOOKUP(A25,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O25" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>184</v>
       </c>
@@ -3029,14 +3620,28 @@
         <v>0.01</v>
       </c>
       <c r="J26" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H26=I26,"",1)</f>
         <v/>
       </c>
       <c r="K26" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L26" s="3">
+        <f>IF(K26=M26,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M26" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N26" s="3" t="e">
+        <f>VLOOKUP(A26,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O26" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
@@ -3068,8 +3673,23 @@
       <c r="K27" s="3">
         <v>181000000</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L27" s="3">
+        <f>IF(K27=M27,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
+        <f>K27*1.25</f>
+        <v>226250000</v>
+      </c>
+      <c r="N27" s="3">
+        <f>VLOOKUP(A27,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="3">
+        <v>226250000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -3099,14 +3719,28 @@
         <v>375</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H28=I28,"",1)</f>
         <v>1</v>
       </c>
       <c r="K28" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L28" s="3">
+        <f>IF(K28=M28,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>100</v>
+      </c>
+      <c r="N28" s="3">
+        <f>VLOOKUP(A28,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>22</v>
       </c>
@@ -3133,14 +3767,28 @@
         <v>4986608.142</v>
       </c>
       <c r="J29" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H29=I29,"",1)</f>
         <v/>
       </c>
       <c r="K29" s="3">
         <v>4986608.142</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L29" s="3">
+        <f>IF(K29=M29,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M29" s="3">
+        <v>4986608.142</v>
+      </c>
+      <c r="N29" s="3">
+        <f>VLOOKUP(A29,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>4986608.142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>42</v>
       </c>
@@ -3170,51 +3818,84 @@
         <v>6976733</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H30=I30,"",1)</f>
         <v>1</v>
       </c>
       <c r="K30" s="3">
         <v>13953467.319999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L30" s="3">
+        <f>IF(K30=M30,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <f>K30*0.75</f>
+        <v>10465100.489999998</v>
+      </c>
+      <c r="N30" s="3">
+        <f>VLOOKUP(A30,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="5">
+        <f>M30*0.75</f>
+        <v>7848825.3674999988</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C31" s="7">
-        <v>432544359.30000001</v>
+        <v>254421.22440000001</v>
       </c>
       <c r="D31" s="6">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E31" s="6">
-        <v>21627217.965</v>
+        <v>1696.141496</v>
       </c>
       <c r="F31" s="11">
-        <v>21627217</v>
-      </c>
-      <c r="G31" s="4">
-        <v>10</v>
+        <v>1696.14</v>
       </c>
       <c r="H31" s="3">
         <f>IF(ISBLANK(G31),F31,F31/G31)</f>
-        <v>2162721.7000000002</v>
+        <v>1696.14</v>
       </c>
       <c r="I31" s="3">
-        <v>2162721</v>
-      </c>
-      <c r="J31" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1696.14</v>
+      </c>
+      <c r="J31" s="3" t="str">
+        <f>IF(H31=I31,"",1)</f>
+        <v/>
       </c>
       <c r="K31" s="3">
-        <v>4325443.4000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1696.14</v>
+      </c>
+      <c r="L31" s="3">
+        <f>IF(K31=M31,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="3">
+        <f>K31*0.75</f>
+        <v>1272.105</v>
+      </c>
+      <c r="N31" s="3" t="str">
+        <f>VLOOKUP(A31,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O31" s="3">
+        <f>M31*0.75</f>
+        <v>954.07875000000001</v>
+      </c>
+      <c r="P31" s="5">
+        <f>O31*0.75</f>
+        <v>715.55906249999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>54</v>
       </c>
@@ -3244,14 +3925,28 @@
         <v>164351</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H32=I32,"",1)</f>
         <v>1</v>
       </c>
       <c r="K32" s="3">
         <v>328703</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L32" s="3">
+        <f>IF(K32=M32,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M32" s="3">
+        <v>328703</v>
+      </c>
+      <c r="N32" s="3">
+        <f>VLOOKUP(A32,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="3">
+        <v>328703</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>189</v>
       </c>
@@ -3278,14 +3973,28 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J33" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H33=I33,"",1)</f>
         <v/>
       </c>
       <c r="K33" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L33" s="3">
+        <f>IF(K33=M33,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M33" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="N33" s="3" t="e">
+        <f>VLOOKUP(A33,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O33" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>188</v>
       </c>
@@ -3312,14 +4021,28 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J34" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H34=I34,"",1)</f>
         <v/>
       </c>
       <c r="K34" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L34" s="3">
+        <f>IF(K34=M34,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M34" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="N34" s="3" t="e">
+        <f>VLOOKUP(A34,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O34" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
@@ -3349,14 +4072,29 @@
         <v>611734</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H35=I35,"",1)</f>
         <v>1</v>
       </c>
       <c r="K35" s="3">
         <v>1411695.7132307691</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L35" s="3">
+        <f>IF(K35=M35,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="3">
+        <f>K35*0.85</f>
+        <v>1199941.3562461538</v>
+      </c>
+      <c r="N35" s="3">
+        <f>VLOOKUP(A35,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="3">
+        <v>1199941.3562461538</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>29</v>
       </c>
@@ -3386,14 +4124,29 @@
         <v>21334</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H36=I36,"",1)</f>
         <v>1</v>
       </c>
       <c r="K36" s="3">
         <v>42669.26666666667</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L36" s="3">
+        <f>IF(K36=M36,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <f>K36*1.15</f>
+        <v>49069.656666666669</v>
+      </c>
+      <c r="N36" s="3">
+        <f>VLOOKUP(A36,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="3">
+        <v>49069.656666666669</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
@@ -3423,14 +4176,29 @@
         <v>696941</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H37=I37,"",1)</f>
         <v>1</v>
       </c>
       <c r="K37" s="3">
         <v>1393882.4</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L37" s="3">
+        <f>IF(K37=M37,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="3">
+        <f>K37*1.25</f>
+        <v>1742353</v>
+      </c>
+      <c r="N37" s="3">
+        <f>VLOOKUP(A37,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="3">
+        <v>1742353</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>48</v>
       </c>
@@ -3457,48 +4225,85 @@
         <v>110.9</v>
       </c>
       <c r="J38" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H38=I38,"",1)</f>
         <v/>
       </c>
       <c r="K38" s="3">
         <v>110.9</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L38" s="3">
+        <f>IF(K38=M38,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M38" s="3">
+        <v>110.9</v>
+      </c>
+      <c r="N38" s="3">
+        <f>VLOOKUP(A38,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="3">
+        <v>110.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="C39" s="7">
-        <v>17230050.359999999</v>
+        <v>15150975.09</v>
       </c>
       <c r="D39" s="6">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E39" s="6">
-        <v>861502.51799999992</v>
+        <v>1893871.875</v>
       </c>
       <c r="F39" s="11">
-        <v>861502.5</v>
+        <v>1893871.875</v>
+      </c>
+      <c r="G39" s="4">
+        <v>10</v>
       </c>
       <c r="H39" s="3">
         <f>IF(ISBLANK(G39),F39,F39/G39)</f>
-        <v>861502.5</v>
+        <v>189387.1875</v>
       </c>
       <c r="I39" s="3">
-        <v>861502.5</v>
-      </c>
-      <c r="J39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>189387</v>
+      </c>
+      <c r="J39" s="3">
+        <f>IF(H39=I39,"",1)</f>
+        <v>1</v>
       </c>
       <c r="K39" s="3">
-        <v>861502.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>378774.375</v>
+      </c>
+      <c r="L39" s="3">
+        <f>IF(K39=M39,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="3">
+        <f>K39*0.85</f>
+        <v>321958.21875</v>
+      </c>
+      <c r="N39" s="3" t="str">
+        <f>VLOOKUP(A39,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O39" s="5">
+        <f>M39*0.75</f>
+        <v>241468.6640625</v>
+      </c>
+      <c r="P39" s="5">
+        <f>O39*0.75</f>
+        <v>181101.498046875</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>51</v>
       </c>
@@ -3525,14 +4330,28 @@
         <v>4273.9050960000004</v>
       </c>
       <c r="J40" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H40=I40,"",1)</f>
         <v/>
       </c>
       <c r="K40" s="3">
         <v>4273.9050960000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L40" s="3">
+        <f>IF(K40=M40,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M40" s="3">
+        <v>4273.9050960000004</v>
+      </c>
+      <c r="N40" s="3">
+        <f>VLOOKUP(A40,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O40" s="3">
+        <v>4273.9050960000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>191</v>
       </c>
@@ -3559,14 +4378,28 @@
         <v>0.05</v>
       </c>
       <c r="J41" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H41=I41,"",1)</f>
         <v/>
       </c>
       <c r="K41" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L41" s="3">
+        <f>IF(K41=M41,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="N41" s="3" t="e">
+        <f>VLOOKUP(A41,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O41" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>190</v>
       </c>
@@ -3593,14 +4426,28 @@
         <v>0.05</v>
       </c>
       <c r="J42" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H42=I42,"",1)</f>
         <v/>
       </c>
       <c r="K42" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L42" s="3">
+        <f>IF(K42=M42,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M42" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="N42" s="3" t="e">
+        <f>VLOOKUP(A42,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>20</v>
       </c>
@@ -3627,14 +4474,28 @@
         <v>80210</v>
       </c>
       <c r="J43" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H43=I43,"",1)</f>
         <v/>
       </c>
       <c r="K43" s="3">
         <v>80210</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L43" s="3">
+        <f>IF(K43=M43,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M43" s="3">
+        <v>80210</v>
+      </c>
+      <c r="N43" s="3">
+        <f>VLOOKUP(A43,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O43" s="3">
+        <v>80210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>56</v>
       </c>
@@ -3661,47 +4522,84 @@
         <v>28898.867849999999</v>
       </c>
       <c r="J44" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H44=I44,"",1)</f>
         <v/>
       </c>
       <c r="K44" s="3">
         <v>28898.867849999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L44" s="3">
+        <f>IF(K44=M44,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M44" s="3">
+        <v>28898.867849999999</v>
+      </c>
+      <c r="N44" s="3">
+        <f>VLOOKUP(A44,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O44" s="3">
+        <v>28898.867849999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C45" s="7">
-        <v>15779070.359999999</v>
+        <v>20527442.649999999</v>
       </c>
       <c r="D45" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E45" s="6">
-        <v>1314922.53</v>
+        <v>2052744.2649999999</v>
       </c>
       <c r="F45" s="11">
-        <v>1314922.53</v>
+        <v>2052744.2649999999</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4</v>
       </c>
       <c r="H45" s="3">
         <f>IF(ISBLANK(G45),F45,F45/G45)</f>
-        <v>1314922.53</v>
+        <v>513186.06624999997</v>
       </c>
       <c r="I45" s="3">
-        <v>27400000</v>
+        <v>22700000</v>
       </c>
       <c r="J45" s="3">
         <v>2</v>
       </c>
       <c r="K45" s="3">
-        <v>27400000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>22700000</v>
+      </c>
+      <c r="L45" s="3">
+        <f>IF(K45=M45,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M45" s="3">
+        <f>K45*0.75</f>
+        <v>17025000</v>
+      </c>
+      <c r="N45" s="3" t="str">
+        <f>VLOOKUP(A45,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>--</v>
+      </c>
+      <c r="O45" s="3">
+        <f>M45*0.75</f>
+        <v>12768750</v>
+      </c>
+      <c r="P45" s="5">
+        <f>O45*0.75</f>
+        <v>9576562.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
@@ -3728,14 +4626,28 @@
         <v>6221.5131609999999</v>
       </c>
       <c r="J46" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H46=I46,"",1)</f>
         <v/>
       </c>
       <c r="K46" s="3">
         <v>6221.5131609999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L46" s="3">
+        <f>IF(K46=M46,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M46" s="3">
+        <v>6221.5131609999999</v>
+      </c>
+      <c r="N46" s="3">
+        <f>VLOOKUP(A46,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O46" s="3">
+        <v>6221.5131609999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>31</v>
       </c>
@@ -3762,14 +4674,29 @@
         <v>4142428.1669999999</v>
       </c>
       <c r="J47" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H47=I47,"",1)</f>
         <v/>
       </c>
       <c r="K47" s="3">
         <v>4142428.1669999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L47" s="3">
+        <f>IF(K47=M47,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="3">
+        <f>K47*0.85</f>
+        <v>3521063.9419499999</v>
+      </c>
+      <c r="N47" s="3">
+        <f>VLOOKUP(A47,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O47" s="3">
+        <v>3521063.9419499999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>58</v>
       </c>
@@ -3799,14 +4726,29 @@
         <v>26</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H48=I48,"",1)</f>
         <v>1</v>
       </c>
       <c r="K48" s="3">
         <v>26.804801994999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L48" s="3">
+        <f>IF(K48=M48,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M48" s="3">
+        <f>K48*0.75</f>
+        <v>20.10360149625</v>
+      </c>
+      <c r="N48" s="3">
+        <f>VLOOKUP(A48,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O48" s="3">
+        <v>20.10360149625</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>47</v>
       </c>
@@ -3841,41 +4783,76 @@
       <c r="K49" s="3">
         <v>100000</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L49" s="3">
+        <f>IF(K49=M49,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M49" s="3">
+        <f>K49*0.75</f>
+        <v>75000</v>
+      </c>
+      <c r="N49" s="3">
+        <f>VLOOKUP(A49,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O49" s="3">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C50" s="7">
-        <v>5700290.8640000001</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>193</v>
+        <v>15779070.359999999</v>
+      </c>
+      <c r="D50" s="6">
+        <v>12</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1314922.53</v>
       </c>
       <c r="F50" s="11">
-        <v>5700290.8640000001</v>
+        <v>1314922.53</v>
       </c>
       <c r="H50" s="3">
         <f>IF(ISBLANK(G50),F50,F50/G50)</f>
-        <v>5700290.8640000001</v>
+        <v>1314922.53</v>
       </c>
       <c r="I50" s="3">
-        <v>134000000</v>
+        <v>27400000</v>
       </c>
       <c r="J50" s="3">
         <v>2</v>
       </c>
       <c r="K50" s="3">
-        <v>134000000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>27400000</v>
+      </c>
+      <c r="L50" s="3">
+        <f>IF(K50=M50,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M50" s="3">
+        <f>K50/10</f>
+        <v>2740000</v>
+      </c>
+      <c r="N50" s="3" t="str">
+        <f>VLOOKUP(A50,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O50" s="5">
+        <f>M50*0.75</f>
+        <v>2055000</v>
+      </c>
+      <c r="P50" s="3">
+        <f>C50</f>
+        <v>15779070.359999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>55</v>
       </c>
@@ -3902,14 +4879,28 @@
         <v>357460.29800000001</v>
       </c>
       <c r="J51" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H51=I51,"",1)</f>
         <v/>
       </c>
       <c r="K51" s="3">
         <v>357460.29800000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L51" s="3">
+        <f>IF(K51=M51,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M51" s="3">
+        <v>357460.29800000001</v>
+      </c>
+      <c r="N51" s="3">
+        <f>VLOOKUP(A51,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O51" s="3">
+        <v>357460.29800000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
@@ -3942,8 +4933,23 @@
       <c r="K52" s="3">
         <v>3943196.4866666668</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L52" s="3">
+        <f>IF(K52=M52,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M52" s="3">
+        <f>K52*1.25</f>
+        <v>4928995.6083333334</v>
+      </c>
+      <c r="N52" s="3">
+        <f>VLOOKUP(A52,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O52" s="3">
+        <v>4928995.6083333334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>28</v>
       </c>
@@ -3973,14 +4979,29 @@
         <v>48153936</v>
       </c>
       <c r="J53" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H53=I53,"",1)</f>
         <v/>
       </c>
       <c r="K53" s="3">
         <v>57784723.200000003</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L53" s="3">
+        <f>IF(K53=M53,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M53" s="3">
+        <f>K53*1.25</f>
+        <v>72230904</v>
+      </c>
+      <c r="N53" s="3">
+        <f>VLOOKUP(A53,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O53" s="3">
+        <v>72230904</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>60</v>
       </c>
@@ -4007,88 +5028,138 @@
         <v>7496.955054</v>
       </c>
       <c r="J54" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H54=I54,"",1)</f>
         <v/>
       </c>
       <c r="K54" s="3">
         <v>7496.955054</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L54" s="3">
+        <f>IF(K54=M54,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M54" s="3">
+        <v>7496.955054</v>
+      </c>
+      <c r="N54" s="3">
+        <f>VLOOKUP(A54,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O54" s="3">
+        <v>7496.955054</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C55" s="7">
-        <v>358999.37920000002</v>
-      </c>
-      <c r="D55" s="6">
-        <v>12</v>
-      </c>
-      <c r="E55" s="6">
-        <v>29916.614166666666</v>
+        <v>5700290.8640000001</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>193</v>
       </c>
       <c r="F55" s="11">
-        <v>29916.6</v>
-      </c>
-      <c r="G55" s="9">
-        <v>10</v>
+        <v>5700290.8640000001</v>
       </c>
       <c r="H55" s="3">
         <f>IF(ISBLANK(G55),F55,F55/G55)</f>
-        <v>2991.66</v>
+        <v>5700290.8640000001</v>
       </c>
       <c r="I55" s="3">
-        <v>2991</v>
+        <v>134000000</v>
       </c>
       <c r="J55" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K55" s="3">
-        <v>2991.66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>134000000</v>
+      </c>
+      <c r="L55" s="3">
+        <f>IF(K55=M55,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M55" s="3">
+        <f>K55*0.5</f>
+        <v>67000000</v>
+      </c>
+      <c r="N55" s="3" t="str">
+        <f>VLOOKUP(A55,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>--</v>
+      </c>
+      <c r="O55" s="3">
+        <f>M55/2</f>
+        <v>33500000</v>
+      </c>
+      <c r="P55" s="3">
+        <f>O55*0.75</f>
+        <v>25125000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C56" s="7">
-        <v>352590040.69999999</v>
+        <v>358999.37920000002</v>
       </c>
       <c r="D56" s="6">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E56" s="6">
-        <v>50370005.81428571</v>
+        <v>29916.614166666666</v>
       </c>
       <c r="F56" s="11">
-        <v>50370005.799999997</v>
-      </c>
-      <c r="G56" s="4">
-        <v>6</v>
+        <v>29916.6</v>
+      </c>
+      <c r="G56" s="9">
+        <v>10</v>
       </c>
       <c r="H56" s="3">
         <f>IF(ISBLANK(G56),F56,F56/G56)</f>
-        <v>8395000.9666666668</v>
+        <v>2991.66</v>
       </c>
       <c r="I56" s="3">
-        <v>6330000</v>
+        <v>2991</v>
       </c>
       <c r="J56" s="3">
+        <f>IF(H56=I56,"",1)</f>
         <v>1</v>
       </c>
       <c r="K56" s="3">
-        <f>I56/2</f>
-        <v>3165000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2991.66</v>
+      </c>
+      <c r="L56" s="3">
+        <f>IF(K56=M56,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M56" s="3">
+        <f>K56/2</f>
+        <v>1495.83</v>
+      </c>
+      <c r="N56" s="3" t="str">
+        <f>VLOOKUP(A56,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O56" s="3">
+        <f>M56*0.75</f>
+        <v>1121.8724999999999</v>
+      </c>
+      <c r="P56" s="3">
+        <f>O56*0.75</f>
+        <v>841.40437499999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>38</v>
       </c>
@@ -4118,14 +5189,28 @@
         <v>29180</v>
       </c>
       <c r="J57" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H57=I57,"",1)</f>
         <v>1</v>
       </c>
       <c r="K57" s="3">
         <v>58361.849450000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L57" s="3">
+        <f>IF(K57=M57,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M57" s="3">
+        <v>58361.849450000002</v>
+      </c>
+      <c r="N57" s="3">
+        <f>VLOOKUP(A57,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O57" s="3">
+        <v>58361.849450000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>15</v>
       </c>
@@ -4161,8 +5246,28 @@
         <f>I58/10</f>
         <v>5340000</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L58" s="3">
+        <f>IF(K58=M58,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M58" s="3">
+        <f>K58/2</f>
+        <v>2670000</v>
+      </c>
+      <c r="N58" s="3" t="str">
+        <f>VLOOKUP(A58,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>--</v>
+      </c>
+      <c r="O58" s="3">
+        <f>M58*0.5</f>
+        <v>1335000</v>
+      </c>
+      <c r="P58" s="3">
+        <f>O58*0.75</f>
+        <v>1001250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>39</v>
       </c>
@@ -4192,14 +5297,34 @@
         <v>17712</v>
       </c>
       <c r="J59" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H59=I59,"",1)</f>
         <v>1</v>
       </c>
       <c r="K59" s="3">
         <v>35425.880900000004</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L59" s="3">
+        <f>IF(K59=M59,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M59" s="3">
+        <f>K59/2</f>
+        <v>17712.940450000002</v>
+      </c>
+      <c r="N59" s="3" t="str">
+        <f>VLOOKUP(A59,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>--</v>
+      </c>
+      <c r="O59" s="3">
+        <f>M59/2</f>
+        <v>8856.4702250000009</v>
+      </c>
+      <c r="P59" s="3">
+        <f>O59*0.75</f>
+        <v>6642.3526687500007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>34</v>
       </c>
@@ -4235,8 +5360,28 @@
         <f>I60/10</f>
         <v>142000</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L60" s="3">
+        <f>IF(K60=M60,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M60" s="3">
+        <f>I60/5</f>
+        <v>284000</v>
+      </c>
+      <c r="N60" s="3" t="str">
+        <f>VLOOKUP(A60,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+</v>
+      </c>
+      <c r="O60" s="3">
+        <f>M60*1.5</f>
+        <v>426000</v>
+      </c>
+      <c r="P60" s="3">
+        <f>O60*1.5</f>
+        <v>639000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>61</v>
       </c>
@@ -4263,14 +5408,28 @@
         <v>71.004761549999998</v>
       </c>
       <c r="J61" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H61=I61,"",1)</f>
         <v/>
       </c>
       <c r="K61" s="3">
         <v>71.004761549999998</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L61" s="3">
+        <f>IF(K61=M61,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M61" s="3">
+        <v>71.004761549999998</v>
+      </c>
+      <c r="N61" s="3">
+        <f>VLOOKUP(A61,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O61" s="3">
+        <v>71.004761549999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>12</v>
       </c>
@@ -4306,8 +5465,23 @@
         <f>I62*1.5</f>
         <v>7530000</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L62" s="3">
+        <f>IF(K62=M62,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M62" s="3">
+        <f>K62*0.85</f>
+        <v>6400500</v>
+      </c>
+      <c r="N62" s="3">
+        <f>VLOOKUP(A62,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O62" s="3">
+        <v>6400500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>14</v>
       </c>
@@ -4337,14 +5511,29 @@
         <v>439802</v>
       </c>
       <c r="J63" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H63=I63,"",1)</f>
         <v>1</v>
       </c>
       <c r="K63" s="3">
         <v>879605.2</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L63" s="3">
+        <f>IF(K63=M63,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M63" s="3">
+        <f>K63*0.85</f>
+        <v>747664.41999999993</v>
+      </c>
+      <c r="N63" s="3">
+        <f>VLOOKUP(A63,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O63" s="3">
+        <v>747664.41999999993</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>16</v>
       </c>
@@ -4380,8 +5569,28 @@
         <f>I64/1.5</f>
         <v>21600000</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L64" s="3">
+        <f>IF(K64=M64,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M64" s="3">
+        <f>K64/1.5</f>
+        <v>14400000</v>
+      </c>
+      <c r="N64" s="3" t="str">
+        <f>VLOOKUP(A64,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>--</v>
+      </c>
+      <c r="O64" s="3">
+        <f>M64*0.75</f>
+        <v>10800000</v>
+      </c>
+      <c r="P64" s="3">
+        <f>O64/10</f>
+        <v>1080000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>52</v>
       </c>
@@ -4411,14 +5620,34 @@
         <v>42857</v>
       </c>
       <c r="J65" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(H65=I65,"",1)</f>
         <v>1</v>
       </c>
       <c r="K65" s="3">
         <v>42857.142857142855</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L65" s="3">
+        <f>IF(K65=M65,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M65" s="3">
+        <f>K65*0.75</f>
+        <v>32142.857142857141</v>
+      </c>
+      <c r="N65" s="3" t="str">
+        <f>VLOOKUP(A65,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O65" s="3">
+        <f>M65*0.75</f>
+        <v>24107.142857142855</v>
+      </c>
+      <c r="P65" s="3">
+        <f>O65*0.75</f>
+        <v>18080.357142857141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>17</v>
       </c>
@@ -4445,14 +5674,34 @@
         <v>2026568.5109999999</v>
       </c>
       <c r="J66" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H66=I66,"",1)</f>
         <v/>
       </c>
       <c r="K66" s="3">
         <v>2026568.5109999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L66" s="3">
+        <f>IF(K66=M66,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M66" s="3">
+        <f>K66*0.85</f>
+        <v>1722583.2343499998</v>
+      </c>
+      <c r="N66" s="3" t="str">
+        <f>VLOOKUP(A66,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O66" s="3">
+        <f>M66*0.75</f>
+        <v>1291937.4257624999</v>
+      </c>
+      <c r="P66" s="3">
+        <f>O66*0.75</f>
+        <v>968953.06932187499</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>40</v>
       </c>
@@ -4487,8 +5736,22 @@
       <c r="K67" s="3">
         <v>491000</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L67" s="3">
+        <f>IF(K67=M67,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M67" s="3">
+        <v>491000</v>
+      </c>
+      <c r="N67" s="3">
+        <f>VLOOKUP(A67,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O67" s="3">
+        <v>491000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>44</v>
       </c>
@@ -4523,18 +5786,38 @@
       <c r="K68" s="3">
         <v>2925788</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L68" s="3">
+        <f>IF(K68=M68,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M68" s="3">
+        <f>K68*0.85</f>
+        <v>2486919.7999999998</v>
+      </c>
+      <c r="N68" s="3" t="str">
+        <f>VLOOKUP(A68,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="O68" s="3">
+        <f>M68*0.75</f>
+        <v>1865189.8499999999</v>
+      </c>
+      <c r="P68" s="3">
+        <f>O68*0.75</f>
+        <v>1398892.3875</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -4542,17 +5825,23 @@
       <c r="E71"/>
       <c r="F71" s="12"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B72"/>
       <c r="C72"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K68">
-    <filterColumn colId="9">
+  <autoFilter ref="A1:O68">
+    <filterColumn colId="13">
       <filters>
-        <filter val="1"/>
+        <filter val="-"/>
+        <filter val="--"/>
+        <filter val="---"/>
+        <filter val="+"/>
       </filters>
     </filterColumn>
+    <sortState ref="A3:O68">
+      <sortCondition ref="A1:A68"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Final Tuning for Predator Reduction
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Group Condition" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="212">
   <si>
     <t>Too High</t>
   </si>
@@ -643,18 +643,12 @@
     <t>-</t>
   </si>
   <si>
-    <t>--</t>
-  </si>
-  <si>
     <t>Too High Early</t>
   </si>
   <si>
     <t>RemovePred5_tochange</t>
   </si>
   <si>
-    <t>---</t>
-  </si>
-  <si>
     <t>RemovePred5_KDENR</t>
   </si>
   <si>
@@ -665,6 +659,12 @@
   </si>
   <si>
     <t>RemovePred6_Change</t>
+  </si>
+  <si>
+    <t>ORIG</t>
+  </si>
+  <si>
+    <t>RemovePred_KDENR</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1071,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
+      <selection pane="bottomLeft" activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1095,7 @@
         <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1113,7 +1113,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1127,21 +1127,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D3" t="s">
-        <v>181</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>204</v>
+      <c r="H3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1180,7 +1174,7 @@
         <v>181</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1194,7 +1188,7 @@
         <v>181</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1305,21 +1299,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>120</v>
       </c>
-      <c r="C17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" t="s">
-        <v>181</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>207</v>
+      <c r="H17" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1347,7 +1335,7 @@
         <v>181</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1422,7 +1410,7 @@
         <v>181</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1435,11 +1423,8 @@
       <c r="C26" t="s">
         <v>181</v>
       </c>
-      <c r="H26" t="s">
-        <v>181</v>
-      </c>
       <c r="I26" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1453,21 +1438,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
       <c r="B28" t="s">
         <v>132</v>
       </c>
-      <c r="C28" t="s">
-        <v>181</v>
-      </c>
       <c r="H28" t="s">
         <v>181</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1484,7 +1463,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -1520,7 +1499,7 @@
         <v>181</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1628,7 +1607,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1653,7 +1632,7 @@
         <v>181</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1678,7 +1657,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -1690,6 +1669,9 @@
       </c>
       <c r="G46" t="s">
         <v>181</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1761,7 +1743,7 @@
         <v>181</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1830,21 +1812,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>30</v>
       </c>
       <c r="B59" t="s">
         <v>118</v>
       </c>
-      <c r="C59" t="s">
-        <v>181</v>
-      </c>
-      <c r="D59" t="s">
-        <v>181</v>
-      </c>
-      <c r="I59" s="13" t="s">
-        <v>203</v>
+      <c r="H59" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1858,7 +1834,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -1868,8 +1844,8 @@
       <c r="E61" t="s">
         <v>181</v>
       </c>
-      <c r="I61" s="13" t="s">
-        <v>202</v>
+      <c r="G61" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1932,11 +1908,8 @@
       <c r="D66" t="s">
         <v>181</v>
       </c>
-      <c r="G66" t="s">
-        <v>181</v>
-      </c>
       <c r="I66" s="13" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2041,7 +2014,7 @@
         <v>181</v>
       </c>
       <c r="I75" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -2058,7 +2031,7 @@
         <v>181</v>
       </c>
       <c r="I76" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2072,24 +2045,18 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>15</v>
       </c>
       <c r="B78" t="s">
         <v>98</v>
       </c>
-      <c r="C78" t="s">
-        <v>181</v>
-      </c>
-      <c r="D78" t="s">
-        <v>181</v>
-      </c>
-      <c r="G78" t="s">
-        <v>181</v>
-      </c>
-      <c r="I78" s="13" t="s">
-        <v>204</v>
+      <c r="F78" t="s">
+        <v>181</v>
+      </c>
+      <c r="H78" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -2109,7 +2076,7 @@
         <v>181</v>
       </c>
       <c r="I79" s="13" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2137,7 +2104,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -2149,6 +2116,9 @@
       </c>
       <c r="G82" t="s">
         <v>181</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2165,21 +2135,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>16</v>
       </c>
       <c r="B84" t="s">
         <v>99</v>
       </c>
-      <c r="C84" t="s">
-        <v>181</v>
-      </c>
-      <c r="D84" t="s">
-        <v>181</v>
-      </c>
-      <c r="I84" s="13" t="s">
-        <v>204</v>
+      <c r="H84" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -2199,7 +2163,7 @@
         <v>181</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -2216,7 +2180,7 @@
         <v>181</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2247,7 +2211,7 @@
         <v>181</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2257,10 +2221,8 @@
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="7">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2269,14 +2231,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U50" sqref="U50"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2297,10 +2258,11 @@
     <col min="14" max="14" width="8.88671875" style="3"/>
     <col min="15" max="15" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="3"/>
+    <col min="17" max="17" width="20.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>91</v>
       </c>
@@ -2335,22 +2297,25 @@
         <v>199</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2370,7 +2335,7 @@
         <v>66739628</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H33" si="0">IF(ISBLANK(G2),F2,F2/G2)</f>
+        <f t="shared" ref="H2" si="0">IF(ISBLANK(G2),F2,F2/G2)</f>
         <v>66739628</v>
       </c>
       <c r="I2" s="3">
@@ -2397,7 +2362,7 @@
         <v>45700000</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -2417,7 +2382,7 @@
         <v>2124041.1490000002</v>
       </c>
       <c r="H3" s="3">
-        <f>IF(ISBLANK(G3),F3,F3/G3)</f>
+        <f t="shared" ref="H3:H34" si="1">IF(ISBLANK(G3),F3,F3/G3)</f>
         <v>2124041.1490000002</v>
       </c>
       <c r="I3" s="3">
@@ -2431,7 +2396,7 @@
         <v>10000000</v>
       </c>
       <c r="L3" s="3">
-        <f>IF(K3=M3,1,0)</f>
+        <f t="shared" ref="L3:L34" si="2">IF(K3=M3,1,0)</f>
         <v>0</v>
       </c>
       <c r="M3" s="5">
@@ -2440,7 +2405,7 @@
       </c>
       <c r="N3" s="3" t="str">
         <f>VLOOKUP(A3,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O3" s="5">
         <f>M3*0.75</f>
@@ -2450,8 +2415,12 @@
         <f>O3*0.5</f>
         <v>2812500</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q3" s="3">
+        <f>C3</f>
+        <v>2124041.1490000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2471,7 +2440,7 @@
         <v>19030173</v>
       </c>
       <c r="H4" s="3">
-        <f>IF(ISBLANK(G4),F4,F4/G4)</f>
+        <f t="shared" si="1"/>
         <v>19030173</v>
       </c>
       <c r="I4" s="3">
@@ -2485,7 +2454,7 @@
         <v>19030173</v>
       </c>
       <c r="L4" s="3">
-        <f>IF(K4=M4,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M4" s="3">
@@ -2500,7 +2469,7 @@
         <v>19030174.25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -2523,7 +2492,7 @@
         <v>0.25</v>
       </c>
       <c r="H5" s="3">
-        <f>IF(ISBLANK(G5),F5,F5/G5)</f>
+        <f t="shared" si="1"/>
         <v>63265.246760000002</v>
       </c>
       <c r="I5" s="3">
@@ -2537,7 +2506,7 @@
         <v>63265</v>
       </c>
       <c r="L5" s="3">
-        <f>IF(K5=M5,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M5" s="3">
@@ -2551,7 +2520,7 @@
         <v>63265</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>32</v>
       </c>
@@ -2574,7 +2543,7 @@
         <v>75</v>
       </c>
       <c r="H6" s="3">
-        <f>IF(ISBLANK(G6),F6,F6/G6)</f>
+        <f t="shared" si="1"/>
         <v>22916.765253333335</v>
       </c>
       <c r="I6" s="3">
@@ -2587,16 +2556,16 @@
         <v>36100000000</v>
       </c>
       <c r="L6" s="3">
-        <f>IF(K6=M6,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M6" s="3">
         <f>K6/100</f>
         <v>361000000</v>
       </c>
-      <c r="N6" s="3" t="str">
+      <c r="N6" s="3">
         <f>VLOOKUP(A6,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>---</v>
+        <v>0</v>
       </c>
       <c r="O6" s="3">
         <f>M6/5</f>
@@ -2607,7 +2576,7 @@
         <v>54150000</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -2630,21 +2599,21 @@
         <v>5</v>
       </c>
       <c r="H7" s="3">
-        <f>IF(ISBLANK(G7),F7,F7/G7)</f>
+        <f t="shared" si="1"/>
         <v>470787.3</v>
       </c>
       <c r="I7" s="3">
         <v>470787</v>
       </c>
       <c r="J7" s="3">
-        <f>IF(H7=I7,"",1)</f>
+        <f t="shared" ref="J7:J13" si="3">IF(H7=I7,"",1)</f>
         <v>1</v>
       </c>
       <c r="K7" s="11">
         <v>2353936.5</v>
       </c>
       <c r="L7" s="3">
-        <f>IF(K7=M7,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M7" s="11">
@@ -2653,7 +2622,7 @@
       </c>
       <c r="N7" s="3" t="str">
         <f>VLOOKUP(A7,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O7" s="3">
         <f>M7*0.75</f>
@@ -2663,8 +2632,12 @@
         <f>O7*0.75</f>
         <v>993066.9609375</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q7" s="3">
+        <f>C7</f>
+        <v>16477555.609999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -2687,21 +2660,21 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="3">
-        <f>IF(ISBLANK(G8),F8,F8/G8)</f>
+        <f t="shared" si="1"/>
         <v>1000000000000</v>
       </c>
       <c r="I8" s="3">
         <v>1000000000000</v>
       </c>
       <c r="J8" s="3" t="str">
-        <f>IF(H8=I8,"",1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K8" s="3">
         <v>1000000000000</v>
       </c>
       <c r="L8" s="3">
-        <f>IF(K8=M8,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M8" s="3">
@@ -2715,7 +2688,7 @@
         <v>2000000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -2738,21 +2711,21 @@
         <v>15</v>
       </c>
       <c r="H9" s="3">
-        <f>IF(ISBLANK(G9),F9,F9/G9)</f>
+        <f t="shared" si="1"/>
         <v>214151453.67000002</v>
       </c>
       <c r="I9" s="3">
         <v>214151453</v>
       </c>
       <c r="J9" s="3">
-        <f>IF(H9=I9,"",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K9" s="11">
         <v>3212271805.0500002</v>
       </c>
       <c r="L9" s="3">
-        <f>IF(K9=M9,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M9" s="11">
@@ -2767,7 +2740,7 @@
         <v>4015339756.3125</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
@@ -2787,21 +2760,21 @@
         <v>2123.8950410000002</v>
       </c>
       <c r="H10" s="3">
-        <f>IF(ISBLANK(G10),F10,F10/G10)</f>
+        <f t="shared" si="1"/>
         <v>2123.8950410000002</v>
       </c>
       <c r="I10" s="3">
         <v>2123.8950410000002</v>
       </c>
       <c r="J10" s="3" t="str">
-        <f>IF(H10=I10,"",1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K10" s="3">
         <v>2123.8950410000002</v>
       </c>
       <c r="L10" s="3">
-        <f>IF(K10=M10,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M10" s="3">
@@ -2815,7 +2788,7 @@
         <v>2123.8950410000002</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
@@ -2835,21 +2808,21 @@
         <v>74822.192989999996</v>
       </c>
       <c r="H11" s="3">
-        <f>IF(ISBLANK(G11),F11,F11/G11)</f>
+        <f t="shared" si="1"/>
         <v>74822.192989999996</v>
       </c>
       <c r="I11" s="3">
         <v>74822.192989999996</v>
       </c>
       <c r="J11" s="3" t="str">
-        <f>IF(H11=I11,"",1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K11" s="11">
         <v>74822.192989999996</v>
       </c>
       <c r="L11" s="3">
-        <f>IF(K11=M11,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M11" s="11">
@@ -2863,7 +2836,7 @@
         <v>74822.192989999996</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>59</v>
       </c>
@@ -2886,21 +2859,21 @@
         <v>10</v>
       </c>
       <c r="H12" s="3">
-        <f>IF(ISBLANK(G12),F12,F12/G12)</f>
+        <f t="shared" si="1"/>
         <v>23.545910710000001</v>
       </c>
       <c r="I12" s="3">
         <v>23</v>
       </c>
       <c r="J12" s="3">
-        <f>IF(H12=I12,"",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K12" s="3">
         <v>23.545910710000001</v>
       </c>
       <c r="L12" s="3">
-        <f>IF(K12=M12,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M12" s="3">
@@ -2914,7 +2887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
@@ -2937,21 +2910,21 @@
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <f>IF(ISBLANK(G13),F13,F13/G13)</f>
+        <f t="shared" si="1"/>
         <v>51.594000000000008</v>
       </c>
       <c r="I13" s="3">
         <v>51</v>
       </c>
       <c r="J13" s="3">
-        <f>IF(H13=I13,"",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K13" s="3">
         <v>150</v>
       </c>
       <c r="L13" s="3">
-        <f>IF(K13=M13,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M13" s="3">
@@ -2965,7 +2938,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>45</v>
       </c>
@@ -2988,7 +2961,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="3">
-        <f>IF(ISBLANK(G14),F14,F14/G14)</f>
+        <f t="shared" si="1"/>
         <v>8395000.9666666668</v>
       </c>
       <c r="I14" s="3">
@@ -3002,7 +2975,7 @@
         <v>3165000</v>
       </c>
       <c r="L14" s="3">
-        <f>IF(K14=M14,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M14" s="3">
@@ -3011,7 +2984,7 @@
       </c>
       <c r="N14" s="3" t="str">
         <f>VLOOKUP(A14,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O14" s="3">
         <f>M14*0.75</f>
@@ -3021,8 +2994,12 @@
         <f>C14</f>
         <v>352590040.69999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q14" s="3">
+        <f>C14</f>
+        <v>352590040.69999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
@@ -3042,21 +3019,21 @@
         <v>15874.27808</v>
       </c>
       <c r="H15" s="3">
-        <f>IF(ISBLANK(G15),F15,F15/G15)</f>
+        <f t="shared" si="1"/>
         <v>15874.27808</v>
       </c>
       <c r="I15" s="3">
         <v>15874.27808</v>
       </c>
       <c r="J15" s="3" t="str">
-        <f>IF(H15=I15,"",1)</f>
+        <f t="shared" ref="J15:J23" si="4">IF(H15=I15,"",1)</f>
         <v/>
       </c>
       <c r="K15" s="3">
         <v>15874.27808</v>
       </c>
       <c r="L15" s="3">
-        <f>IF(K15=M15,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M15" s="3">
@@ -3070,7 +3047,7 @@
         <v>15874.27808</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
@@ -3093,21 +3070,21 @@
         <v>10</v>
       </c>
       <c r="H16" s="3">
-        <f>IF(ISBLANK(G16),F16,F16/G16)</f>
+        <f t="shared" si="1"/>
         <v>12930.9</v>
       </c>
       <c r="I16" s="3">
         <v>12930</v>
       </c>
       <c r="J16" s="3">
-        <f>IF(H16=I16,"",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K16" s="3">
         <v>12930.9</v>
       </c>
       <c r="L16" s="3">
-        <f>IF(K16=M16,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M16" s="5">
@@ -3116,7 +3093,7 @@
       </c>
       <c r="N16" s="3" t="str">
         <f>VLOOKUP(A16,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O16" s="5">
         <f>M16*0.75</f>
@@ -3126,8 +3103,12 @@
         <f>O16*0.75</f>
         <v>5455.2234374999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q16" s="3">
+        <f>C16</f>
+        <v>129309.07709999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
@@ -3150,21 +3131,21 @@
         <v>10</v>
       </c>
       <c r="H17" s="3">
-        <f>IF(ISBLANK(G17),F17,F17/G17)</f>
+        <f t="shared" si="1"/>
         <v>2199610.6069999998</v>
       </c>
       <c r="I17" s="3">
         <v>8700000</v>
       </c>
       <c r="J17" s="3">
-        <f>IF(H17=I17,"",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K17" s="5">
         <v>4000000</v>
       </c>
       <c r="L17" s="3">
-        <f>IF(K17=M17,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M17" s="5">
@@ -3178,7 +3159,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
@@ -3198,21 +3179,21 @@
         <v>861502.5</v>
       </c>
       <c r="H18" s="3">
-        <f>IF(ISBLANK(G18),F18,F18/G18)</f>
+        <f t="shared" si="1"/>
         <v>861502.5</v>
       </c>
       <c r="I18" s="3">
         <v>861502.5</v>
       </c>
       <c r="J18" s="3" t="str">
-        <f>IF(H18=I18,"",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K18" s="3">
         <v>861502.5</v>
       </c>
       <c r="L18" s="3">
-        <f>IF(K18=M18,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M18" s="3">
@@ -3221,18 +3202,22 @@
       </c>
       <c r="N18" s="3" t="str">
         <f>VLOOKUP(A18,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O18" s="5">
         <f>M18*0.75</f>
         <v>549207.84375</v>
       </c>
       <c r="P18" s="5">
-        <f t="shared" ref="P18:P20" si="1">O18*0.75</f>
+        <f t="shared" ref="P18:P20" si="5">O18*0.75</f>
         <v>411905.8828125</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q18" s="3">
+        <f t="shared" ref="Q18:Q20" si="6">C18</f>
+        <v>17230050.359999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -3255,21 +3240,21 @@
         <v>7</v>
       </c>
       <c r="H19" s="3">
-        <f>IF(ISBLANK(G19),F19,F19/G19)</f>
+        <f t="shared" si="1"/>
         <v>189098.12857142856</v>
       </c>
       <c r="I19" s="3">
         <v>189098</v>
       </c>
       <c r="J19" s="3">
-        <f>IF(H19=I19,"",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K19" s="3">
         <v>189098.12857142856</v>
       </c>
       <c r="L19" s="3">
-        <f>IF(K19=M19,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M19" s="5">
@@ -3278,18 +3263,22 @@
       </c>
       <c r="N19" s="3" t="str">
         <f>VLOOKUP(A19,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O19" s="5">
         <f>M19*0.75</f>
         <v>106367.69732142857</v>
       </c>
       <c r="P19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>79775.772991071426</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q19" s="3">
+        <f t="shared" si="6"/>
+        <v>13236869.029999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>25</v>
       </c>
@@ -3312,21 +3301,21 @@
         <v>10</v>
       </c>
       <c r="H20" s="3">
-        <f>IF(ISBLANK(G20),F20,F20/G20)</f>
+        <f t="shared" si="1"/>
         <v>2162721.7000000002</v>
       </c>
       <c r="I20" s="3">
         <v>2162721</v>
       </c>
       <c r="J20" s="3">
-        <f>IF(H20=I20,"",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K20" s="3">
         <v>4325443.4000000004</v>
       </c>
       <c r="L20" s="3">
-        <f>IF(K20=M20,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M20" s="3">
@@ -3335,18 +3324,22 @@
       </c>
       <c r="N20" s="3" t="str">
         <f>VLOOKUP(A20,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O20" s="5">
         <f>M20*0.75</f>
         <v>2433061.9125000001</v>
       </c>
       <c r="P20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1824796.4343750002</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q20" s="3">
+        <f t="shared" si="6"/>
+        <v>432544359.30000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>187</v>
       </c>
@@ -3366,21 +3359,21 @@
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="H21" s="3">
-        <f>IF(ISBLANK(G21),F21,F21/G21)</f>
+        <f t="shared" si="1"/>
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="I21" s="3">
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="J21" s="3" t="str">
-        <f>IF(H21=I21,"",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K21" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="L21" s="3">
-        <f>IF(K21=M21,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M21" s="3">
@@ -3394,7 +3387,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>186</v>
       </c>
@@ -3414,21 +3407,21 @@
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="H22" s="3">
-        <f>IF(ISBLANK(G22),F22,F22/G22)</f>
+        <f t="shared" si="1"/>
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="I22" s="3">
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f>IF(H22=I22,"",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K22" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="L22" s="3">
-        <f>IF(K22=M22,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M22" s="3">
@@ -3442,7 +3435,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>62</v>
       </c>
@@ -3462,21 +3455,21 @@
         <v>149515.5</v>
       </c>
       <c r="H23" s="3">
-        <f>IF(ISBLANK(G23),F23,F23/G23)</f>
+        <f t="shared" si="1"/>
         <v>149515.5</v>
       </c>
       <c r="I23" s="3">
         <v>149515.5</v>
       </c>
       <c r="J23" s="3" t="str">
-        <f>IF(H23=I23,"",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K23" s="3">
         <v>350000</v>
       </c>
       <c r="L23" s="3">
-        <f>IF(K23=M23,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M23" s="3">
@@ -3492,7 +3485,7 @@
         <v>196875</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>43</v>
       </c>
@@ -3512,7 +3505,7 @@
         <v>34529920</v>
       </c>
       <c r="H24" s="3">
-        <f>IF(ISBLANK(G24),F24,F24/G24)</f>
+        <f t="shared" si="1"/>
         <v>34529920</v>
       </c>
       <c r="I24" s="3">
@@ -3525,16 +3518,16 @@
         <v>104000000</v>
       </c>
       <c r="L24" s="3">
-        <f>IF(K24=M24,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M24" s="3">
         <f>K24*0.85</f>
         <v>88400000</v>
       </c>
-      <c r="N24" s="3" t="str">
+      <c r="N24" s="3">
         <f>VLOOKUP(A24,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="O24" s="5">
         <f>M24*0.75</f>
@@ -3545,7 +3538,7 @@
         <v>49725000</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>185</v>
       </c>
@@ -3565,7 +3558,7 @@
         <v>0.01</v>
       </c>
       <c r="H25" s="3">
-        <f>IF(ISBLANK(G25),F25,F25/G25)</f>
+        <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
       <c r="I25" s="3">
@@ -3579,7 +3572,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="L25" s="3">
-        <f>IF(K25=M25,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M25" s="3">
@@ -3593,7 +3586,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>184</v>
       </c>
@@ -3613,7 +3606,7 @@
         <v>0.01</v>
       </c>
       <c r="H26" s="3">
-        <f>IF(ISBLANK(G26),F26,F26/G26)</f>
+        <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
       <c r="I26" s="3">
@@ -3627,7 +3620,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="L26" s="3">
-        <f>IF(K26=M26,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M26" s="3">
@@ -3641,7 +3634,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
@@ -3661,7 +3654,7 @@
         <v>100000000</v>
       </c>
       <c r="H27" s="3">
-        <f>IF(ISBLANK(G27),F27,F27/G27)</f>
+        <f t="shared" si="1"/>
         <v>100000000</v>
       </c>
       <c r="I27" s="3">
@@ -3674,7 +3667,7 @@
         <v>181000000</v>
       </c>
       <c r="L27" s="3">
-        <f>IF(K27=M27,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M27" s="3">
@@ -3689,7 +3682,7 @@
         <v>226250000</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -3712,21 +3705,21 @@
         <v>2</v>
       </c>
       <c r="H28" s="3">
-        <f>IF(ISBLANK(G28),F28,F28/G28)</f>
+        <f t="shared" si="1"/>
         <v>374.91549774999999</v>
       </c>
       <c r="I28" s="3">
         <v>375</v>
       </c>
       <c r="J28" s="3">
-        <f>IF(H28=I28,"",1)</f>
+        <f t="shared" ref="J28:J44" si="7">IF(H28=I28,"",1)</f>
         <v>1</v>
       </c>
       <c r="K28" s="3">
         <v>150</v>
       </c>
       <c r="L28" s="3">
-        <f>IF(K28=M28,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M28" s="3">
@@ -3740,7 +3733,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>22</v>
       </c>
@@ -3760,21 +3753,21 @@
         <v>4986608.142</v>
       </c>
       <c r="H29" s="3">
-        <f>IF(ISBLANK(G29),F29,F29/G29)</f>
+        <f t="shared" si="1"/>
         <v>4986608.142</v>
       </c>
       <c r="I29" s="3">
         <v>4986608.142</v>
       </c>
       <c r="J29" s="3" t="str">
-        <f>IF(H29=I29,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K29" s="3">
         <v>4986608.142</v>
       </c>
       <c r="L29" s="3">
-        <f>IF(K29=M29,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M29" s="3">
@@ -3788,7 +3781,7 @@
         <v>4986608.142</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>42</v>
       </c>
@@ -3811,21 +3804,21 @@
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <f>IF(ISBLANK(G30),F30,F30/G30)</f>
+        <f t="shared" si="1"/>
         <v>6976733.6599999992</v>
       </c>
       <c r="I30" s="3">
         <v>6976733</v>
       </c>
       <c r="J30" s="3">
-        <f>IF(H30=I30,"",1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K30" s="3">
         <v>13953467.319999998</v>
       </c>
       <c r="L30" s="3">
-        <f>IF(K30=M30,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M30" s="3">
@@ -3841,7 +3834,7 @@
         <v>7848825.3674999988</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>9</v>
       </c>
@@ -3861,21 +3854,21 @@
         <v>1696.14</v>
       </c>
       <c r="H31" s="3">
-        <f>IF(ISBLANK(G31),F31,F31/G31)</f>
+        <f t="shared" si="1"/>
         <v>1696.14</v>
       </c>
       <c r="I31" s="3">
         <v>1696.14</v>
       </c>
       <c r="J31" s="3" t="str">
-        <f>IF(H31=I31,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K31" s="3">
         <v>1696.14</v>
       </c>
       <c r="L31" s="3">
-        <f>IF(K31=M31,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M31" s="3">
@@ -3884,7 +3877,7 @@
       </c>
       <c r="N31" s="3" t="str">
         <f>VLOOKUP(A31,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O31" s="3">
         <f>M31*0.75</f>
@@ -3894,8 +3887,12 @@
         <f>O31*0.75</f>
         <v>715.55906249999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q31" s="3">
+        <f>C31</f>
+        <v>254421.22440000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>54</v>
       </c>
@@ -3918,21 +3915,21 @@
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <f>IF(ISBLANK(G32),F32,F32/G32)</f>
+        <f t="shared" si="1"/>
         <v>164351.5</v>
       </c>
       <c r="I32" s="3">
         <v>164351</v>
       </c>
       <c r="J32" s="3">
-        <f>IF(H32=I32,"",1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K32" s="3">
         <v>328703</v>
       </c>
       <c r="L32" s="3">
-        <f>IF(K32=M32,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M32" s="3">
@@ -3946,7 +3943,7 @@
         <v>328703</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>189</v>
       </c>
@@ -3966,21 +3963,21 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="H33" s="3">
-        <f>IF(ISBLANK(G33),F33,F33/G33)</f>
+        <f t="shared" si="1"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="I33" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J33" s="3" t="str">
-        <f>IF(H33=I33,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K33" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="L33" s="3">
-        <f>IF(K33=M33,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M33" s="3">
@@ -3994,7 +3991,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>188</v>
       </c>
@@ -4014,21 +4011,21 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="H34" s="3">
-        <f>IF(ISBLANK(G34),F34,F34/G34)</f>
+        <f t="shared" si="1"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="I34" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J34" s="3" t="str">
-        <f>IF(H34=I34,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K34" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="L34" s="3">
-        <f>IF(K34=M34,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M34" s="3">
@@ -4042,7 +4039,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
@@ -4065,36 +4062,40 @@
         <v>7.5</v>
       </c>
       <c r="H35" s="3">
-        <f>IF(ISBLANK(G35),F35,F35/G35)</f>
+        <f t="shared" ref="H35:H66" si="8">IF(ISBLANK(G35),F35,F35/G35)</f>
         <v>611734.80906666664</v>
       </c>
       <c r="I35" s="3">
         <v>611734</v>
       </c>
       <c r="J35" s="3">
-        <f>IF(H35=I35,"",1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K35" s="3">
         <v>1411695.7132307691</v>
       </c>
       <c r="L35" s="3">
-        <f>IF(K35=M35,1,0)</f>
+        <f t="shared" ref="L35:L66" si="9">IF(K35=M35,1,0)</f>
         <v>0</v>
       </c>
       <c r="M35" s="3">
         <f>K35*0.85</f>
         <v>1199941.3562461538</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35" s="3" t="str">
         <f>VLOOKUP(A35,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>ORIG</v>
       </c>
       <c r="O35" s="3">
         <v>1199941.3562461538</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q35" s="3">
+        <f>C35</f>
+        <v>22940055.34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>29</v>
       </c>
@@ -4117,21 +4118,21 @@
         <v>6</v>
       </c>
       <c r="H36" s="3">
-        <f>IF(ISBLANK(G36),F36,F36/G36)</f>
+        <f t="shared" si="8"/>
         <v>21334.633333333335</v>
       </c>
       <c r="I36" s="3">
         <v>21334</v>
       </c>
       <c r="J36" s="3">
-        <f>IF(H36=I36,"",1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K36" s="3">
         <v>42669.26666666667</v>
       </c>
       <c r="L36" s="3">
-        <f>IF(K36=M36,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M36" s="3">
@@ -4146,7 +4147,7 @@
         <v>49069.656666666669</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
@@ -4169,21 +4170,21 @@
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <f>IF(ISBLANK(G37),F37,F37/G37)</f>
+        <f t="shared" si="8"/>
         <v>696941.2</v>
       </c>
       <c r="I37" s="3">
         <v>696941</v>
       </c>
       <c r="J37" s="3">
-        <f>IF(H37=I37,"",1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K37" s="3">
         <v>1393882.4</v>
       </c>
       <c r="L37" s="3">
-        <f>IF(K37=M37,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M37" s="3">
@@ -4198,7 +4199,7 @@
         <v>1742353</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>48</v>
       </c>
@@ -4218,21 +4219,21 @@
         <v>110.9</v>
       </c>
       <c r="H38" s="3">
-        <f>IF(ISBLANK(G38),F38,F38/G38)</f>
+        <f t="shared" si="8"/>
         <v>110.9</v>
       </c>
       <c r="I38" s="3">
         <v>110.9</v>
       </c>
       <c r="J38" s="3" t="str">
-        <f>IF(H38=I38,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K38" s="3">
         <v>110.9</v>
       </c>
       <c r="L38" s="3">
-        <f>IF(K38=M38,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M38" s="3">
@@ -4246,7 +4247,7 @@
         <v>110.9</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>53</v>
       </c>
@@ -4269,21 +4270,21 @@
         <v>10</v>
       </c>
       <c r="H39" s="3">
-        <f>IF(ISBLANK(G39),F39,F39/G39)</f>
+        <f t="shared" si="8"/>
         <v>189387.1875</v>
       </c>
       <c r="I39" s="3">
         <v>189387</v>
       </c>
       <c r="J39" s="3">
-        <f>IF(H39=I39,"",1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K39" s="3">
         <v>378774.375</v>
       </c>
       <c r="L39" s="3">
-        <f>IF(K39=M39,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M39" s="3">
@@ -4292,7 +4293,7 @@
       </c>
       <c r="N39" s="3" t="str">
         <f>VLOOKUP(A39,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O39" s="5">
         <f>M39*0.75</f>
@@ -4302,8 +4303,12 @@
         <f>O39*0.75</f>
         <v>181101.498046875</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q39" s="3">
+        <f>C39</f>
+        <v>15150975.09</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>51</v>
       </c>
@@ -4323,21 +4328,21 @@
         <v>4273.9050960000004</v>
       </c>
       <c r="H40" s="3">
-        <f>IF(ISBLANK(G40),F40,F40/G40)</f>
+        <f t="shared" si="8"/>
         <v>4273.9050960000004</v>
       </c>
       <c r="I40" s="3">
         <v>4273.9050960000004</v>
       </c>
       <c r="J40" s="3" t="str">
-        <f>IF(H40=I40,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K40" s="3">
         <v>4273.9050960000004</v>
       </c>
       <c r="L40" s="3">
-        <f>IF(K40=M40,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M40" s="3">
@@ -4351,7 +4356,7 @@
         <v>4273.9050960000004</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>191</v>
       </c>
@@ -4371,21 +4376,21 @@
         <v>0.05</v>
       </c>
       <c r="H41" s="3">
-        <f>IF(ISBLANK(G41),F41,F41/G41)</f>
+        <f t="shared" si="8"/>
         <v>0.05</v>
       </c>
       <c r="I41" s="3">
         <v>0.05</v>
       </c>
       <c r="J41" s="3" t="str">
-        <f>IF(H41=I41,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K41" s="3">
         <v>0.05</v>
       </c>
       <c r="L41" s="3">
-        <f>IF(K41=M41,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M41" s="3">
@@ -4399,7 +4404,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>190</v>
       </c>
@@ -4419,21 +4424,21 @@
         <v>0.05</v>
       </c>
       <c r="H42" s="3">
-        <f>IF(ISBLANK(G42),F42,F42/G42)</f>
+        <f t="shared" si="8"/>
         <v>0.05</v>
       </c>
       <c r="I42" s="3">
         <v>0.05</v>
       </c>
       <c r="J42" s="3" t="str">
-        <f>IF(H42=I42,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K42" s="3">
         <v>0.05</v>
       </c>
       <c r="L42" s="3">
-        <f>IF(K42=M42,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M42" s="3">
@@ -4447,7 +4452,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>20</v>
       </c>
@@ -4467,21 +4472,21 @@
         <v>80210</v>
       </c>
       <c r="H43" s="3">
-        <f>IF(ISBLANK(G43),F43,F43/G43)</f>
+        <f t="shared" si="8"/>
         <v>80210</v>
       </c>
       <c r="I43" s="3">
         <v>80210</v>
       </c>
       <c r="J43" s="3" t="str">
-        <f>IF(H43=I43,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K43" s="3">
         <v>80210</v>
       </c>
       <c r="L43" s="3">
-        <f>IF(K43=M43,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M43" s="3">
@@ -4495,7 +4500,7 @@
         <v>80210</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>56</v>
       </c>
@@ -4515,21 +4520,21 @@
         <v>28898.867849999999</v>
       </c>
       <c r="H44" s="3">
-        <f>IF(ISBLANK(G44),F44,F44/G44)</f>
+        <f t="shared" si="8"/>
         <v>28898.867849999999</v>
       </c>
       <c r="I44" s="3">
         <v>28898.867849999999</v>
       </c>
       <c r="J44" s="3" t="str">
-        <f>IF(H44=I44,"",1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K44" s="3">
         <v>28898.867849999999</v>
       </c>
       <c r="L44" s="3">
-        <f>IF(K44=M44,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M44" s="3">
@@ -4543,7 +4548,7 @@
         <v>28898.867849999999</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>5</v>
       </c>
@@ -4566,7 +4571,7 @@
         <v>4</v>
       </c>
       <c r="H45" s="3">
-        <f>IF(ISBLANK(G45),F45,F45/G45)</f>
+        <f t="shared" si="8"/>
         <v>513186.06624999997</v>
       </c>
       <c r="I45" s="3">
@@ -4579,16 +4584,16 @@
         <v>22700000</v>
       </c>
       <c r="L45" s="3">
-        <f>IF(K45=M45,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M45" s="3">
         <f>K45*0.75</f>
         <v>17025000</v>
       </c>
-      <c r="N45" s="3" t="str">
+      <c r="N45" s="3">
         <f>VLOOKUP(A45,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="O45" s="3">
         <f>M45*0.75</f>
@@ -4599,7 +4604,7 @@
         <v>9576562.5</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
@@ -4619,7 +4624,7 @@
         <v>6221.5131609999999</v>
       </c>
       <c r="H46" s="3">
-        <f>IF(ISBLANK(G46),F46,F46/G46)</f>
+        <f t="shared" si="8"/>
         <v>6221.5131609999999</v>
       </c>
       <c r="I46" s="3">
@@ -4633,7 +4638,7 @@
         <v>6221.5131609999999</v>
       </c>
       <c r="L46" s="3">
-        <f>IF(K46=M46,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M46" s="3">
@@ -4647,7 +4652,7 @@
         <v>6221.5131609999999</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>31</v>
       </c>
@@ -4667,7 +4672,7 @@
         <v>4142428.1669999999</v>
       </c>
       <c r="H47" s="3">
-        <f>IF(ISBLANK(G47),F47,F47/G47)</f>
+        <f t="shared" si="8"/>
         <v>4142428.1669999999</v>
       </c>
       <c r="I47" s="3">
@@ -4681,7 +4686,7 @@
         <v>4142428.1669999999</v>
       </c>
       <c r="L47" s="3">
-        <f>IF(K47=M47,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M47" s="3">
@@ -4696,7 +4701,7 @@
         <v>3521063.9419499999</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>58</v>
       </c>
@@ -4719,7 +4724,7 @@
         <v>2</v>
       </c>
       <c r="H48" s="3">
-        <f>IF(ISBLANK(G48),F48,F48/G48)</f>
+        <f t="shared" si="8"/>
         <v>26.804801994999998</v>
       </c>
       <c r="I48" s="3">
@@ -4733,7 +4738,7 @@
         <v>26.804801994999998</v>
       </c>
       <c r="L48" s="3">
-        <f>IF(K48=M48,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M48" s="3">
@@ -4748,7 +4753,7 @@
         <v>20.10360149625</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>47</v>
       </c>
@@ -4771,7 +4776,7 @@
         <v>15</v>
       </c>
       <c r="H49" s="3">
-        <f>IF(ISBLANK(G49),F49,F49/G49)</f>
+        <f t="shared" si="8"/>
         <v>1113.668496</v>
       </c>
       <c r="I49" s="3">
@@ -4784,7 +4789,7 @@
         <v>100000</v>
       </c>
       <c r="L49" s="3">
-        <f>IF(K49=M49,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M49" s="3">
@@ -4799,7 +4804,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>30</v>
       </c>
@@ -4819,7 +4824,7 @@
         <v>1314922.53</v>
       </c>
       <c r="H50" s="3">
-        <f>IF(ISBLANK(G50),F50,F50/G50)</f>
+        <f t="shared" si="8"/>
         <v>1314922.53</v>
       </c>
       <c r="I50" s="3">
@@ -4832,16 +4837,16 @@
         <v>27400000</v>
       </c>
       <c r="L50" s="3">
-        <f>IF(K50=M50,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M50" s="3">
         <f>K50/10</f>
         <v>2740000</v>
       </c>
-      <c r="N50" s="3" t="str">
+      <c r="N50" s="3">
         <f>VLOOKUP(A50,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="O50" s="5">
         <f>M50*0.75</f>
@@ -4852,7 +4857,7 @@
         <v>15779070.359999999</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>55</v>
       </c>
@@ -4872,7 +4877,7 @@
         <v>357460.29800000001</v>
       </c>
       <c r="H51" s="3">
-        <f>IF(ISBLANK(G51),F51,F51/G51)</f>
+        <f t="shared" si="8"/>
         <v>357460.29800000001</v>
       </c>
       <c r="I51" s="3">
@@ -4886,7 +4891,7 @@
         <v>357460.29800000001</v>
       </c>
       <c r="L51" s="3">
-        <f>IF(K51=M51,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M51" s="3">
@@ -4900,7 +4905,7 @@
         <v>357460.29800000001</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
@@ -4920,7 +4925,7 @@
         <v>2957397.3650000002</v>
       </c>
       <c r="H52" s="3">
-        <f>IF(ISBLANK(G52),F52,F52/G52)</f>
+        <f t="shared" si="8"/>
         <v>2957397.3650000002</v>
       </c>
       <c r="I52" s="3">
@@ -4934,7 +4939,7 @@
         <v>3943196.4866666668</v>
       </c>
       <c r="L52" s="3">
-        <f>IF(K52=M52,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M52" s="3">
@@ -4949,7 +4954,7 @@
         <v>4928995.6083333334</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>28</v>
       </c>
@@ -4972,7 +4977,7 @@
         <v>1.5</v>
       </c>
       <c r="H53" s="3">
-        <f>IF(ISBLANK(G53),F53,F53/G53)</f>
+        <f t="shared" si="8"/>
         <v>48153936</v>
       </c>
       <c r="I53" s="3">
@@ -4986,7 +4991,7 @@
         <v>57784723.200000003</v>
       </c>
       <c r="L53" s="3">
-        <f>IF(K53=M53,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M53" s="3">
@@ -5001,7 +5006,7 @@
         <v>72230904</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>60</v>
       </c>
@@ -5021,7 +5026,7 @@
         <v>7496.955054</v>
       </c>
       <c r="H54" s="3">
-        <f>IF(ISBLANK(G54),F54,F54/G54)</f>
+        <f t="shared" si="8"/>
         <v>7496.955054</v>
       </c>
       <c r="I54" s="3">
@@ -5035,7 +5040,7 @@
         <v>7496.955054</v>
       </c>
       <c r="L54" s="3">
-        <f>IF(K54=M54,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M54" s="3">
@@ -5049,7 +5054,7 @@
         <v>7496.955054</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>33</v>
       </c>
@@ -5069,7 +5074,7 @@
         <v>5700290.8640000001</v>
       </c>
       <c r="H55" s="3">
-        <f>IF(ISBLANK(G55),F55,F55/G55)</f>
+        <f t="shared" si="8"/>
         <v>5700290.8640000001</v>
       </c>
       <c r="I55" s="3">
@@ -5082,7 +5087,7 @@
         <v>134000000</v>
       </c>
       <c r="L55" s="3">
-        <f>IF(K55=M55,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M55" s="3">
@@ -5091,7 +5096,7 @@
       </c>
       <c r="N55" s="3" t="str">
         <f>VLOOKUP(A55,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>--</v>
+        <v>ORIG</v>
       </c>
       <c r="O55" s="3">
         <f>M55/2</f>
@@ -5101,8 +5106,12 @@
         <f>O55*0.75</f>
         <v>25125000</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q55" s="3">
+        <f t="shared" ref="Q55:Q56" si="10">C55</f>
+        <v>5700290.8640000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>46</v>
       </c>
@@ -5125,7 +5134,7 @@
         <v>10</v>
       </c>
       <c r="H56" s="3">
-        <f>IF(ISBLANK(G56),F56,F56/G56)</f>
+        <f t="shared" si="8"/>
         <v>2991.66</v>
       </c>
       <c r="I56" s="3">
@@ -5139,7 +5148,7 @@
         <v>2991.66</v>
       </c>
       <c r="L56" s="3">
-        <f>IF(K56=M56,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M56" s="3">
@@ -5148,7 +5157,7 @@
       </c>
       <c r="N56" s="3" t="str">
         <f>VLOOKUP(A56,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O56" s="3">
         <f>M56*0.75</f>
@@ -5158,8 +5167,12 @@
         <f>O56*0.75</f>
         <v>841.40437499999996</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q56" s="3">
+        <f t="shared" si="10"/>
+        <v>358999.37920000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>38</v>
       </c>
@@ -5182,7 +5195,7 @@
         <v>8</v>
       </c>
       <c r="H57" s="3">
-        <f>IF(ISBLANK(G57),F57,F57/G57)</f>
+        <f t="shared" si="8"/>
         <v>29180.924725000001</v>
       </c>
       <c r="I57" s="3">
@@ -5196,7 +5209,7 @@
         <v>58361.849450000002</v>
       </c>
       <c r="L57" s="3">
-        <f>IF(K57=M57,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M57" s="3">
@@ -5210,7 +5223,7 @@
         <v>58361.849450000002</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>15</v>
       </c>
@@ -5233,7 +5246,7 @@
         <v>7.5</v>
       </c>
       <c r="H58" s="3">
-        <f>IF(ISBLANK(G58),F58,F58/G58)</f>
+        <f t="shared" si="8"/>
         <v>28098.719999999998</v>
       </c>
       <c r="I58" s="3">
@@ -5247,16 +5260,16 @@
         <v>5340000</v>
       </c>
       <c r="L58" s="3">
-        <f>IF(K58=M58,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M58" s="3">
         <f>K58/2</f>
         <v>2670000</v>
       </c>
-      <c r="N58" s="3" t="str">
+      <c r="N58" s="3">
         <f>VLOOKUP(A58,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="O58" s="3">
         <f>M58*0.5</f>
@@ -5267,7 +5280,7 @@
         <v>1001250</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>39</v>
       </c>
@@ -5290,7 +5303,7 @@
         <v>10</v>
       </c>
       <c r="H59" s="3">
-        <f>IF(ISBLANK(G59),F59,F59/G59)</f>
+        <f t="shared" si="8"/>
         <v>17712.940450000002</v>
       </c>
       <c r="I59" s="3">
@@ -5304,7 +5317,7 @@
         <v>35425.880900000004</v>
       </c>
       <c r="L59" s="3">
-        <f>IF(K59=M59,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M59" s="3">
@@ -5313,7 +5326,7 @@
       </c>
       <c r="N59" s="3" t="str">
         <f>VLOOKUP(A59,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>--</v>
+        <v>ORIG</v>
       </c>
       <c r="O59" s="3">
         <f>M59/2</f>
@@ -5323,8 +5336,12 @@
         <f>O59*0.75</f>
         <v>6642.3526687500007</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q59" s="3">
+        <f>C59</f>
+        <v>177129.4045</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>34</v>
       </c>
@@ -5347,7 +5364,7 @@
         <v>0.2</v>
       </c>
       <c r="H60" s="3">
-        <f>IF(ISBLANK(G60),F60,F60/G60)</f>
+        <f t="shared" si="8"/>
         <v>20480</v>
       </c>
       <c r="I60" s="3">
@@ -5361,7 +5378,7 @@
         <v>142000</v>
       </c>
       <c r="L60" s="3">
-        <f>IF(K60=M60,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M60" s="3">
@@ -5381,7 +5398,7 @@
         <v>639000</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>61</v>
       </c>
@@ -5401,7 +5418,7 @@
         <v>71.004761549999998</v>
       </c>
       <c r="H61" s="3">
-        <f>IF(ISBLANK(G61),F61,F61/G61)</f>
+        <f t="shared" si="8"/>
         <v>71.004761549999998</v>
       </c>
       <c r="I61" s="3">
@@ -5415,7 +5432,7 @@
         <v>71.004761549999998</v>
       </c>
       <c r="L61" s="3">
-        <f>IF(K61=M61,1,0)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M61" s="3">
@@ -5429,7 +5446,7 @@
         <v>71.004761549999998</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>12</v>
       </c>
@@ -5452,7 +5469,7 @@
         <v>10</v>
       </c>
       <c r="H62" s="3">
-        <f>IF(ISBLANK(G62),F62,F62/G62)</f>
+        <f t="shared" si="8"/>
         <v>5202018.7369999997</v>
       </c>
       <c r="I62" s="3">
@@ -5466,22 +5483,26 @@
         <v>7530000</v>
       </c>
       <c r="L62" s="3">
-        <f>IF(K62=M62,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M62" s="3">
         <f>K62*0.85</f>
         <v>6400500</v>
       </c>
-      <c r="N62" s="3">
+      <c r="N62" s="3" t="str">
         <f>VLOOKUP(A62,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>ORIG</v>
       </c>
       <c r="O62" s="3">
         <v>6400500</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q62" s="3">
+        <f>C62</f>
+        <v>52020187.369999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>14</v>
       </c>
@@ -5504,7 +5525,7 @@
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <f>IF(ISBLANK(G63),F63,F63/G63)</f>
+        <f t="shared" si="8"/>
         <v>439802.6</v>
       </c>
       <c r="I63" s="3">
@@ -5518,7 +5539,7 @@
         <v>879605.2</v>
       </c>
       <c r="L63" s="3">
-        <f>IF(K63=M63,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M63" s="3">
@@ -5533,7 +5554,7 @@
         <v>747664.41999999993</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>16</v>
       </c>
@@ -5556,7 +5577,7 @@
         <v>15</v>
       </c>
       <c r="H64" s="3">
-        <f>IF(ISBLANK(G64),F64,F64/G64)</f>
+        <f t="shared" si="8"/>
         <v>249251.73559999999</v>
       </c>
       <c r="I64" s="3">
@@ -5570,16 +5591,16 @@
         <v>21600000</v>
       </c>
       <c r="L64" s="3">
-        <f>IF(K64=M64,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M64" s="3">
         <f>K64/1.5</f>
         <v>14400000</v>
       </c>
-      <c r="N64" s="3" t="str">
+      <c r="N64" s="3">
         <f>VLOOKUP(A64,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="O64" s="3">
         <f>M64*0.75</f>
@@ -5590,7 +5611,7 @@
         <v>1080000</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>52</v>
       </c>
@@ -5613,7 +5634,7 @@
         <v>7</v>
       </c>
       <c r="H65" s="3">
-        <f>IF(ISBLANK(G65),F65,F65/G65)</f>
+        <f t="shared" si="8"/>
         <v>42857.142857142855</v>
       </c>
       <c r="I65" s="3">
@@ -5627,7 +5648,7 @@
         <v>42857.142857142855</v>
       </c>
       <c r="L65" s="3">
-        <f>IF(K65=M65,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M65" s="3">
@@ -5636,7 +5657,7 @@
       </c>
       <c r="N65" s="3" t="str">
         <f>VLOOKUP(A65,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O65" s="3">
         <f>M65*0.75</f>
@@ -5646,8 +5667,12 @@
         <f>O65*0.75</f>
         <v>18080.357142857141</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q65" s="3">
+        <f t="shared" ref="Q65:Q66" si="11">C65</f>
+        <v>97071048.260000005</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>17</v>
       </c>
@@ -5667,7 +5692,7 @@
         <v>2026568.5109999999</v>
       </c>
       <c r="H66" s="3">
-        <f>IF(ISBLANK(G66),F66,F66/G66)</f>
+        <f t="shared" si="8"/>
         <v>2026568.5109999999</v>
       </c>
       <c r="I66" s="3">
@@ -5681,7 +5706,7 @@
         <v>2026568.5109999999</v>
       </c>
       <c r="L66" s="3">
-        <f>IF(K66=M66,1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M66" s="3">
@@ -5690,7 +5715,7 @@
       </c>
       <c r="N66" s="3" t="str">
         <f>VLOOKUP(A66,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O66" s="3">
         <f>M66*0.75</f>
@@ -5700,8 +5725,12 @@
         <f>O66*0.75</f>
         <v>968953.06932187499</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q66" s="3">
+        <f t="shared" si="11"/>
+        <v>20265685.109999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>40</v>
       </c>
@@ -5724,7 +5753,7 @@
         <v>10</v>
       </c>
       <c r="H67" s="3">
-        <f>IF(ISBLANK(G67),F67,F67/G67)</f>
+        <f t="shared" ref="H67:H98" si="12">IF(ISBLANK(G67),F67,F67/G67)</f>
         <v>298370.68709999998</v>
       </c>
       <c r="I67" s="3">
@@ -5737,7 +5766,7 @@
         <v>491000</v>
       </c>
       <c r="L67" s="3">
-        <f>IF(K67=M67,1,0)</f>
+        <f t="shared" ref="L67:L98" si="13">IF(K67=M67,1,0)</f>
         <v>1</v>
       </c>
       <c r="M67" s="3">
@@ -5751,7 +5780,7 @@
         <v>491000</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>44</v>
       </c>
@@ -5774,7 +5803,7 @@
         <v>7</v>
       </c>
       <c r="H68" s="3">
-        <f>IF(ISBLANK(G68),F68,F68/G68)</f>
+        <f t="shared" si="12"/>
         <v>2925788</v>
       </c>
       <c r="I68" s="3">
@@ -5787,7 +5816,7 @@
         <v>2925788</v>
       </c>
       <c r="L68" s="3">
-        <f>IF(K68=M68,1,0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M68" s="3">
@@ -5796,7 +5825,7 @@
       </c>
       <c r="N68" s="3" t="str">
         <f>VLOOKUP(A68,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>ORIG</v>
       </c>
       <c r="O68" s="3">
         <f>M68*0.75</f>
@@ -5806,18 +5835,22 @@
         <f>O68*0.75</f>
         <v>1398892.3875</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q68" s="3">
+        <f>C68</f>
+        <v>204805160.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -5825,24 +5858,12 @@
       <c r="E71"/>
       <c r="F71" s="12"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B72"/>
       <c r="C72"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O68">
-    <filterColumn colId="13">
-      <filters>
-        <filter val="-"/>
-        <filter val="--"/>
-        <filter val="---"/>
-        <filter val="+"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A3:O68">
-      <sortCondition ref="A1:A68"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O68"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added old mortality terms - Restored Ryan's ml and mQ terms
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="189">
   <si>
     <t>Too Low</t>
   </si>
@@ -577,30 +577,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>LSQj</t>
-  </si>
-  <si>
-    <t>LSQa</t>
-  </si>
-  <si>
-    <t>ISQj</t>
-  </si>
-  <si>
-    <t>ISQa</t>
-  </si>
-  <si>
-    <t>NSHj</t>
-  </si>
-  <si>
-    <t>NSHa</t>
-  </si>
-  <si>
-    <t>OSHj</t>
-  </si>
-  <si>
-    <t>OSHa</t>
-  </si>
-  <si>
     <t>KDENR_Orig</t>
   </si>
   <si>
@@ -614,6 +590,12 @@
   </si>
   <si>
     <t>Too High Late</t>
+  </si>
+  <si>
+    <t>Change_Instructions</t>
+  </si>
+  <si>
+    <t>ReducePred9_DKENR</t>
   </si>
 </sst>
 </file>
@@ -1015,12 +997,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,10 +1025,10 @@
         <v>179</v>
       </c>
       <c r="C1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1062,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1098,7 +1079,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1110,7 +1091,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1161,7 +1142,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1179,7 +1160,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1175,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1212,7 +1193,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1227,7 +1208,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1242,7 +1223,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1257,7 +1238,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1269,7 +1250,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1320,7 +1301,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1332,7 +1313,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1347,7 +1328,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1362,7 +1343,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1377,7 +1358,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1389,7 +1370,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -1401,7 +1382,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1449,7 +1430,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1464,7 +1445,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1494,7 +1475,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1506,7 +1487,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1536,7 +1517,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1551,7 +1532,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1566,7 +1547,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1584,7 +1565,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1596,7 +1577,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1611,7 +1592,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -1623,7 +1604,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -1638,7 +1619,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -1653,7 +1634,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1665,7 +1646,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1698,7 +1679,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1713,7 +1694,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -1740,7 +1721,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1755,7 +1736,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1770,7 +1751,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -1785,7 +1766,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -1797,7 +1778,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -1827,7 +1808,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1839,7 +1820,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -1851,7 +1832,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -1863,7 +1844,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -1875,7 +1856,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -1887,7 +1868,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -1899,7 +1880,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -1911,7 +1892,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -1923,7 +1904,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -1938,7 +1919,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>30</v>
       </c>
@@ -1953,7 +1934,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -1965,7 +1946,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -1980,7 +1961,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -2010,7 +1991,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -2025,7 +2006,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>54</v>
       </c>
@@ -2037,7 +2018,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2052,7 +2033,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -2064,7 +2045,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -2076,7 +2057,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2091,7 +2072,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>27</v>
       </c>
@@ -2106,7 +2087,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -2154,7 +2135,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -2208,7 +2189,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -2223,7 +2204,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>60</v>
       </c>
@@ -2235,7 +2216,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -2247,7 +2228,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2262,7 +2243,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -2310,7 +2291,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -2341,29 +2322,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I88">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I88"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P72"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2371,12 +2344,12 @@
     <col min="1" max="1" width="8.88671875" style="3"/>
     <col min="2" max="2" width="17.21875" style="3" customWidth="1"/>
     <col min="3" max="3" width="27.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" style="3" customWidth="1"/>
@@ -2396,10 +2369,16 @@
         <v>181</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2412,11 +2391,17 @@
       <c r="C2" s="7">
         <v>1001094433</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="7" t="str">
+        <f>IF(VLOOKUP(A2,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E2" s="6">
+        <v>45700000</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -2426,14 +2411,20 @@
       <c r="C3" s="7">
         <v>2124041.1490000002</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="11"/>
+      <c r="D3" s="7" t="str">
+        <f>IF(VLOOKUP(A3,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E3" s="6">
+        <v>2124041.1490000002</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="11"/>
       <c r="K3" s="5"/>
       <c r="M3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2443,11 +2434,17 @@
       <c r="C4" s="7">
         <v>114181041.2</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="7" t="str">
+        <f>IF(VLOOKUP(A4,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E4" s="6">
+        <v>19030174.25</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -2457,9 +2454,15 @@
       <c r="C5" s="7">
         <v>15816.31169</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="7" t="str">
+        <f>IF(VLOOKUP(A5,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E5" s="6">
+        <v>175816.31169</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
@@ -2471,9 +2474,15 @@
       <c r="C6" s="7">
         <v>1718757.3940000001</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="7" t="str">
+        <f>IF(VLOOKUP(A6,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1718757.3940000001</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
@@ -2485,13 +2494,19 @@
       <c r="C7" s="7">
         <v>16477555.609999999</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="11"/>
+      <c r="D7" s="7" t="str">
+        <f>IF(VLOOKUP(A7,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E7" s="6">
+        <v>993066.96089999995</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="11"/>
       <c r="K7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -2501,11 +2516,17 @@
       <c r="C8" s="8">
         <v>229000000000</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="7" t="str">
+        <f>IF(VLOOKUP(A8,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E8" s="6">
+        <v>2000000000000</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -2515,14 +2536,20 @@
       <c r="C9" s="7">
         <v>32122718.550000001</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11"/>
+      <c r="D9" s="7" t="str">
+        <f>IF(VLOOKUP(A9,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E9" s="6">
+        <v>321227180.55000001</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="11"/>
       <c r="K9" s="11"/>
       <c r="M9" s="11"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
@@ -2532,11 +2559,17 @@
       <c r="C10" s="7">
         <v>2123.8950410000002</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="7" t="str">
+        <f>IF(VLOOKUP(A10,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E10" s="6">
+        <v>2123.8950410000002</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
@@ -2546,14 +2579,20 @@
       <c r="C11" s="7">
         <v>74822.192989999996</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="11"/>
+      <c r="D11" s="7" t="str">
+        <f>IF(VLOOKUP(A11,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E11" s="6">
+        <v>74822.192989999996</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="11"/>
       <c r="K11" s="11"/>
       <c r="M11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>58</v>
       </c>
@@ -2563,9 +2602,15 @@
       <c r="C12" s="7">
         <v>235.45910710000001</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="11"/>
+      <c r="D12" s="7" t="str">
+        <f>IF(VLOOKUP(A12,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E12" s="6">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
@@ -2577,9 +2622,15 @@
       <c r="C13" s="7">
         <v>25797.24295</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="11"/>
+      <c r="D13" s="7" t="str">
+        <f>IF(VLOOKUP(A13,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E13" s="6">
+        <v>100</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -2591,11 +2642,17 @@
       <c r="C14" s="7">
         <v>352590040.69999999</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="7" t="str">
+        <f>IF(VLOOKUP(A14,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E14" s="6">
+        <v>176000000</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>48</v>
       </c>
@@ -2605,9 +2662,15 @@
       <c r="C15" s="7">
         <v>15874.27808</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="11"/>
+      <c r="D15" s="7" t="str">
+        <f>IF(VLOOKUP(A15,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E15" s="6">
+        <v>15874.27808</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
@@ -2619,14 +2682,20 @@
       <c r="C16" s="7">
         <v>129309.07709999999</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="11"/>
+      <c r="D16" s="7" t="str">
+        <f>IF(VLOOKUP(A16,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E16" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="11"/>
       <c r="M16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>22</v>
       </c>
@@ -2636,9 +2705,15 @@
       <c r="C17" s="7">
         <v>21996106.07</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="11"/>
+      <c r="D17" s="7" t="str">
+        <f>IF(VLOOKUP(A17,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E17" s="6">
+        <v>4000000</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="11"/>
       <c r="K17" s="5"/>
       <c r="M17" s="5"/>
       <c r="O17" s="5"/>
@@ -2653,9 +2728,15 @@
       <c r="C18" s="7">
         <v>17230050.359999999</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="11"/>
+      <c r="D18" s="7" t="str">
+        <f>IF(VLOOKUP(A18,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E18" s="6">
+        <v>8500000</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="11"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
@@ -2669,9 +2750,15 @@
       <c r="C19" s="7">
         <v>13236869.029999999</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="11"/>
+      <c r="D19" s="7" t="str">
+        <f>IF(VLOOKUP(A19,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E19" s="6">
+        <v>6500000</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="11"/>
       <c r="M19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
@@ -2686,15 +2773,21 @@
       <c r="C20" s="7">
         <v>432544359.30000001</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="7" t="str">
+        <f>IF(VLOOKUP(A20,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E20" s="6">
+        <v>2430000</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="11"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>185</v>
+        <v>63</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>152</v>
@@ -2702,702 +2795,930 @@
       <c r="C21" s="7">
         <v>0.05</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="7" t="str">
+        <f>IF(VLOOKUP(A21,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E21" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C22" s="7">
+        <v>747577.53830000001</v>
+      </c>
+      <c r="D22" s="7" t="str">
+        <f>IF(VLOOKUP(A22,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E22" s="6">
+        <v>197000</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="7">
+        <v>172649603.19999999</v>
+      </c>
+      <c r="D23" s="7" t="str">
+        <f>IF(VLOOKUP(A23,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E23" s="6">
+        <v>49700000</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="11"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="7">
         <v>0.05</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="7">
-        <v>747577.53830000001</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="11"/>
-      <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="7">
-        <v>172649603.19999999</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="11"/>
+      <c r="D24" s="7" t="str">
+        <f>IF(VLOOKUP(A24,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E24" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="11"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>183</v>
+        <v>10</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>151</v>
+        <v>92</v>
       </c>
       <c r="C25" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>932233758.39999998</v>
+      </c>
+      <c r="D25" s="7" t="str">
+        <f>IF(VLOOKUP(A25,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E25" s="6">
+        <v>532233758.39999998</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>182</v>
+        <v>56</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C26" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>749.83099549999997</v>
+      </c>
+      <c r="D26" s="7" t="str">
+        <f>IF(VLOOKUP(A26,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E26" s="6">
+        <v>100</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C27" s="7">
-        <v>932233758.39999998</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4986608.142</v>
+      </c>
+      <c r="D27" s="7" t="str">
+        <f>IF(VLOOKUP(A27,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E27" s="6">
+        <v>4986608.142</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C28" s="7">
-        <v>749.83099549999997</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="11"/>
+        <v>174418341.5</v>
+      </c>
+      <c r="D28" s="7" t="str">
+        <f>IF(VLOOKUP(A28,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E28" s="6">
+        <v>7850000</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C29" s="7">
-        <v>4986608.142</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>254421.22440000001</v>
+      </c>
+      <c r="D29" s="7" t="str">
+        <f>IF(VLOOKUP(A29,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E29" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="C30" s="7">
-        <v>174418341.5</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="11"/>
+        <v>4108787.665</v>
+      </c>
+      <c r="D30" s="7" t="str">
+        <f>IF(VLOOKUP(A30,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E30" s="6">
+        <v>328703</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="11"/>
       <c r="O30" s="5"/>
     </row>
-    <row r="31" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="C31" s="7">
-        <v>254421.22440000001</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="11"/>
+        <v>0.05</v>
+      </c>
+      <c r="D31" s="7" t="str">
+        <f>IF(VLOOKUP(A31,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E31" s="6">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="11"/>
       <c r="P31" s="5"/>
     </row>
     <row r="32" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C32" s="7">
-        <v>4108787.665</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>22940055.34</v>
+      </c>
+      <c r="D32" s="7" t="str">
+        <f>IF(VLOOKUP(A32,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E32" s="6">
+        <v>22940055.34</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
-        <v>187</v>
+        <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="C33" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19201175.25</v>
+      </c>
+      <c r="D33" s="7" t="str">
+        <f>IF(VLOOKUP(A33,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E33" s="6">
+        <v>49069.656669999997</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
-        <v>186</v>
+        <v>23</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="C34" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="11"/>
-    </row>
-    <row r="35" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34847060.600000001</v>
+      </c>
+      <c r="D34" s="7" t="str">
+        <f>IF(VLOOKUP(A34,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E34" s="6">
+        <v>1742353</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C35" s="7">
-        <v>22940055.34</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="11"/>
+        <v>554.64984700000002</v>
+      </c>
+      <c r="D35" s="7" t="str">
+        <f>IF(VLOOKUP(A35,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E35" s="6">
+        <v>110.9</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="C36" s="7">
-        <v>19201175.25</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15150975.09</v>
+      </c>
+      <c r="D36" s="7" t="str">
+        <f>IF(VLOOKUP(A36,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E36" s="6">
+        <v>15150975.09</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C37" s="7">
-        <v>34847060.600000001</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4273.9050960000004</v>
+      </c>
+      <c r="D37" s="7" t="str">
+        <f>IF(VLOOKUP(A37,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E37" s="6">
+        <v>4273.9050960000004</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="C38" s="7">
-        <v>554.64984700000002</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.05</v>
+      </c>
+      <c r="D38" s="7" t="str">
+        <f>IF(VLOOKUP(A38,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E38" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C39" s="7">
-        <v>15150975.09</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="11"/>
+        <v>401050.08909999998</v>
+      </c>
+      <c r="D39" s="7" t="str">
+        <f>IF(VLOOKUP(A39,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E39" s="6">
+        <v>201050.08910000001</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="11"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C40" s="7">
-        <v>4273.9050960000004</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="11"/>
+        <v>28898.867849999999</v>
+      </c>
+      <c r="D40" s="7" t="str">
+        <f>IF(VLOOKUP(A40,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E40" s="6">
+        <v>28898.867849999999</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
-        <v>189</v>
+        <v>4</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>162</v>
+        <v>102</v>
       </c>
       <c r="C41" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="11"/>
-    </row>
-    <row r="42" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20527442.649999999</v>
+      </c>
+      <c r="D41" s="7" t="str">
+        <f>IF(VLOOKUP(A41,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E41" s="6">
+        <v>6384375</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>188</v>
+        <v>49</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C42" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6221.5131609999999</v>
+      </c>
+      <c r="D42" s="7" t="str">
+        <f>IF(VLOOKUP(A42,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E42" s="6">
+        <v>6221.5131609999999</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C43" s="7">
-        <v>401050.08909999998</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="11"/>
-    </row>
-    <row r="44" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24854569.199999999</v>
+      </c>
+      <c r="D43" s="7" t="str">
+        <f>IF(VLOOKUP(A43,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E43" s="6">
+        <v>3521063.9419999998</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C44" s="7">
-        <v>28898.867849999999</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="11"/>
-    </row>
-    <row r="45" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53.609603989999997</v>
+      </c>
+      <c r="D44" s="7" t="str">
+        <f>IF(VLOOKUP(A44,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E44" s="6">
+        <v>20</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="C45" s="7">
-        <v>20527442.649999999</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="11"/>
+        <v>16705.027440000002</v>
+      </c>
+      <c r="D45" s="7" t="str">
+        <f>IF(VLOOKUP(A45,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E45" s="6">
+        <v>75000</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="11"/>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C46" s="7">
-        <v>6221.5131609999999</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="11"/>
-    </row>
-    <row r="47" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15779070.359999999</v>
+      </c>
+      <c r="D46" s="7" t="str">
+        <f>IF(VLOOKUP(A46,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E46" s="6">
+        <v>1540000</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C47" s="7">
-        <v>24854569.199999999</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="11"/>
-    </row>
-    <row r="48" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10723808.939999999</v>
+      </c>
+      <c r="D47" s="7" t="str">
+        <f>IF(VLOOKUP(A47,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E47" s="6">
+        <v>357460.29800000001</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="C48" s="7">
-        <v>53.609603989999997</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="11"/>
-    </row>
-    <row r="49" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2957397.3650000002</v>
+      </c>
+      <c r="D48" s="7" t="str">
+        <f>IF(VLOOKUP(A48,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E48" s="6">
+        <v>4928995.608</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C49" s="7">
-        <v>16705.027440000002</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="11"/>
-    </row>
-    <row r="50" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>361154520.60000002</v>
+      </c>
+      <c r="D49" s="7" t="str">
+        <f>IF(VLOOKUP(A49,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E49" s="6">
+        <v>72230904</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C50" s="7">
-        <v>15779070.359999999</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="11"/>
+        <v>7496.955054</v>
+      </c>
+      <c r="D50" s="7" t="str">
+        <f>IF(VLOOKUP(A50,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E50" s="6">
+        <v>7496.955054</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="11"/>
       <c r="O50" s="5"/>
     </row>
     <row r="51" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C51" s="7">
-        <v>10723808.939999999</v>
-      </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="11"/>
+        <v>5700290.8640000001</v>
+      </c>
+      <c r="D51" s="7" t="str">
+        <f>IF(VLOOKUP(A51,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E51" s="6">
+        <v>5700290.8640000001</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="C52" s="7">
-        <v>2957397.3650000002</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="11"/>
-    </row>
-    <row r="53" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>358999.37920000002</v>
+      </c>
+      <c r="D52" s="7" t="str">
+        <f>IF(VLOOKUP(A52,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E52" s="6">
+        <v>250000</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C53" s="7">
-        <v>361154520.60000002</v>
-      </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="11"/>
+        <v>233447.39780000001</v>
+      </c>
+      <c r="D53" s="7" t="str">
+        <f>IF(VLOOKUP(A53,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E53" s="6">
+        <v>58361.849450000002</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
       <c r="C54" s="7">
-        <v>7496.955054</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="11"/>
+        <v>1053704.304</v>
+      </c>
+      <c r="D54" s="7" t="str">
+        <f>IF(VLOOKUP(A54,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E54" s="6">
+        <v>1001250</v>
+      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C55" s="7">
-        <v>5700290.8640000001</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="11"/>
-    </row>
-    <row r="56" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>177129.4045</v>
+      </c>
+      <c r="D55" s="7" t="str">
+        <f>IF(VLOOKUP(A55,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E55" s="6">
+        <v>125000</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C56" s="7">
-        <v>358999.37920000002</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="9"/>
-    </row>
-    <row r="57" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>40960.04507</v>
+      </c>
+      <c r="D56" s="7" t="str">
+        <f>IF(VLOOKUP(A56,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E56" s="6">
+        <v>639000</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="9"/>
+    </row>
+    <row r="57" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="C57" s="7">
-        <v>233447.39780000001</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="11"/>
-    </row>
-    <row r="58" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>71.004761549999998</v>
+      </c>
+      <c r="D57" s="7" t="str">
+        <f>IF(VLOOKUP(A57,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E57" s="6">
+        <v>71.004761549999998</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C58" s="7">
-        <v>1053704.304</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="11"/>
-    </row>
-    <row r="59" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>52020187.369999997</v>
+      </c>
+      <c r="D58" s="7" t="str">
+        <f>IF(VLOOKUP(A58,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E58" s="6">
+        <v>52020187.369999997</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="C59" s="7">
-        <v>177129.4045</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="11"/>
-    </row>
-    <row r="60" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14975339.800000001</v>
+      </c>
+      <c r="D59" s="7" t="str">
+        <f>IF(VLOOKUP(A59,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E59" s="6">
+        <v>747664.42</v>
+      </c>
+      <c r="F59" s="6"/>
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="C60" s="7">
-        <v>40960.04507</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="11"/>
+        <v>3738776.034</v>
+      </c>
+      <c r="D60" s="7" t="str">
+        <f>IF(VLOOKUP(A60,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E60" s="6">
+        <v>1080000</v>
+      </c>
+      <c r="F60" s="6"/>
+      <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C61" s="7">
-        <v>71.004761549999998</v>
-      </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="11"/>
+        <v>97071048.260000005</v>
+      </c>
+      <c r="D61" s="7" t="str">
+        <f>IF(VLOOKUP(A61,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E61" s="6">
+        <v>60071048.259999998</v>
+      </c>
+      <c r="F61" s="6"/>
+      <c r="G61" s="11"/>
     </row>
     <row r="62" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C62" s="7">
-        <v>52020187.369999997</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="11"/>
-    </row>
-    <row r="63" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20265685.109999999</v>
+      </c>
+      <c r="D62" s="7" t="str">
+        <f>IF(VLOOKUP(A62,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E62" s="6">
+        <v>10265685.109999999</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="C63" s="7">
-        <v>14975339.800000001</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="11"/>
+        <v>2983706.8709999998</v>
+      </c>
+      <c r="D63" s="7" t="str">
+        <f>IF(VLOOKUP(A63,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v/>
+      </c>
+      <c r="E63" s="6">
+        <v>491000</v>
+      </c>
+      <c r="F63" s="6"/>
+      <c r="G63" s="11"/>
     </row>
     <row r="64" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="C64" s="7">
-        <v>3738776.034</v>
-      </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="11"/>
-    </row>
-    <row r="65" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C65" s="7">
-        <v>97071048.260000005</v>
-      </c>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="11"/>
-    </row>
-    <row r="66" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" s="7">
-        <v>20265685.109999999</v>
-      </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="11"/>
-    </row>
-    <row r="67" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C67" s="7">
-        <v>2983706.8709999998</v>
-      </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="11"/>
-    </row>
-    <row r="68" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68" s="7">
         <v>204805160.5</v>
       </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="11"/>
-    </row>
-    <row r="69" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="1"/>
-      <c r="B69"/>
-      <c r="C69"/>
-    </row>
-    <row r="70" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="1"/>
-      <c r="B70"/>
-      <c r="C70"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="2"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71" s="12"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B72"/>
-      <c r="C72"/>
+      <c r="D64" s="7" t="str">
+        <f>IF(VLOOKUP(A64,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <v>-</v>
+      </c>
+      <c r="E64" s="6">
+        <v>150805160.5</v>
+      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1"/>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="11"/>
+    </row>
+    <row r="66" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1"/>
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="2"/>
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="11"/>
+    </row>
+    <row r="68" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="11"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F71"/>
+      <c r="G71" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O68"/>
+  <autoFilter ref="A1:O68">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ReducePred 9 - Decrease squid recruitment - Increase marine mammal/ TYL recruitment - Reduce additional pred group recruitment
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Group Condition" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="193">
   <si>
     <t>Too Low</t>
   </si>
@@ -596,6 +596,18 @@
   </si>
   <si>
     <t>ReducePred9_DKENR</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ORIG</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -997,11 +1009,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,40 +1059,37 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>122</v>
       </c>
-      <c r="C2" t="s">
-        <v>180</v>
+      <c r="G2" t="s">
+        <v>189</v>
       </c>
       <c r="H2" t="str">
         <f>IF(COUNTIF(C2:G2,"X")=0,"X","")</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>102</v>
       </c>
-      <c r="C3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" t="s">
-        <v>180</v>
-      </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">IF(COUNTIF(C3:G3,"X")=0,"X","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1091,7 +1101,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1109,19 +1119,16 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>114</v>
       </c>
-      <c r="C6" t="s">
-        <v>180</v>
-      </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1141,26 +1148,23 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>93</v>
       </c>
-      <c r="F8" t="s">
-        <v>180</v>
-      </c>
-      <c r="G8" t="s">
-        <v>180</v>
-      </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1175,16 +1179,13 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>124</v>
       </c>
-      <c r="F10" t="s">
-        <v>180</v>
-      </c>
       <c r="G10" t="s">
         <v>180</v>
       </c>
@@ -1193,7 +1194,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1223,22 +1224,19 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>147</v>
       </c>
-      <c r="D13" t="s">
-        <v>180</v>
-      </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1250,7 +1248,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1265,25 +1263,19 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>106</v>
       </c>
-      <c r="C16" t="s">
-        <v>180</v>
-      </c>
-      <c r="F16" t="s">
-        <v>180</v>
-      </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1300,8 +1292,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1313,7 +1308,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1323,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1343,7 +1338,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1357,8 +1352,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1370,7 +1368,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -1382,7 +1380,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1394,7 +1392,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1411,26 +1409,23 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>100</v>
       </c>
-      <c r="C26" t="s">
-        <v>180</v>
-      </c>
-      <c r="D26" t="s">
-        <v>180</v>
-      </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1445,7 +1440,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1452,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1474,8 +1469,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1487,7 +1485,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1499,25 +1497,19 @@
         <v>X</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>52</v>
       </c>
       <c r="B32" t="s">
         <v>141</v>
       </c>
-      <c r="C32" t="s">
-        <v>180</v>
-      </c>
-      <c r="D32" t="s">
-        <v>180</v>
-      </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1532,7 +1524,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1546,8 +1538,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1565,7 +1560,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1577,22 +1572,19 @@
         <v>X</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
       <c r="B37" t="s">
         <v>145</v>
       </c>
-      <c r="D37" t="s">
-        <v>180</v>
-      </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -1604,7 +1596,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -1618,8 +1610,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -1633,8 +1628,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1646,7 +1644,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1661,16 +1659,13 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43" t="s">
         <v>111</v>
       </c>
-      <c r="C43" t="s">
-        <v>180</v>
-      </c>
       <c r="G43" t="s">
         <v>180</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1694,7 +1689,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -1706,22 +1701,19 @@
         <v>X</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>34</v>
       </c>
       <c r="B46" t="s">
         <v>123</v>
       </c>
-      <c r="C46" t="s">
-        <v>180</v>
-      </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1736,7 +1728,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1751,7 +1743,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -1766,7 +1758,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -1778,7 +1770,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -1790,25 +1782,19 @@
         <v>X</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>18</v>
       </c>
       <c r="B52" t="s">
         <v>103</v>
       </c>
-      <c r="C52" t="s">
-        <v>180</v>
-      </c>
-      <c r="D52" t="s">
-        <v>180</v>
-      </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1820,7 +1806,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -1832,7 +1818,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -1844,7 +1830,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -1856,7 +1842,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -1868,7 +1854,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -1880,7 +1866,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -1892,7 +1878,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -1904,7 +1890,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -1919,7 +1905,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>30</v>
       </c>
@@ -1934,7 +1920,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -1946,22 +1932,19 @@
         <v>X</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
       <c r="B64" t="s">
         <v>146</v>
       </c>
-      <c r="D64" t="s">
-        <v>180</v>
-      </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -1973,16 +1956,13 @@
         <v>X</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>32</v>
       </c>
       <c r="B66" t="s">
         <v>120</v>
       </c>
-      <c r="C66" t="s">
-        <v>180</v>
-      </c>
       <c r="G66" t="s">
         <v>180</v>
       </c>
@@ -1991,7 +1971,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -2006,7 +1986,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>54</v>
       </c>
@@ -2018,7 +1998,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2033,7 +2013,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -2045,7 +2025,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -2057,7 +2037,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2072,7 +2052,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>27</v>
       </c>
@@ -2087,7 +2067,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -2098,8 +2078,11 @@
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>45</v>
       </c>
@@ -2116,8 +2099,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>44</v>
       </c>
@@ -2134,8 +2120,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -2150,7 +2139,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -2167,8 +2156,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I78" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>38</v>
       </c>
@@ -2188,8 +2180,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -2203,8 +2198,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>60</v>
       </c>
@@ -2216,7 +2214,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -2228,7 +2226,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2243,7 +2241,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -2255,43 +2253,31 @@
         <v>X</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>51</v>
       </c>
       <c r="B85" t="s">
         <v>140</v>
       </c>
-      <c r="C85" t="s">
-        <v>180</v>
-      </c>
-      <c r="D85" t="s">
-        <v>180</v>
-      </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
       <c r="B86" t="s">
         <v>99</v>
       </c>
-      <c r="C86" t="s">
-        <v>180</v>
-      </c>
-      <c r="D86" t="s">
-        <v>180</v>
-      </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -2303,26 +2289,26 @@
         <v>X</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>43</v>
       </c>
       <c r="B88" t="s">
         <v>132</v>
       </c>
-      <c r="C88" t="s">
-        <v>180</v>
-      </c>
-      <c r="D88" t="s">
-        <v>180</v>
-      </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I88"/>
+  <autoFilter ref="A1:I88">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2332,11 +2318,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2392,13 +2378,15 @@
         <v>1001094433</v>
       </c>
       <c r="D2" s="7" t="str">
-        <f>IF(VLOOKUP(A2,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+        <f>VLOOKUP(A2,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+</v>
       </c>
       <c r="E2" s="6">
         <v>45700000</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="7">
+        <v>1001094433</v>
+      </c>
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2411,9 +2399,9 @@
       <c r="C3" s="7">
         <v>2124041.1490000002</v>
       </c>
-      <c r="D3" s="7" t="str">
-        <f>IF(VLOOKUP(A3,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D3" s="7">
+        <f>VLOOKUP(A3,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E3" s="6">
         <v>2124041.1490000002</v>
@@ -2434,9 +2422,9 @@
       <c r="C4" s="7">
         <v>114181041.2</v>
       </c>
-      <c r="D4" s="7" t="str">
-        <f>IF(VLOOKUP(A4,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D4" s="7">
+        <f>VLOOKUP(A4,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E4" s="6">
         <v>19030174.25</v>
@@ -2454,9 +2442,9 @@
       <c r="C5" s="7">
         <v>15816.31169</v>
       </c>
-      <c r="D5" s="7" t="str">
-        <f>IF(VLOOKUP(A5,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D5" s="7">
+        <f>VLOOKUP(A5,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E5" s="6">
         <v>175816.31169</v>
@@ -2475,16 +2463,19 @@
         <v>1718757.3940000001</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f>IF(VLOOKUP(A6,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A6,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E6" s="6">
         <v>1718757.3940000001</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6">
+        <f>E6*0.5</f>
+        <v>859378.69700000004</v>
+      </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -2494,9 +2485,9 @@
       <c r="C7" s="7">
         <v>16477555.609999999</v>
       </c>
-      <c r="D7" s="7" t="str">
-        <f>IF(VLOOKUP(A7,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D7" s="7">
+        <f>VLOOKUP(A7,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E7" s="6">
         <v>993066.96089999995</v>
@@ -2516,9 +2507,9 @@
       <c r="C8" s="8">
         <v>229000000000</v>
       </c>
-      <c r="D8" s="7" t="str">
-        <f>IF(VLOOKUP(A8,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D8" s="7">
+        <f>VLOOKUP(A8,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E8" s="6">
         <v>2000000000000</v>
@@ -2536,9 +2527,9 @@
       <c r="C9" s="7">
         <v>32122718.550000001</v>
       </c>
-      <c r="D9" s="7" t="str">
-        <f>IF(VLOOKUP(A9,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D9" s="7">
+        <f>VLOOKUP(A9,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E9" s="6">
         <v>321227180.55000001</v>
@@ -2559,9 +2550,9 @@
       <c r="C10" s="7">
         <v>2123.8950410000002</v>
       </c>
-      <c r="D10" s="7" t="str">
-        <f>IF(VLOOKUP(A10,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D10" s="7">
+        <f>VLOOKUP(A10,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E10" s="6">
         <v>2123.8950410000002</v>
@@ -2579,9 +2570,9 @@
       <c r="C11" s="7">
         <v>74822.192989999996</v>
       </c>
-      <c r="D11" s="7" t="str">
-        <f>IF(VLOOKUP(A11,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D11" s="7">
+        <f>VLOOKUP(A11,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E11" s="6">
         <v>74822.192989999996</v>
@@ -2602,9 +2593,9 @@
       <c r="C12" s="7">
         <v>235.45910710000001</v>
       </c>
-      <c r="D12" s="7" t="str">
-        <f>IF(VLOOKUP(A12,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D12" s="7">
+        <f>VLOOKUP(A12,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E12" s="6">
         <v>10</v>
@@ -2612,7 +2603,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
@@ -2622,9 +2613,9 @@
       <c r="C13" s="7">
         <v>25797.24295</v>
       </c>
-      <c r="D13" s="7" t="str">
-        <f>IF(VLOOKUP(A13,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D13" s="7">
+        <f>VLOOKUP(A13,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E13" s="6">
         <v>100</v>
@@ -2643,13 +2634,16 @@
         <v>352590040.69999999</v>
       </c>
       <c r="D14" s="7" t="str">
-        <f>IF(VLOOKUP(A14,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A14,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E14" s="6">
         <v>176000000</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="7">
+        <f>E14*0.75</f>
+        <v>132000000</v>
+      </c>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2662,9 +2656,9 @@
       <c r="C15" s="7">
         <v>15874.27808</v>
       </c>
-      <c r="D15" s="7" t="str">
-        <f>IF(VLOOKUP(A15,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D15" s="7">
+        <f>VLOOKUP(A15,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E15" s="6">
         <v>15874.27808</v>
@@ -2683,13 +2677,16 @@
         <v>129309.07709999999</v>
       </c>
       <c r="D16" s="7" t="str">
-        <f>IF(VLOOKUP(A16,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A16,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E16" s="6">
         <v>100000</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6">
+        <f>E16*0.75</f>
+        <v>75000</v>
+      </c>
       <c r="G16" s="11"/>
       <c r="M16" s="5"/>
       <c r="O16" s="5"/>
@@ -2705,9 +2702,9 @@
       <c r="C17" s="7">
         <v>21996106.07</v>
       </c>
-      <c r="D17" s="7" t="str">
-        <f>IF(VLOOKUP(A17,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D17" s="7">
+        <f>VLOOKUP(A17,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E17" s="6">
         <v>4000000</v>
@@ -2718,7 +2715,7 @@
       <c r="M17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -2728,9 +2725,9 @@
       <c r="C18" s="7">
         <v>17230050.359999999</v>
       </c>
-      <c r="D18" s="7" t="str">
-        <f>IF(VLOOKUP(A18,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D18" s="7">
+        <f>VLOOKUP(A18,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E18" s="6">
         <v>8500000</v>
@@ -2740,7 +2737,7 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
@@ -2750,9 +2747,9 @@
       <c r="C19" s="7">
         <v>13236869.029999999</v>
       </c>
-      <c r="D19" s="7" t="str">
-        <f>IF(VLOOKUP(A19,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D19" s="7">
+        <f>VLOOKUP(A19,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E19" s="6">
         <v>6500000</v>
@@ -2763,7 +2760,7 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -2773,9 +2770,9 @@
       <c r="C20" s="7">
         <v>432544359.30000001</v>
       </c>
-      <c r="D20" s="7" t="str">
-        <f>IF(VLOOKUP(A20,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D20" s="7">
+        <f>VLOOKUP(A20,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E20" s="6">
         <v>2430000</v>
@@ -2796,13 +2793,16 @@
         <v>0.05</v>
       </c>
       <c r="D21" s="7" t="str">
-        <f>IF(VLOOKUP(A21,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A21,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E21" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="6">
+        <f>0.02</f>
+        <v>0.02</v>
+      </c>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2815,9 +2815,9 @@
       <c r="C22" s="7">
         <v>747577.53830000001</v>
       </c>
-      <c r="D22" s="7" t="str">
-        <f>IF(VLOOKUP(A22,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D22" s="7">
+        <f>VLOOKUP(A22,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E22" s="6">
         <v>197000</v>
@@ -2835,9 +2835,9 @@
       <c r="C23" s="7">
         <v>172649603.19999999</v>
       </c>
-      <c r="D23" s="7" t="str">
-        <f>IF(VLOOKUP(A23,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D23" s="7">
+        <f>VLOOKUP(A23,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E23" s="6">
         <v>49700000</v>
@@ -2846,7 +2846,7 @@
       <c r="G23" s="11"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>62</v>
       </c>
@@ -2857,13 +2857,15 @@
         <v>0.05</v>
       </c>
       <c r="D24" s="7" t="str">
-        <f>IF(VLOOKUP(A24,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+        <f>VLOOKUP(A24,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-</v>
       </c>
       <c r="E24" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="6">
+        <v>0.02</v>
+      </c>
       <c r="G24" s="11"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
@@ -2878,9 +2880,9 @@
       <c r="C25" s="7">
         <v>932233758.39999998</v>
       </c>
-      <c r="D25" s="7" t="str">
-        <f>IF(VLOOKUP(A25,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D25" s="7">
+        <f>VLOOKUP(A25,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E25" s="6">
         <v>532233758.39999998</v>
@@ -2898,9 +2900,9 @@
       <c r="C26" s="7">
         <v>749.83099549999997</v>
       </c>
-      <c r="D26" s="7" t="str">
-        <f>IF(VLOOKUP(A26,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D26" s="7">
+        <f>VLOOKUP(A26,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E26" s="6">
         <v>100</v>
@@ -2918,9 +2920,9 @@
       <c r="C27" s="7">
         <v>4986608.142</v>
       </c>
-      <c r="D27" s="7" t="str">
-        <f>IF(VLOOKUP(A27,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D27" s="7">
+        <f>VLOOKUP(A27,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E27" s="6">
         <v>4986608.142</v>
@@ -2938,9 +2940,9 @@
       <c r="C28" s="7">
         <v>174418341.5</v>
       </c>
-      <c r="D28" s="7" t="str">
-        <f>IF(VLOOKUP(A28,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D28" s="7">
+        <f>VLOOKUP(A28,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E28" s="6">
         <v>7850000</v>
@@ -2959,13 +2961,15 @@
         <v>254421.22440000001</v>
       </c>
       <c r="D29" s="7" t="str">
-        <f>IF(VLOOKUP(A29,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A29,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E29" s="6">
         <v>150000</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="6">
+        <v>100000</v>
+      </c>
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2978,9 +2982,9 @@
       <c r="C30" s="7">
         <v>4108787.665</v>
       </c>
-      <c r="D30" s="7" t="str">
-        <f>IF(VLOOKUP(A30,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D30" s="7">
+        <f>VLOOKUP(A30,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E30" s="6">
         <v>328703</v>
@@ -2999,9 +3003,9 @@
       <c r="C31" s="7">
         <v>0.05</v>
       </c>
-      <c r="D31" s="7" t="str">
-        <f>IF(VLOOKUP(A31,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D31" s="7">
+        <f>VLOOKUP(A31,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E31" s="6">
         <v>1.2500000000000001E-2</v>
@@ -3010,7 +3014,7 @@
       <c r="G31" s="11"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>34</v>
       </c>
@@ -3020,9 +3024,9 @@
       <c r="C32" s="7">
         <v>22940055.34</v>
       </c>
-      <c r="D32" s="7" t="str">
-        <f>IF(VLOOKUP(A32,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D32" s="7">
+        <f>VLOOKUP(A32,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E32" s="6">
         <v>22940055.34</v>
@@ -3040,9 +3044,9 @@
       <c r="C33" s="7">
         <v>19201175.25</v>
       </c>
-      <c r="D33" s="7" t="str">
-        <f>IF(VLOOKUP(A33,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D33" s="7">
+        <f>VLOOKUP(A33,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E33" s="6">
         <v>49069.656669999997</v>
@@ -3060,9 +3064,9 @@
       <c r="C34" s="7">
         <v>34847060.600000001</v>
       </c>
-      <c r="D34" s="7" t="str">
-        <f>IF(VLOOKUP(A34,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D34" s="7">
+        <f>VLOOKUP(A34,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E34" s="6">
         <v>1742353</v>
@@ -3080,9 +3084,9 @@
       <c r="C35" s="7">
         <v>554.64984700000002</v>
       </c>
-      <c r="D35" s="7" t="str">
-        <f>IF(VLOOKUP(A35,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D35" s="7">
+        <f>VLOOKUP(A35,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E35" s="6">
         <v>110.9</v>
@@ -3090,7 +3094,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>52</v>
       </c>
@@ -3100,9 +3104,9 @@
       <c r="C36" s="7">
         <v>15150975.09</v>
       </c>
-      <c r="D36" s="7" t="str">
-        <f>IF(VLOOKUP(A36,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D36" s="7">
+        <f>VLOOKUP(A36,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E36" s="6">
         <v>15150975.09</v>
@@ -3120,9 +3124,9 @@
       <c r="C37" s="7">
         <v>4273.9050960000004</v>
       </c>
-      <c r="D37" s="7" t="str">
-        <f>IF(VLOOKUP(A37,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D37" s="7">
+        <f>VLOOKUP(A37,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E37" s="6">
         <v>4273.9050960000004</v>
@@ -3140,9 +3144,9 @@
       <c r="C38" s="7">
         <v>0.05</v>
       </c>
-      <c r="D38" s="7" t="str">
-        <f>IF(VLOOKUP(A38,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D38" s="7">
+        <f>VLOOKUP(A38,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E38" s="6">
         <v>0.05</v>
@@ -3160,9 +3164,9 @@
       <c r="C39" s="7">
         <v>401050.08909999998</v>
       </c>
-      <c r="D39" s="7" t="str">
-        <f>IF(VLOOKUP(A39,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D39" s="7">
+        <f>VLOOKUP(A39,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E39" s="6">
         <v>201050.08910000001</v>
@@ -3182,9 +3186,9 @@
       <c r="C40" s="7">
         <v>28898.867849999999</v>
       </c>
-      <c r="D40" s="7" t="str">
-        <f>IF(VLOOKUP(A40,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D40" s="7">
+        <f>VLOOKUP(A40,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E40" s="6">
         <v>28898.867849999999</v>
@@ -3192,7 +3196,7 @@
       <c r="F40" s="6"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>4</v>
       </c>
@@ -3202,9 +3206,9 @@
       <c r="C41" s="7">
         <v>20527442.649999999</v>
       </c>
-      <c r="D41" s="7" t="str">
-        <f>IF(VLOOKUP(A41,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D41" s="7">
+        <f>VLOOKUP(A41,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E41" s="6">
         <v>6384375</v>
@@ -3222,9 +3226,9 @@
       <c r="C42" s="7">
         <v>6221.5131609999999</v>
       </c>
-      <c r="D42" s="7" t="str">
-        <f>IF(VLOOKUP(A42,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D42" s="7">
+        <f>VLOOKUP(A42,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E42" s="6">
         <v>6221.5131609999999</v>
@@ -3242,9 +3246,9 @@
       <c r="C43" s="7">
         <v>24854569.199999999</v>
       </c>
-      <c r="D43" s="7" t="str">
-        <f>IF(VLOOKUP(A43,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D43" s="7">
+        <f>VLOOKUP(A43,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E43" s="6">
         <v>3521063.9419999998</v>
@@ -3262,9 +3266,9 @@
       <c r="C44" s="7">
         <v>53.609603989999997</v>
       </c>
-      <c r="D44" s="7" t="str">
-        <f>IF(VLOOKUP(A44,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D44" s="7">
+        <f>VLOOKUP(A44,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E44" s="6">
         <v>20</v>
@@ -3282,9 +3286,9 @@
       <c r="C45" s="7">
         <v>16705.027440000002</v>
       </c>
-      <c r="D45" s="7" t="str">
-        <f>IF(VLOOKUP(A45,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D45" s="7">
+        <f>VLOOKUP(A45,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E45" s="6">
         <v>75000</v>
@@ -3303,9 +3307,9 @@
       <c r="C46" s="7">
         <v>15779070.359999999</v>
       </c>
-      <c r="D46" s="7" t="str">
-        <f>IF(VLOOKUP(A46,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D46" s="7">
+        <f>VLOOKUP(A46,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E46" s="6">
         <v>1540000</v>
@@ -3323,9 +3327,9 @@
       <c r="C47" s="7">
         <v>10723808.939999999</v>
       </c>
-      <c r="D47" s="7" t="str">
-        <f>IF(VLOOKUP(A47,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D47" s="7">
+        <f>VLOOKUP(A47,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E47" s="6">
         <v>357460.29800000001</v>
@@ -3343,9 +3347,9 @@
       <c r="C48" s="7">
         <v>2957397.3650000002</v>
       </c>
-      <c r="D48" s="7" t="str">
-        <f>IF(VLOOKUP(A48,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D48" s="7">
+        <f>VLOOKUP(A48,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E48" s="6">
         <v>4928995.608</v>
@@ -3363,9 +3367,9 @@
       <c r="C49" s="7">
         <v>361154520.60000002</v>
       </c>
-      <c r="D49" s="7" t="str">
-        <f>IF(VLOOKUP(A49,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D49" s="7">
+        <f>VLOOKUP(A49,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E49" s="6">
         <v>72230904</v>
@@ -3373,7 +3377,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>59</v>
       </c>
@@ -3384,17 +3388,19 @@
         <v>7496.955054</v>
       </c>
       <c r="D50" s="7" t="str">
-        <f>IF(VLOOKUP(A50,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+        <f>VLOOKUP(A50,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>ORIG</v>
       </c>
       <c r="E50" s="6">
         <v>7496.955054</v>
       </c>
-      <c r="F50" s="6"/>
+      <c r="F50" s="6">
+        <v>10000</v>
+      </c>
       <c r="G50" s="11"/>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>32</v>
       </c>
@@ -3404,9 +3410,9 @@
       <c r="C51" s="7">
         <v>5700290.8640000001</v>
       </c>
-      <c r="D51" s="7" t="str">
-        <f>IF(VLOOKUP(A51,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D51" s="7">
+        <f>VLOOKUP(A51,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E51" s="6">
         <v>5700290.8640000001</v>
@@ -3425,13 +3431,15 @@
         <v>358999.37920000002</v>
       </c>
       <c r="D52" s="7" t="str">
-        <f>IF(VLOOKUP(A52,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A52,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E52" s="6">
         <v>250000</v>
       </c>
-      <c r="F52" s="6"/>
+      <c r="F52" s="6">
+        <v>200000</v>
+      </c>
       <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3444,9 +3452,9 @@
       <c r="C53" s="7">
         <v>233447.39780000001</v>
       </c>
-      <c r="D53" s="7" t="str">
-        <f>IF(VLOOKUP(A53,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D53" s="7">
+        <f>VLOOKUP(A53,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E53" s="6">
         <v>58361.849450000002</v>
@@ -3465,13 +3473,15 @@
         <v>1053704.304</v>
       </c>
       <c r="D54" s="7" t="str">
-        <f>IF(VLOOKUP(A54,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A54,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E54" s="6">
         <v>1001250</v>
       </c>
-      <c r="F54" s="6"/>
+      <c r="F54" s="6">
+        <v>750000</v>
+      </c>
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3485,16 +3495,18 @@
         <v>177129.4045</v>
       </c>
       <c r="D55" s="7" t="str">
-        <f>IF(VLOOKUP(A55,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
+        <f>VLOOKUP(A55,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
         <v>-</v>
       </c>
       <c r="E55" s="6">
         <v>125000</v>
       </c>
-      <c r="F55" s="6"/>
+      <c r="F55" s="6">
+        <v>100000</v>
+      </c>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>33</v>
       </c>
@@ -3505,13 +3517,15 @@
         <v>40960.04507</v>
       </c>
       <c r="D56" s="7" t="str">
-        <f>IF(VLOOKUP(A56,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+        <f>VLOOKUP(A56,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+</v>
       </c>
       <c r="E56" s="6">
         <v>639000</v>
       </c>
-      <c r="F56" s="6"/>
+      <c r="F56" s="6">
+        <v>1000000</v>
+      </c>
       <c r="G56" s="11"/>
       <c r="H56" s="9"/>
     </row>
@@ -3525,9 +3539,9 @@
       <c r="C57" s="7">
         <v>71.004761549999998</v>
       </c>
-      <c r="D57" s="7" t="str">
-        <f>IF(VLOOKUP(A57,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D57" s="7">
+        <f>VLOOKUP(A57,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E57" s="6">
         <v>71.004761549999998</v>
@@ -3545,9 +3559,9 @@
       <c r="C58" s="7">
         <v>52020187.369999997</v>
       </c>
-      <c r="D58" s="7" t="str">
-        <f>IF(VLOOKUP(A58,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D58" s="7">
+        <f>VLOOKUP(A58,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E58" s="6">
         <v>52020187.369999997</v>
@@ -3565,9 +3579,9 @@
       <c r="C59" s="7">
         <v>14975339.800000001</v>
       </c>
-      <c r="D59" s="7" t="str">
-        <f>IF(VLOOKUP(A59,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D59" s="7">
+        <f>VLOOKUP(A59,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E59" s="6">
         <v>747664.42</v>
@@ -3585,9 +3599,9 @@
       <c r="C60" s="7">
         <v>3738776.034</v>
       </c>
-      <c r="D60" s="7" t="str">
-        <f>IF(VLOOKUP(A60,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D60" s="7">
+        <f>VLOOKUP(A60,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E60" s="6">
         <v>1080000</v>
@@ -3595,7 +3609,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="11"/>
     </row>
-    <row r="61" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>51</v>
       </c>
@@ -3605,9 +3619,9 @@
       <c r="C61" s="7">
         <v>97071048.260000005</v>
       </c>
-      <c r="D61" s="7" t="str">
-        <f>IF(VLOOKUP(A61,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D61" s="7">
+        <f>VLOOKUP(A61,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E61" s="6">
         <v>60071048.259999998</v>
@@ -3615,7 +3629,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="11"/>
     </row>
-    <row r="62" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>16</v>
       </c>
@@ -3625,9 +3639,9 @@
       <c r="C62" s="7">
         <v>20265685.109999999</v>
       </c>
-      <c r="D62" s="7" t="str">
-        <f>IF(VLOOKUP(A62,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D62" s="7">
+        <f>VLOOKUP(A62,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E62" s="6">
         <v>10265685.109999999</v>
@@ -3645,9 +3659,9 @@
       <c r="C63" s="7">
         <v>2983706.8709999998</v>
       </c>
-      <c r="D63" s="7" t="str">
-        <f>IF(VLOOKUP(A63,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v/>
+      <c r="D63" s="7">
+        <f>VLOOKUP(A63,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E63" s="6">
         <v>491000</v>
@@ -3655,7 +3669,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="11"/>
     </row>
-    <row r="64" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>43</v>
       </c>
@@ -3665,9 +3679,9 @@
       <c r="C64" s="7">
         <v>204805160.5</v>
       </c>
-      <c r="D64" s="7" t="str">
-        <f>IF(VLOOKUP(A64,'Group Condition'!$A$2:$C$88,3,FALSE)="X","-","")</f>
-        <v>-</v>
+      <c r="D64" s="7">
+        <f>VLOOKUP(A64,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="E64" s="6">
         <v>150805160.5</v>
@@ -3714,9 +3728,11 @@
   </sheetData>
   <autoFilter ref="A1:O68">
     <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters>
+        <filter val="-"/>
+        <filter val="+"/>
+        <filter val="ORIG"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ReducePred 10 - Turned on all previous mL and mQ mortality terms that were turned off by RM for tuning - Reformated some of biology.prm for easier parsing. Remove tab delimiters for mortality terms - modified mL decreased mL for MAK and COD - Increased mQ for pred groups with longterm sustained growth - Decreased mQ for pred groups with rapid declines/extinctions - Restored KDENR for protected spp to original values now that mortality is back on - Generally, if mortality was changed, KDENR was reverted to original RM value
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -9,14 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Group Condition" sheetId="1" r:id="rId1"/>
     <sheet name="Recruitment_Log" sheetId="3" r:id="rId2"/>
+    <sheet name="mL-Log" sheetId="4" r:id="rId3"/>
+    <sheet name="mQ-log" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group Condition'!$A$1:$I$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'mL-Log'!$A$1:$G$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'mQ-log'!$A$1:$G$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recruitment_Log!$A$1:$O$68</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="208">
   <si>
     <t>Too Low</t>
   </si>
@@ -598,16 +602,61 @@
     <t>ReducePred9_DKENR</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>ORIG</t>
-  </si>
-  <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>REVERT</t>
+  </si>
+  <si>
+    <t>PRED</t>
+  </si>
+  <si>
+    <t>-/MORT</t>
+  </si>
+  <si>
+    <t>MORT</t>
+  </si>
+  <si>
+    <t>+/MORT</t>
+  </si>
+  <si>
+    <t>REVERT/-MORT</t>
+  </si>
+  <si>
+    <t>+/-MORT</t>
+  </si>
+  <si>
+    <t>-/+MORT</t>
+  </si>
+  <si>
+    <t>-/+M,ORT</t>
+  </si>
+  <si>
+    <t>-/PRED/MORT</t>
+  </si>
+  <si>
+    <t>-MORT/PRED</t>
+  </si>
+  <si>
+    <t>DIET</t>
+  </si>
+  <si>
+    <t>DIET/-MORT</t>
+  </si>
+  <si>
+    <t>orig_mL1</t>
+  </si>
+  <si>
+    <t>orig_mL2</t>
+  </si>
+  <si>
+    <t>ReducePred10_DKENR</t>
+  </si>
+  <si>
+    <t>ReducePred10_mL1</t>
+  </si>
+  <si>
+    <t>ReducePred10_mL2</t>
   </si>
 </sst>
 </file>
@@ -696,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -729,6 +778,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,9 +1062,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,7 +1109,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1067,41 +1117,46 @@
         <v>122</v>
       </c>
       <c r="G2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H2" t="str">
         <f>IF(COUNTIF(C2:G2,"X")=0,"X","")</f>
         <v/>
       </c>
       <c r="I2" s="13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>102</v>
       </c>
+      <c r="G3" t="s">
+        <v>180</v>
+      </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">IF(COUNTIF(C3:G3,"X")=0,"X","")</f>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>110</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1119,16 +1174,22 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>114</v>
       </c>
+      <c r="G6" t="s">
+        <v>180</v>
+      </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1149,7 +1210,7 @@
         <v/>
       </c>
       <c r="I7" s="13" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1164,7 +1225,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1178,8 +1239,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1193,8 +1257,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1208,8 +1275,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1224,31 +1294,40 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>147</v>
       </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>167</v>
       </c>
+      <c r="E14" t="s">
+        <v>180</v>
+      </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1275,7 +1354,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1293,7 +1372,7 @@
         <v/>
       </c>
       <c r="I17" s="13" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1308,7 +1387,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1322,8 +1401,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1337,8 +1419,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1353,19 +1438,22 @@
         <v/>
       </c>
       <c r="I21" s="13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>164</v>
       </c>
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1380,19 +1468,22 @@
         <v>X</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
       <c r="B24" t="s">
         <v>170</v>
       </c>
+      <c r="D24" t="s">
+        <v>180</v>
+      </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1410,7 +1501,7 @@
         <v/>
       </c>
       <c r="I25" s="13" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1425,7 +1516,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1440,16 +1531,22 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
       <c r="B28" t="s">
         <v>131</v>
       </c>
+      <c r="E28" t="s">
+        <v>180</v>
+      </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1469,20 +1566,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I29" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
       <c r="B30" t="s">
         <v>150</v>
       </c>
+      <c r="C30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D30" t="s">
+        <v>180</v>
+      </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1516,12 +1619,9 @@
       <c r="B33" t="s">
         <v>158</v>
       </c>
-      <c r="G33" t="s">
-        <v>180</v>
-      </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1531,6 +1631,9 @@
       <c r="B34" t="s">
         <v>151</v>
       </c>
+      <c r="C34" t="s">
+        <v>180</v>
+      </c>
       <c r="D34" t="s">
         <v>180</v>
       </c>
@@ -1538,11 +1641,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I34" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1559,6 +1659,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="I35" s="13" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -1572,16 +1675,25 @@
         <v>X</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
       <c r="B37" t="s">
         <v>145</v>
       </c>
+      <c r="C37" t="s">
+        <v>180</v>
+      </c>
+      <c r="D37" t="s">
+        <v>180</v>
+      </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1596,7 +1708,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -1611,10 +1723,10 @@
         <v/>
       </c>
       <c r="I39" s="13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -1629,7 +1741,7 @@
         <v/>
       </c>
       <c r="I40" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1651,15 +1763,12 @@
       <c r="B42" t="s">
         <v>130</v>
       </c>
-      <c r="G42" t="s">
-        <v>180</v>
-      </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -1673,6 +1782,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="I43" s="13" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -1681,12 +1793,9 @@
       <c r="B44" t="s">
         <v>142</v>
       </c>
-      <c r="G44" t="s">
-        <v>180</v>
-      </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -1701,19 +1810,25 @@
         <v>X</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>34</v>
       </c>
       <c r="B46" t="s">
         <v>123</v>
       </c>
+      <c r="D46" t="s">
+        <v>180</v>
+      </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1735,15 +1850,12 @@
       <c r="B48" t="s">
         <v>116</v>
       </c>
-      <c r="G48" t="s">
-        <v>180</v>
-      </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -1758,7 +1870,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -1770,7 +1882,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -1782,19 +1894,25 @@
         <v>X</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>18</v>
       </c>
       <c r="B52" t="s">
         <v>103</v>
       </c>
+      <c r="D52" t="s">
+        <v>180</v>
+      </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1806,7 +1924,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -1818,7 +1936,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -1830,7 +1948,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -1842,7 +1960,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -1854,19 +1972,25 @@
         <v>X</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>55</v>
       </c>
       <c r="B58" t="s">
         <v>144</v>
       </c>
+      <c r="E58" t="s">
+        <v>180</v>
+      </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -1878,7 +2002,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -1890,7 +2014,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -1904,23 +2028,23 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I61" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>30</v>
       </c>
       <c r="B62" t="s">
         <v>118</v>
       </c>
-      <c r="G62" t="s">
-        <v>180</v>
-      </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -1932,31 +2056,43 @@
         <v>X</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
       <c r="B64" t="s">
         <v>146</v>
       </c>
+      <c r="D64" t="s">
+        <v>180</v>
+      </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>46</v>
       </c>
       <c r="B65" t="s">
         <v>135</v>
       </c>
+      <c r="D65" t="s">
+        <v>180</v>
+      </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -1970,8 +2106,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I66" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -1986,16 +2125,22 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>54</v>
       </c>
       <c r="B68" t="s">
         <v>143</v>
       </c>
+      <c r="E68" t="s">
+        <v>180</v>
+      </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v/>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -2025,19 +2170,28 @@
         <v>X</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>26</v>
       </c>
       <c r="B71" t="s">
         <v>113</v>
       </c>
+      <c r="C71" t="s">
+        <v>180</v>
+      </c>
+      <c r="D71" t="s">
+        <v>180</v>
+      </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I71" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2052,7 +2206,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>27</v>
       </c>
@@ -2066,20 +2220,26 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I73" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>59</v>
       </c>
       <c r="B74" t="s">
         <v>148</v>
       </c>
+      <c r="E74" t="s">
+        <v>180</v>
+      </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="I74" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -2100,7 +2260,7 @@
         <v/>
       </c>
       <c r="I75" s="13" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -2121,10 +2281,10 @@
         <v/>
       </c>
       <c r="I76" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -2138,8 +2298,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I77" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -2157,7 +2320,7 @@
         <v/>
       </c>
       <c r="I78" s="13" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -2181,10 +2344,10 @@
         <v/>
       </c>
       <c r="I79" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -2199,10 +2362,10 @@
         <v/>
       </c>
       <c r="I80" s="13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>60</v>
       </c>
@@ -2213,20 +2376,29 @@
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I81" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
       <c r="B82" t="s">
         <v>94</v>
       </c>
+      <c r="G82" t="s">
+        <v>180</v>
+      </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2240,20 +2412,29 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I83" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>15</v>
       </c>
       <c r="B84" t="s">
         <v>98</v>
       </c>
+      <c r="G84" t="s">
+        <v>180</v>
+      </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I84" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>51</v>
       </c>
@@ -2265,19 +2446,25 @@
         <v>X</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
       <c r="B86" t="s">
         <v>99</v>
       </c>
+      <c r="G86" t="s">
+        <v>180</v>
+      </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I86" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -2289,7 +2476,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>43</v>
       </c>
@@ -2303,10 +2490,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I88">
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="7">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2318,11 +2503,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
+      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2366,6 +2551,9 @@
       <c r="F1" s="3" t="s">
         <v>188</v>
       </c>
+      <c r="G1" s="10" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="2" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -2379,7 +2567,7 @@
       </c>
       <c r="D2" s="7" t="str">
         <f>VLOOKUP(A2,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>+</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E2" s="6">
         <v>45700000</v>
@@ -2387,9 +2575,12 @@
       <c r="F2" s="7">
         <v>1001094433</v>
       </c>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="11">
+        <f>F2*1.25</f>
+        <v>1251368041.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -2399,20 +2590,23 @@
       <c r="C3" s="7">
         <v>2124041.1490000002</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="str">
         <f>VLOOKUP(A3,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E3" s="6">
         <v>2124041.1490000002</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="11"/>
+      <c r="G3" s="11">
+        <f>E3*1.25</f>
+        <v>2655051.4362500003</v>
+      </c>
       <c r="K3" s="5"/>
       <c r="M3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2422,15 +2616,17 @@
       <c r="C4" s="7">
         <v>114181041.2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="7" t="str">
         <f>VLOOKUP(A4,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+</v>
       </c>
       <c r="E4" s="6">
         <v>19030174.25</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="11"/>
+      <c r="G4" s="7">
+        <v>114181041.2</v>
+      </c>
     </row>
     <row r="5" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
@@ -2464,7 +2660,7 @@
       </c>
       <c r="D6" s="7" t="str">
         <f>VLOOKUP(A6,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>-/MORT</v>
       </c>
       <c r="E6" s="6">
         <v>1718757.3940000001</v>
@@ -2473,9 +2669,11 @@
         <f>E6*0.5</f>
         <v>859378.69700000004</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="11">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -2485,15 +2683,18 @@
       <c r="C7" s="7">
         <v>16477555.609999999</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="7" t="str">
         <f>VLOOKUP(A7,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E7" s="6">
         <v>993066.96089999995</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="11"/>
+      <c r="G7" s="7">
+        <f>C7*0.75</f>
+        <v>12358166.7075</v>
+      </c>
       <c r="K7" s="11"/>
       <c r="M7" s="11"/>
     </row>
@@ -2527,9 +2728,9 @@
       <c r="C9" s="7">
         <v>32122718.550000001</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="7" t="str">
         <f>VLOOKUP(A9,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>PRED</v>
       </c>
       <c r="E9" s="6">
         <v>321227180.55000001</v>
@@ -2550,9 +2751,9 @@
       <c r="C10" s="7">
         <v>2123.8950410000002</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="7" t="str">
         <f>VLOOKUP(A10,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>DIET</v>
       </c>
       <c r="E10" s="6">
         <v>2123.8950410000002</v>
@@ -2570,9 +2771,9 @@
       <c r="C11" s="7">
         <v>74822.192989999996</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="7" t="str">
         <f>VLOOKUP(A11,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>DIET/-MORT</v>
       </c>
       <c r="E11" s="6">
         <v>74822.192989999996</v>
@@ -2583,7 +2784,7 @@
       <c r="M11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>58</v>
       </c>
@@ -2593,15 +2794,17 @@
       <c r="C12" s="7">
         <v>235.45910710000001</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="7" t="str">
         <f>VLOOKUP(A12,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>REVERT</v>
       </c>
       <c r="E12" s="6">
         <v>10</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="11">
+        <v>235</v>
+      </c>
     </row>
     <row r="13" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
@@ -2635,7 +2838,7 @@
       </c>
       <c r="D14" s="7" t="str">
         <f>VLOOKUP(A14,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>-/+M,ORT</v>
       </c>
       <c r="E14" s="6">
         <v>176000000</v>
@@ -2644,7 +2847,9 @@
         <f>E14*0.75</f>
         <v>132000000</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="6">
+        <v>176000000</v>
+      </c>
     </row>
     <row r="15" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
@@ -2678,7 +2883,7 @@
       </c>
       <c r="D16" s="7" t="str">
         <f>VLOOKUP(A16,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>+/MORT</v>
       </c>
       <c r="E16" s="6">
         <v>100000</v>
@@ -2687,12 +2892,14 @@
         <f>E16*0.75</f>
         <v>75000</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="6">
+        <v>100000</v>
+      </c>
       <c r="M16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>22</v>
       </c>
@@ -2702,20 +2909,22 @@
       <c r="C17" s="7">
         <v>21996106.07</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="7" t="str">
         <f>VLOOKUP(A17,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E17" s="6">
         <v>4000000</v>
       </c>
       <c r="F17" s="6"/>
-      <c r="G17" s="11"/>
+      <c r="G17" s="11">
+        <v>10000000</v>
+      </c>
       <c r="K17" s="5"/>
       <c r="M17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -2725,15 +2934,17 @@
       <c r="C18" s="7">
         <v>17230050.359999999</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="7" t="str">
         <f>VLOOKUP(A18,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>-/MORT</v>
       </c>
       <c r="E18" s="6">
         <v>8500000</v>
       </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="11">
+        <v>10000000</v>
+      </c>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
@@ -2770,9 +2981,9 @@
       <c r="C20" s="7">
         <v>432544359.30000001</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="7" t="str">
         <f>VLOOKUP(A20,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>MORT</v>
       </c>
       <c r="E20" s="6">
         <v>2430000</v>
@@ -2782,7 +2993,7 @@
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>63</v>
       </c>
@@ -2792,9 +3003,9 @@
       <c r="C21" s="7">
         <v>0.05</v>
       </c>
-      <c r="D21" s="7" t="str">
+      <c r="D21" s="7">
         <f>VLOOKUP(A21,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="E21" s="6">
         <v>3.5000000000000003E-2</v>
@@ -2805,7 +3016,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>61</v>
       </c>
@@ -2815,17 +3026,19 @@
       <c r="C22" s="7">
         <v>747577.53830000001</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="7" t="str">
         <f>VLOOKUP(A22,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>-/+MORT</v>
       </c>
       <c r="E22" s="6">
         <v>197000</v>
       </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="11">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>42</v>
       </c>
@@ -2835,18 +3048,20 @@
       <c r="C23" s="7">
         <v>172649603.19999999</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="7" t="str">
         <f>VLOOKUP(A23,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E23" s="6">
         <v>49700000</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="11">
+        <v>100000000</v>
+      </c>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>62</v>
       </c>
@@ -2856,9 +3071,9 @@
       <c r="C24" s="7">
         <v>0.05</v>
       </c>
-      <c r="D24" s="7" t="str">
+      <c r="D24" s="7">
         <f>VLOOKUP(A24,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="E24" s="6">
         <v>3.5000000000000003E-2</v>
@@ -2880,9 +3095,9 @@
       <c r="C25" s="7">
         <v>932233758.39999998</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="7" t="str">
         <f>VLOOKUP(A25,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>PRED</v>
       </c>
       <c r="E25" s="6">
         <v>532233758.39999998</v>
@@ -2890,7 +3105,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>56</v>
       </c>
@@ -2900,15 +3115,17 @@
       <c r="C26" s="7">
         <v>749.83099549999997</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="7" t="str">
         <f>VLOOKUP(A26,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>REVERT</v>
       </c>
       <c r="E26" s="6">
         <v>100</v>
       </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="11"/>
+      <c r="G26" s="7">
+        <v>749.83099549999997</v>
+      </c>
     </row>
     <row r="27" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
@@ -2962,7 +3179,7 @@
       </c>
       <c r="D29" s="7" t="str">
         <f>VLOOKUP(A29,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>-/+MORT</v>
       </c>
       <c r="E29" s="6">
         <v>150000</v>
@@ -2970,7 +3187,9 @@
       <c r="F29" s="6">
         <v>100000</v>
       </c>
-      <c r="G29" s="11"/>
+      <c r="G29" s="11">
+        <v>200000</v>
+      </c>
     </row>
     <row r="30" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
@@ -3024,9 +3243,9 @@
       <c r="C32" s="7">
         <v>22940055.34</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="7" t="str">
         <f>VLOOKUP(A32,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>-/MORT</v>
       </c>
       <c r="E32" s="6">
         <v>22940055.34</v>
@@ -3186,9 +3405,9 @@
       <c r="C40" s="7">
         <v>28898.867849999999</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="7" t="str">
         <f>VLOOKUP(A40,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>REVERT</v>
       </c>
       <c r="E40" s="6">
         <v>28898.867849999999</v>
@@ -3256,7 +3475,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>57</v>
       </c>
@@ -3266,17 +3485,19 @@
       <c r="C44" s="7">
         <v>53.609603989999997</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="7" t="str">
         <f>VLOOKUP(A44,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>REVERT</v>
       </c>
       <c r="E44" s="6">
         <v>20</v>
       </c>
       <c r="F44" s="6"/>
-      <c r="G44" s="11"/>
-    </row>
-    <row r="45" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G44" s="11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
@@ -3286,15 +3507,17 @@
       <c r="C45" s="7">
         <v>16705.027440000002</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="7" t="str">
         <f>VLOOKUP(A45,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>-/+MORT</v>
       </c>
       <c r="E45" s="6">
         <v>75000</v>
       </c>
       <c r="F45" s="6"/>
-      <c r="G45" s="11"/>
+      <c r="G45" s="7">
+        <v>16705.027440000002</v>
+      </c>
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3317,7 +3540,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>54</v>
       </c>
@@ -3327,17 +3550,19 @@
       <c r="C47" s="7">
         <v>10723808.939999999</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="7" t="str">
         <f>VLOOKUP(A47,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>REVERT/-MORT</v>
       </c>
       <c r="E47" s="6">
         <v>357460.29800000001</v>
       </c>
       <c r="F47" s="6"/>
-      <c r="G47" s="11"/>
-    </row>
-    <row r="48" spans="1:16" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G47" s="7">
+        <v>10723808.939999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>26</v>
       </c>
@@ -3347,17 +3572,19 @@
       <c r="C48" s="7">
         <v>2957397.3650000002</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="7" t="str">
         <f>VLOOKUP(A48,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>-/+MORT</v>
       </c>
       <c r="E48" s="6">
         <v>4928995.608</v>
       </c>
       <c r="F48" s="6"/>
-      <c r="G48" s="11"/>
-    </row>
-    <row r="49" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G48" s="7">
+        <v>2957397.3650000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>27</v>
       </c>
@@ -3367,15 +3594,17 @@
       <c r="C49" s="7">
         <v>361154520.60000002</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="7" t="str">
         <f>VLOOKUP(A49,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E49" s="6">
         <v>72230904</v>
       </c>
       <c r="F49" s="6"/>
-      <c r="G49" s="11"/>
+      <c r="G49" s="7">
+        <v>361154520.60000002</v>
+      </c>
     </row>
     <row r="50" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
@@ -3389,7 +3618,7 @@
       </c>
       <c r="D50" s="7" t="str">
         <f>VLOOKUP(A50,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>ORIG</v>
+        <v>REVERT</v>
       </c>
       <c r="E50" s="6">
         <v>7496.955054</v>
@@ -3397,7 +3626,9 @@
       <c r="F50" s="6">
         <v>10000</v>
       </c>
-      <c r="G50" s="11"/>
+      <c r="G50" s="7">
+        <v>7496.955054</v>
+      </c>
       <c r="O50" s="5"/>
     </row>
     <row r="51" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3410,9 +3641,9 @@
       <c r="C51" s="7">
         <v>5700290.8640000001</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="7" t="str">
         <f>VLOOKUP(A51,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>MORT</v>
       </c>
       <c r="E51" s="6">
         <v>5700290.8640000001</v>
@@ -3432,7 +3663,7 @@
       </c>
       <c r="D52" s="7" t="str">
         <f>VLOOKUP(A52,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>-/+MORT</v>
       </c>
       <c r="E52" s="6">
         <v>250000</v>
@@ -3440,9 +3671,11 @@
       <c r="F52" s="6">
         <v>200000</v>
       </c>
-      <c r="G52" s="11"/>
-    </row>
-    <row r="53" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G52" s="6">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>37</v>
       </c>
@@ -3452,15 +3685,17 @@
       <c r="C53" s="7">
         <v>233447.39780000001</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="7" t="str">
         <f>VLOOKUP(A53,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E53" s="6">
         <v>58361.849450000002</v>
       </c>
       <c r="F53" s="6"/>
-      <c r="G53" s="11"/>
+      <c r="G53" s="7">
+        <v>233447.39780000001</v>
+      </c>
     </row>
     <row r="54" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
@@ -3474,7 +3709,7 @@
       </c>
       <c r="D54" s="7" t="str">
         <f>VLOOKUP(A54,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>-/PRED/MORT</v>
       </c>
       <c r="E54" s="6">
         <v>1001250</v>
@@ -3482,7 +3717,9 @@
       <c r="F54" s="6">
         <v>750000</v>
       </c>
-      <c r="G54" s="11"/>
+      <c r="G54" s="7">
+        <v>1053704.304</v>
+      </c>
     </row>
     <row r="55" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
@@ -3496,7 +3733,7 @@
       </c>
       <c r="D55" s="7" t="str">
         <f>VLOOKUP(A55,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>-</v>
+        <v>-/+MORT</v>
       </c>
       <c r="E55" s="6">
         <v>125000</v>
@@ -3504,7 +3741,9 @@
       <c r="F55" s="6">
         <v>100000</v>
       </c>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11">
+        <v>150000</v>
+      </c>
     </row>
     <row r="56" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
@@ -3518,7 +3757,7 @@
       </c>
       <c r="D56" s="7" t="str">
         <f>VLOOKUP(A56,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>+</v>
+        <v>-MORT/PRED</v>
       </c>
       <c r="E56" s="6">
         <v>639000</v>
@@ -3526,7 +3765,9 @@
       <c r="F56" s="6">
         <v>1000000</v>
       </c>
-      <c r="G56" s="11"/>
+      <c r="G56" s="7">
+        <v>40960.04507</v>
+      </c>
       <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3539,9 +3780,9 @@
       <c r="C57" s="7">
         <v>71.004761549999998</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="7" t="str">
         <f>VLOOKUP(A57,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>REVERT</v>
       </c>
       <c r="E57" s="6">
         <v>71.004761549999998</v>
@@ -3559,9 +3800,9 @@
       <c r="C58" s="7">
         <v>52020187.369999997</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="7" t="str">
         <f>VLOOKUP(A58,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E58" s="6">
         <v>52020187.369999997</v>
@@ -3569,7 +3810,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>13</v>
       </c>
@@ -3579,17 +3820,19 @@
       <c r="C59" s="7">
         <v>14975339.800000001</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="7" t="str">
         <f>VLOOKUP(A59,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E59" s="6">
         <v>747664.42</v>
       </c>
       <c r="F59" s="6"/>
-      <c r="G59" s="11"/>
-    </row>
-    <row r="60" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G59" s="11">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>15</v>
       </c>
@@ -3599,15 +3842,17 @@
       <c r="C60" s="7">
         <v>3738776.034</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="7" t="str">
         <f>VLOOKUP(A60,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E60" s="6">
         <v>1080000</v>
       </c>
       <c r="F60" s="6"/>
-      <c r="G60" s="11"/>
+      <c r="G60" s="11">
+        <v>2000000</v>
+      </c>
     </row>
     <row r="61" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
@@ -3629,7 +3874,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="11"/>
     </row>
-    <row r="62" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>16</v>
       </c>
@@ -3639,15 +3884,17 @@
       <c r="C62" s="7">
         <v>20265685.109999999</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D62" s="7" t="str">
         <f>VLOOKUP(A62,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
-        <v>0</v>
+        <v>+/-MORT</v>
       </c>
       <c r="E62" s="6">
         <v>10265685.109999999</v>
       </c>
       <c r="F62" s="6"/>
-      <c r="G62" s="11"/>
+      <c r="G62" s="11">
+        <v>15000000</v>
+      </c>
     </row>
     <row r="63" spans="1:15" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
@@ -3729,13 +3976,2639 @@
   <autoFilter ref="A1:O68">
     <filterColumn colId="3">
       <filters>
-        <filter val="-"/>
+        <filter val="-/+M,ORT"/>
+        <filter val="-/+MORT"/>
+        <filter val="-/MORT"/>
+        <filter val="-/PRED/MORT"/>
         <filter val="+"/>
-        <filter val="ORIG"/>
+        <filter val="+/MORT"/>
+        <filter val="+/-MORT"/>
+        <filter val="DIET"/>
+        <filter val="DIET/-MORT"/>
+        <filter val="MORT"/>
+        <filter val="-MORT/PRED"/>
+        <filter val="PRED"/>
+        <filter val="REVERT"/>
+        <filter val="REVERT/-MORT"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="str">
+        <f>VLOOKUP(A2,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="str">
+        <f>VLOOKUP(A3,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4">
+        <v>7.9999999999999998E-12</v>
+      </c>
+      <c r="D4">
+        <v>7.9999999999999998E-12</v>
+      </c>
+      <c r="E4" s="7" t="str">
+        <f>VLOOKUP(A4,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <f>VLOOKUP(A5,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="str">
+        <f>VLOOKUP(A6,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/MORT</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7">
+        <v>8.2499999999999999E-11</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f>VLOOKUP(A7,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1E-13</v>
+      </c>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <f>VLOOKUP(A8,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9">
+        <v>9E-13</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="str">
+        <f>VLOOKUP(A9,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>PRED</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f>VLOOKUP(A10,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>DIET</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="str">
+        <f>VLOOKUP(A11,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>DIET/-MORT</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12">
+        <v>1.0999999999999999E-8</v>
+      </c>
+      <c r="D12">
+        <v>1.0999999999999999E-8</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f>VLOOKUP(A12,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <f>VLOOKUP(A13,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="str">
+        <f>VLOOKUP(A14,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+M,ORT</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <f>VLOOKUP(A15,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7" t="str">
+        <f>VLOOKUP(A16,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/MORT</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17">
+        <v>7.9999999999999998E-12</v>
+      </c>
+      <c r="D17">
+        <v>7.9999999999999998E-12</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f>VLOOKUP(A17,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7" t="str">
+        <f>VLOOKUP(A18,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/MORT</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <f>VLOOKUP(A19,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f>VLOOKUP(A20,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>MORT</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D21">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E21" s="7">
+        <f>VLOOKUP(A21,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="str">
+        <f>VLOOKUP(A22,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7" t="str">
+        <f>VLOOKUP(A23,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D24">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E24" s="7">
+        <f>VLOOKUP(A24,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7" t="str">
+        <f>VLOOKUP(A25,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>PRED</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="D26">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="E26" s="7" t="str">
+        <f>VLOOKUP(A26,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27">
+        <v>6.9999999999999997E-7</v>
+      </c>
+      <c r="D27">
+        <v>6.9999999999999997E-7</v>
+      </c>
+      <c r="E27" s="7">
+        <f>VLOOKUP(A27,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
+        <f>VLOOKUP(A28,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7" t="str">
+        <f>VLOOKUP(A29,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30">
+        <v>1E-10</v>
+      </c>
+      <c r="D30">
+        <v>1E-10</v>
+      </c>
+      <c r="E30" s="7">
+        <f>VLOOKUP(A30,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31">
+        <v>6.7499999999999997E-6</v>
+      </c>
+      <c r="D31">
+        <v>6.7499999999999997E-6</v>
+      </c>
+      <c r="E31" s="7">
+        <f>VLOOKUP(A31,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7" t="str">
+        <f>VLOOKUP(A32,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/MORT</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="7">
+        <f>VLOOKUP(A33,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34">
+        <v>7.9999999999999998E-12</v>
+      </c>
+      <c r="D34">
+        <v>7.9999999999999998E-12</v>
+      </c>
+      <c r="E34" s="7">
+        <f>VLOOKUP(A34,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7">
+        <f>VLOOKUP(A35,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36">
+        <v>1E-10</v>
+      </c>
+      <c r="D36">
+        <v>1E-10</v>
+      </c>
+      <c r="E36" s="7">
+        <f>VLOOKUP(A36,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="7">
+        <f>VLOOKUP(A37,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38">
+        <v>6.7499999999999997E-6</v>
+      </c>
+      <c r="D38">
+        <v>6.7499999999999997E-6</v>
+      </c>
+      <c r="E38" s="7">
+        <f>VLOOKUP(A38,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
+        <f>VLOOKUP(A39,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40">
+        <v>8.9999999999999996E-7</v>
+      </c>
+      <c r="D40">
+        <v>8.9999999999999996E-7</v>
+      </c>
+      <c r="E40" s="7" t="str">
+        <f>VLOOKUP(A40,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" s="7">
+        <f>VLOOKUP(A41,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <f>VLOOKUP(A42,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" s="7">
+        <f>VLOOKUP(A43,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44">
+        <v>1.0999999999999999E-8</v>
+      </c>
+      <c r="D44">
+        <v>1.0999999999999999E-8</v>
+      </c>
+      <c r="E44" s="7" t="str">
+        <f>VLOOKUP(A44,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" s="7" t="str">
+        <f>VLOOKUP(A45,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" s="7">
+        <f>VLOOKUP(A46,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" s="7" t="str">
+        <f>VLOOKUP(A47,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT/-MORT</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48">
+        <v>9E-13</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" s="7" t="str">
+        <f>VLOOKUP(A48,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" s="7" t="str">
+        <f>VLOOKUP(A49,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50">
+        <v>2E-8</v>
+      </c>
+      <c r="D50">
+        <v>2E-8</v>
+      </c>
+      <c r="E50" s="7" t="str">
+        <f>VLOOKUP(A50,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7" t="str">
+        <f>VLOOKUP(A51,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>MORT</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7" t="str">
+        <f>VLOOKUP(A52,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7" t="str">
+        <f>VLOOKUP(A53,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="7" t="str">
+        <f>VLOOKUP(A54,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/PRED/MORT</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="str">
+        <f>VLOOKUP(A55,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7" t="str">
+        <f>VLOOKUP(A56,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-MORT/PRED</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57">
+        <v>2E-8</v>
+      </c>
+      <c r="D57">
+        <v>2E-8</v>
+      </c>
+      <c r="E57" s="7" t="str">
+        <f>VLOOKUP(A57,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58">
+        <v>3.8000000000000001E-9</v>
+      </c>
+      <c r="D58">
+        <v>3.8000000000000001E-9</v>
+      </c>
+      <c r="E58" s="7" t="str">
+        <f>VLOOKUP(A58,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="str">
+        <f>VLOOKUP(A59,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="str">
+        <f>VLOOKUP(A60,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61">
+        <v>1E-10</v>
+      </c>
+      <c r="D61">
+        <v>1E-10</v>
+      </c>
+      <c r="E61" s="7">
+        <f>VLOOKUP(A61,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="str">
+        <f>VLOOKUP(A62,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7">
+        <f>VLOOKUP(A63,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64">
+        <v>5.0000000000000004E-19</v>
+      </c>
+      <c r="D64">
+        <v>5.0000000000000004E-19</v>
+      </c>
+      <c r="E64" s="7">
+        <f>VLOOKUP(A64,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G64"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45:XFD45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D2">
+        <v>3E-10</v>
+      </c>
+      <c r="E2" s="7" t="str">
+        <f>VLOOKUP(A2,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F2">
+        <f>C2*0.75</f>
+        <v>2.25E-13</v>
+      </c>
+      <c r="G2" s="14">
+        <f>D2*0.75</f>
+        <v>2.25E-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>9.25E-13</v>
+      </c>
+      <c r="D3">
+        <v>1.8E-9</v>
+      </c>
+      <c r="E3" s="7" t="str">
+        <f>VLOOKUP(A3,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F3">
+        <f>C3*0.75</f>
+        <v>6.9374999999999995E-13</v>
+      </c>
+      <c r="G3" s="14">
+        <f>D3*0.75</f>
+        <v>1.3500000000000001E-9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4">
+        <v>2.25E-11</v>
+      </c>
+      <c r="D4">
+        <v>1.8E-10</v>
+      </c>
+      <c r="E4" s="7" t="str">
+        <f>VLOOKUP(A4,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="D5">
+        <v>2E-8</v>
+      </c>
+      <c r="E5" s="7">
+        <f>VLOOKUP(A5,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D6">
+        <v>3E-10</v>
+      </c>
+      <c r="E6" s="7" t="str">
+        <f>VLOOKUP(A6,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/MORT</v>
+      </c>
+      <c r="F6">
+        <f>C6*1.25</f>
+        <v>3.7499999999999997E-13</v>
+      </c>
+      <c r="G6" s="14">
+        <f>D6*1.25</f>
+        <v>3.75E-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7">
+        <v>1.5E-11</v>
+      </c>
+      <c r="D7">
+        <v>7.8999999999999996E-9</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f>VLOOKUP(A7,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F7">
+        <f>C7*0.75</f>
+        <v>1.125E-11</v>
+      </c>
+      <c r="G7" s="14">
+        <f>D7*0.75</f>
+        <v>5.9250000000000001E-9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8">
+        <v>1E-14</v>
+      </c>
+      <c r="D8">
+        <v>1E-14</v>
+      </c>
+      <c r="E8" s="7">
+        <f>VLOOKUP(A8,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9">
+        <v>1E-14</v>
+      </c>
+      <c r="D9">
+        <v>8.0000000000000002E-13</v>
+      </c>
+      <c r="E9" s="7" t="str">
+        <f>VLOOKUP(A9,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>PRED</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1.4999999999999999E-14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D10">
+        <v>3E-10</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f>VLOOKUP(A10,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>DIET</v>
+      </c>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D11">
+        <v>3E-10</v>
+      </c>
+      <c r="E11" s="7" t="str">
+        <f>VLOOKUP(A11,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>DIET/-MORT</v>
+      </c>
+      <c r="G11" s="14">
+        <v>3E-11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12">
+        <v>1.5E-6</v>
+      </c>
+      <c r="D12">
+        <v>3.15E-5</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f>VLOOKUP(A12,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13">
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="D13">
+        <v>2E-8</v>
+      </c>
+      <c r="E13" s="7">
+        <f>VLOOKUP(A13,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14">
+        <v>1E-14</v>
+      </c>
+      <c r="D14">
+        <v>1E-13</v>
+      </c>
+      <c r="E14" s="7" t="str">
+        <f>VLOOKUP(A14,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+M,ORT</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1E-13</v>
+      </c>
+      <c r="G14" s="14">
+        <v>2.0000000000000001E-13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15">
+        <v>1E-8</v>
+      </c>
+      <c r="D15">
+        <v>4.4999999999999999E-8</v>
+      </c>
+      <c r="E15" s="7">
+        <f>VLOOKUP(A15,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D16">
+        <v>3E-10</v>
+      </c>
+      <c r="E16" s="7" t="str">
+        <f>VLOOKUP(A16,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/MORT</v>
+      </c>
+      <c r="F16" s="14">
+        <v>1E-13</v>
+      </c>
+      <c r="G16" s="14">
+        <v>1E-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17">
+        <v>2.25E-11</v>
+      </c>
+      <c r="D17">
+        <v>1.8E-10</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f>VLOOKUP(A17,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F17">
+        <f>C17*0.5</f>
+        <v>1.125E-11</v>
+      </c>
+      <c r="G17" s="14">
+        <f>D17*0.5</f>
+        <v>8.9999999999999999E-11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D18">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E18" s="7" t="str">
+        <f>VLOOKUP(A18,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/MORT</v>
+      </c>
+      <c r="F18">
+        <f>C18*1.25</f>
+        <v>6.4999999999999993E-10</v>
+      </c>
+      <c r="G18" s="14">
+        <f>D18*1.25</f>
+        <v>4.0000000000000002E-9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D19">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E19" s="7">
+        <f>VLOOKUP(A19,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="D20">
+        <v>8.5E-9</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f>VLOOKUP(A20,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>MORT</v>
+      </c>
+      <c r="F20">
+        <f>C20*0.5</f>
+        <v>1.25E-11</v>
+      </c>
+      <c r="G20" s="14">
+        <f>D20*0.5</f>
+        <v>4.25E-9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21">
+        <v>1.47E-3</v>
+      </c>
+      <c r="D21">
+        <v>1.7600000000000001E-3</v>
+      </c>
+      <c r="E21" s="7">
+        <f>VLOOKUP(A21,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D22">
+        <v>3E-10</v>
+      </c>
+      <c r="E22" s="7" t="str">
+        <f>VLOOKUP(A22,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+      <c r="F22">
+        <f>C22*1.5</f>
+        <v>4.5E-13</v>
+      </c>
+      <c r="G22" s="14">
+        <f>D22*1.5</f>
+        <v>4.5E-10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23">
+        <v>2.6499999999999999E-11</v>
+      </c>
+      <c r="D23">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="E23" s="7" t="str">
+        <f>VLOOKUP(A23,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F23">
+        <f>C23*0.75</f>
+        <v>1.9874999999999999E-11</v>
+      </c>
+      <c r="G23" s="14">
+        <f>D23*0.75</f>
+        <v>3.0000000000000004E-9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24">
+        <v>1.47E-3</v>
+      </c>
+      <c r="D24">
+        <v>1.7600000000000001E-3</v>
+      </c>
+      <c r="E24" s="7">
+        <f>VLOOKUP(A24,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25">
+        <v>1E-14</v>
+      </c>
+      <c r="D25">
+        <v>2.4999999999999998E-12</v>
+      </c>
+      <c r="E25" s="7" t="str">
+        <f>VLOOKUP(A25,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>PRED</v>
+      </c>
+      <c r="F25">
+        <f>C25*1.25</f>
+        <v>1.25E-14</v>
+      </c>
+      <c r="G25" s="14">
+        <f>D25*1.25</f>
+        <v>3.1249999999999997E-12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26">
+        <v>5.5000000000000003E-7</v>
+      </c>
+      <c r="D26">
+        <v>2.4999999999999999E-7</v>
+      </c>
+      <c r="E26" s="7" t="str">
+        <f>VLOOKUP(A26,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="D27">
+        <v>4.4999999999999998E-9</v>
+      </c>
+      <c r="E27" s="7">
+        <f>VLOOKUP(A27,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D28">
+        <v>3E-10</v>
+      </c>
+      <c r="E28" s="7">
+        <f>VLOOKUP(A28,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D29">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E29" s="7" t="str">
+        <f>VLOOKUP(A29,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+      <c r="F29">
+        <f>C29*1.5</f>
+        <v>7.7999999999999999E-10</v>
+      </c>
+      <c r="G29" s="14">
+        <f>D29*1.5</f>
+        <v>4.8E-9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30">
+        <v>5.0000000000000003E-10</v>
+      </c>
+      <c r="D30">
+        <v>2.5000000000000001E-9</v>
+      </c>
+      <c r="E30" s="7">
+        <f>VLOOKUP(A30,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31">
+        <v>1.7700000000000001E-3</v>
+      </c>
+      <c r="D31">
+        <v>1.7700000000000001E-3</v>
+      </c>
+      <c r="E31" s="7">
+        <f>VLOOKUP(A31,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D32">
+        <v>3E-10</v>
+      </c>
+      <c r="E32" s="7" t="str">
+        <f>VLOOKUP(A32,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/MORT</v>
+      </c>
+      <c r="F32">
+        <f>C32*1.5</f>
+        <v>4.5E-13</v>
+      </c>
+      <c r="G32" s="14">
+        <f>D32*1.5</f>
+        <v>4.5E-10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D33">
+        <v>3E-10</v>
+      </c>
+      <c r="E33" s="7">
+        <f>VLOOKUP(A33,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34">
+        <v>2.25E-11</v>
+      </c>
+      <c r="D34">
+        <v>1.8E-10</v>
+      </c>
+      <c r="E34" s="7">
+        <f>VLOOKUP(A34,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35">
+        <v>4.9999999999999999E-13</v>
+      </c>
+      <c r="D35">
+        <v>3.4999999999999998E-10</v>
+      </c>
+      <c r="E35" s="7">
+        <f>VLOOKUP(A35,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36">
+        <v>5.0000000000000003E-10</v>
+      </c>
+      <c r="D36">
+        <v>2.5000000000000001E-9</v>
+      </c>
+      <c r="E36" s="7">
+        <f>VLOOKUP(A36,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37">
+        <v>1E-8</v>
+      </c>
+      <c r="D37">
+        <v>4.4999999999999999E-8</v>
+      </c>
+      <c r="E37" s="7">
+        <f>VLOOKUP(A37,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38">
+        <v>1.7700000000000001E-3</v>
+      </c>
+      <c r="D38">
+        <v>1.7700000000000001E-3</v>
+      </c>
+      <c r="E38" s="7">
+        <f>VLOOKUP(A38,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39">
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="D39">
+        <v>2E-8</v>
+      </c>
+      <c r="E39" s="7">
+        <f>VLOOKUP(A39,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40">
+        <v>1.4999999999999999E-7</v>
+      </c>
+      <c r="D40">
+        <v>6.8999999999999996E-7</v>
+      </c>
+      <c r="E40" s="7" t="str">
+        <f>VLOOKUP(A40,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D41">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E41" s="7">
+        <f>VLOOKUP(A41,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42">
+        <v>1E-8</v>
+      </c>
+      <c r="D42">
+        <v>4.4999999999999999E-8</v>
+      </c>
+      <c r="E42" s="7">
+        <f>VLOOKUP(A42,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D43">
+        <v>3E-10</v>
+      </c>
+      <c r="E43" s="7">
+        <f>VLOOKUP(A43,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44">
+        <v>1.5E-6</v>
+      </c>
+      <c r="D44">
+        <v>3.15E-5</v>
+      </c>
+      <c r="E44" s="7" t="str">
+        <f>VLOOKUP(A44,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45">
+        <v>4.9999999999999999E-13</v>
+      </c>
+      <c r="D45">
+        <v>3.4999999999999998E-10</v>
+      </c>
+      <c r="E45" s="7" t="str">
+        <f>VLOOKUP(A45,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+      <c r="F45">
+        <f>C45*1.5</f>
+        <v>7.5000000000000004E-13</v>
+      </c>
+      <c r="G45" s="14">
+        <f>D45*1.5</f>
+        <v>5.2499999999999994E-10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D46">
+        <v>3E-10</v>
+      </c>
+      <c r="E46" s="7">
+        <f>VLOOKUP(A46,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G46"/>
+    </row>
+    <row r="47" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47">
+        <v>4.3000000000000001E-7</v>
+      </c>
+      <c r="D47">
+        <v>1.3E-6</v>
+      </c>
+      <c r="E47" s="7" t="str">
+        <f>VLOOKUP(A47,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT/-MORT</v>
+      </c>
+      <c r="G47"/>
+    </row>
+    <row r="48" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48">
+        <v>1E-14</v>
+      </c>
+      <c r="D48">
+        <v>8.0000000000000002E-13</v>
+      </c>
+      <c r="E48" s="7" t="str">
+        <f>VLOOKUP(A48,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49">
+        <v>1.5E-11</v>
+      </c>
+      <c r="D49">
+        <v>2.6000000000000001E-9</v>
+      </c>
+      <c r="E49" s="7" t="str">
+        <f>VLOOKUP(A49,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50">
+        <v>4.5000000000000001E-6</v>
+      </c>
+      <c r="D50">
+        <v>1.5E-5</v>
+      </c>
+      <c r="E50" s="7" t="str">
+        <f>VLOOKUP(A50,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D51">
+        <v>3E-10</v>
+      </c>
+      <c r="E51" s="7" t="str">
+        <f>VLOOKUP(A51,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>MORT</v>
+      </c>
+      <c r="F51">
+        <f>C51*0.75</f>
+        <v>2.25E-13</v>
+      </c>
+      <c r="G51" s="14">
+        <f>D51*0.75</f>
+        <v>2.25E-10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52">
+        <v>4.9999999999999999E-13</v>
+      </c>
+      <c r="D52">
+        <v>3.4999999999999998E-10</v>
+      </c>
+      <c r="E52" s="7" t="str">
+        <f>VLOOKUP(A52,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+      <c r="F52">
+        <f>C52*1.5</f>
+        <v>7.5000000000000004E-13</v>
+      </c>
+      <c r="G52" s="14">
+        <f>D52*1.5</f>
+        <v>5.2499999999999994E-10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C53">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D53">
+        <v>3E-10</v>
+      </c>
+      <c r="E53" s="7" t="str">
+        <f>VLOOKUP(A53,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="G53"/>
+    </row>
+    <row r="54" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D54">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E54" s="7" t="str">
+        <f>VLOOKUP(A54,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/PRED/MORT</v>
+      </c>
+      <c r="F54">
+        <f>C54*1.25</f>
+        <v>6.4999999999999993E-10</v>
+      </c>
+      <c r="G54" s="14">
+        <f>D54*1.25</f>
+        <v>4.0000000000000002E-9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D55">
+        <v>3E-10</v>
+      </c>
+      <c r="E55" s="7" t="str">
+        <f>VLOOKUP(A55,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-/+MORT</v>
+      </c>
+      <c r="F55">
+        <f>C55*2</f>
+        <v>5.9999999999999997E-13</v>
+      </c>
+      <c r="G55" s="14">
+        <f>D55*2</f>
+        <v>6E-10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D56">
+        <v>3E-10</v>
+      </c>
+      <c r="E56" s="7" t="str">
+        <f>VLOOKUP(A56,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>-MORT/PRED</v>
+      </c>
+      <c r="F56">
+        <f>C56/2</f>
+        <v>1.4999999999999999E-13</v>
+      </c>
+      <c r="G56" s="14">
+        <f>D56/2</f>
+        <v>1.5E-10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57">
+        <v>4.5000000000000001E-6</v>
+      </c>
+      <c r="D57">
+        <v>1.5E-5</v>
+      </c>
+      <c r="E57" s="7" t="str">
+        <f>VLOOKUP(A57,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>REVERT</v>
+      </c>
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58">
+        <v>2.7499999999999998E-9</v>
+      </c>
+      <c r="D58">
+        <v>3.7499999999999998E-8</v>
+      </c>
+      <c r="E58" s="7" t="str">
+        <f>VLOOKUP(A58,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F58" s="14">
+        <v>1E-10</v>
+      </c>
+      <c r="G58" s="14">
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D59">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E59" s="7" t="str">
+        <f>VLOOKUP(A59,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F59">
+        <f>C59*0.5</f>
+        <v>2.5999999999999998E-10</v>
+      </c>
+      <c r="G59" s="14">
+        <f>D59*0.5</f>
+        <v>1.6000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D60">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E60" s="7" t="str">
+        <f>VLOOKUP(A60,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F60">
+        <f>C60*0.5</f>
+        <v>2.5999999999999998E-10</v>
+      </c>
+      <c r="G60" s="14">
+        <f>D60*0.5</f>
+        <v>1.6000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61">
+        <v>5.0000000000000003E-10</v>
+      </c>
+      <c r="D61">
+        <v>2.5000000000000001E-9</v>
+      </c>
+      <c r="E61" s="7">
+        <f>VLOOKUP(A61,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G61"/>
+    </row>
+    <row r="62" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D62">
+        <v>3.2000000000000001E-9</v>
+      </c>
+      <c r="E62" s="7" t="str">
+        <f>VLOOKUP(A62,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>+/-MORT</v>
+      </c>
+      <c r="F62">
+        <f>C62*0.5</f>
+        <v>2.5999999999999998E-10</v>
+      </c>
+      <c r="G62" s="14">
+        <f>D62*0.5</f>
+        <v>1.6000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="D63">
+        <v>3E-10</v>
+      </c>
+      <c r="E63" s="7">
+        <f>VLOOKUP(A63,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G63"/>
+    </row>
+    <row r="64" spans="1:7" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="D64">
+        <v>1.9000000000000001E-9</v>
+      </c>
+      <c r="E64" s="7">
+        <f>VLOOKUP(A64,'Group Condition'!$A$2:$I$88,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G64"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G64">
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with Fishing and Initial Scalar
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -22,14 +22,13 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Crash Diagnosis'!$A$1:$J$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group Condition'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group Condition'!$A$1:$K$88</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'mL-Log'!$A$1:$G$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'mQ-log'!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Notes Log'!$A$1:$E$88</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Recruitment_Log!$A$1:$O$68</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1684,13 +1683,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1746,7 +1746,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>110</v>
       </c>
       <c r="H2" t="str">
-        <f>IF(OR(COUNTIF(C2:G2,"X")=0,COUNTIF(C2:G2,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" ref="H2:H33" si="0">IF(OR(COUNTIF(C2:G2,"X")=0,COUNTIF(C2:G2,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
       <c r="K2" s="13">
@@ -1765,7 +1765,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>175</v>
       </c>
       <c r="H3" t="str">
-        <f>IF(OR(COUNTIF(C3:G3,"X")=0,COUNTIF(C3:G3,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K3" s="13" t="s">
@@ -1784,7 +1784,7 @@
         <v>1000.68</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>180</v>
       </c>
       <c r="H4" t="str">
-        <f>IF(OR(COUNTIF(C4:G4,"X")=0,COUNTIF(C4:G4,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K4" s="13" t="s">
@@ -1806,7 +1806,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>164</v>
       </c>
       <c r="H5" t="str">
-        <f>IF(OR(COUNTIF(C5:G5,"X")=0,COUNTIF(C5:G5,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K5" s="13" t="s">
@@ -1825,7 +1825,7 @@
         <v>4.8259999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>264</v>
       </c>
       <c r="H6" t="str">
-        <f>IF(OR(COUNTIF(C6:G6,"X")=0,COUNTIF(C6:G6,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="L6">
@@ -1858,7 +1858,7 @@
         <v>180</v>
       </c>
       <c r="H7" t="str">
-        <f>IF(OR(COUNTIF(C7:G7,"X")=0,COUNTIF(C7:G7,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I7" s="13" t="s">
@@ -1875,7 +1875,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>264</v>
       </c>
       <c r="H8" t="str">
-        <f>IF(OR(COUNTIF(C8:G8,"X")=0,COUNTIF(C8:G8,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="L8">
@@ -1902,7 +1902,7 @@
         <v>106</v>
       </c>
       <c r="H9" t="str">
-        <f>IF(OR(COUNTIF(C9:G9,"X")=0,COUNTIF(C9:G9,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="J9" t="s">
@@ -1930,7 +1930,7 @@
         <v>180</v>
       </c>
       <c r="H10" t="str">
-        <f>IF(OR(COUNTIF(C10:G10,"X")=0,COUNTIF(C10:G10,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I10" s="13" t="s">
@@ -1952,7 +1952,7 @@
         <v>137</v>
       </c>
       <c r="H11" t="str">
-        <f>IF(OR(COUNTIF(C11:G11,"X")=0,COUNTIF(C11:G11,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="J11" t="s">
@@ -1966,7 +1966,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>180</v>
       </c>
       <c r="H12" t="str">
-        <f>IF(OR(COUNTIF(C12:G12,"X")=0,COUNTIF(C12:G12,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L12">
@@ -1985,7 +1985,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>176</v>
       </c>
       <c r="H13" t="str">
-        <f>IF(OR(COUNTIF(C13:G13,"X")=0,COUNTIF(C13:G13,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K13" s="13" t="s">
@@ -2004,7 +2004,7 @@
         <v>49.42</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>109</v>
       </c>
       <c r="H14" t="str">
-        <f>IF(OR(COUNTIF(C14:G14,"X")=0,COUNTIF(C14:G14,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K14" s="13" t="s">
@@ -2037,7 +2037,7 @@
         <v>180</v>
       </c>
       <c r="H15" t="str">
-        <f>IF(OR(COUNTIF(C15:G15,"X")=0,COUNTIF(C15:G15,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I15" s="13" t="s">
@@ -2068,7 +2068,7 @@
         <v>180</v>
       </c>
       <c r="H16" t="str">
-        <f>IF(OR(COUNTIF(C16:G16,"X")=0,COUNTIF(C16:G16,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I16" s="13" t="s">
@@ -2085,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>180</v>
       </c>
       <c r="H17" t="str">
-        <f>IF(OR(COUNTIF(C17:G17,"X")=0,COUNTIF(C17:G17,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K17" s="13" t="s">
@@ -2107,7 +2107,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>264</v>
       </c>
       <c r="H18" t="str">
-        <f>IF(OR(COUNTIF(C18:G18,"X")=0,COUNTIF(C18:G18,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="L18">
@@ -2126,7 +2126,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>114</v>
       </c>
       <c r="H19" t="str">
-        <f>IF(OR(COUNTIF(C19:G19,"X")=0,COUNTIF(C19:G19,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K19" s="13" t="s">
@@ -2145,7 +2145,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>170</v>
       </c>
       <c r="H20" t="str">
-        <f>IF(OR(COUNTIF(C20:G20,"X")=0,COUNTIF(C20:G20,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K20" s="13" t="s">
@@ -2164,7 +2164,7 @@
         <v>7.84</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>177</v>
       </c>
       <c r="H21" t="str">
-        <f>IF(OR(COUNTIF(C21:G21,"X")=0,COUNTIF(C21:G21,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="L21">
@@ -2180,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>133</v>
       </c>
       <c r="H22" t="str">
-        <f>IF(OR(COUNTIF(C22:G22,"X")=0,COUNTIF(C22:G22,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K22" s="13" t="s">
@@ -2199,7 +2199,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>178</v>
       </c>
       <c r="H23" t="str">
-        <f>IF(OR(COUNTIF(C23:G23,"X")=0,COUNTIF(C23:G23,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="L23">
@@ -2229,7 +2229,7 @@
         <v>180</v>
       </c>
       <c r="H24" t="str">
-        <f>IF(OR(COUNTIF(C24:G24,"X")=0,COUNTIF(C24:G24,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I24" s="13" t="s">
@@ -2246,7 +2246,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>136</v>
       </c>
       <c r="H25" t="str">
-        <f>IF(OR(COUNTIF(C25:G25,"X")=0,COUNTIF(C25:G25,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K25" s="13" t="s">
@@ -2273,7 +2273,7 @@
         <v>113</v>
       </c>
       <c r="H26" t="str">
-        <f>IF(OR(COUNTIF(C26:G26,"X")=0,COUNTIF(C26:G26,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="J26" t="s">
@@ -2287,7 +2287,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>180</v>
       </c>
       <c r="H27" t="str">
-        <f>IF(OR(COUNTIF(C27:G27,"X")=0,COUNTIF(C27:G27,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L27">
@@ -2306,7 +2306,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>103</v>
       </c>
       <c r="H28" t="str">
-        <f>IF(OR(COUNTIF(C28:G28,"X")=0,COUNTIF(C28:G28,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K28" s="13" t="s">
@@ -2325,7 +2325,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>100</v>
       </c>
       <c r="H29" t="str">
-        <f>IF(OR(COUNTIF(C29:G29,"X")=0,COUNTIF(C29:G29,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="K29" s="13" t="s">
@@ -2344,7 +2344,7 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>180</v>
       </c>
       <c r="H30" t="str">
-        <f>IF(OR(COUNTIF(C30:G30,"X")=0,COUNTIF(C30:G30,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I30" s="13" t="s">
@@ -2372,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>180</v>
       </c>
       <c r="H31" t="str">
-        <f>IF(OR(COUNTIF(C31:G31,"X")=0,COUNTIF(C31:G31,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I31" s="13" t="s">
@@ -2397,7 +2397,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>180</v>
       </c>
       <c r="H32" t="str">
-        <f>IF(OR(COUNTIF(C32:G32,"X")=0,COUNTIF(C32:G32,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I32" s="13" t="s">
@@ -2433,7 +2433,7 @@
         <v>93</v>
       </c>
       <c r="H33" t="str">
-        <f>IF(OR(COUNTIF(C33:G33,"X")=0,COUNTIF(C33:G33,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="J33" t="s">
@@ -2447,7 +2447,7 @@
         <v>373.37</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>150</v>
       </c>
       <c r="H34" t="str">
-        <f>IF(OR(COUNTIF(C34:G34,"X")=0,COUNTIF(C34:G34,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" ref="H34:H65" si="1">IF(OR(COUNTIF(C34:G34,"X")=0,COUNTIF(C34:G34,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
       <c r="K34" s="13" t="s">
@@ -2466,7 +2466,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>152</v>
       </c>
       <c r="H35" t="str">
-        <f>IF(OR(COUNTIF(C35:G35,"X")=0,COUNTIF(C35:G35,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K35" s="13" t="s">
@@ -2485,7 +2485,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>264</v>
       </c>
       <c r="H36" t="str">
-        <f>IF(OR(COUNTIF(C36:G36,"X")=0,COUNTIF(C36:G36,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K36" s="13" t="s">
@@ -2510,7 +2510,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>141</v>
       </c>
       <c r="H37" t="str">
-        <f>IF(OR(COUNTIF(C37:G37,"X")=0,COUNTIF(C37:G37,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K37" s="13" t="s">
@@ -2529,7 +2529,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>151</v>
       </c>
       <c r="H38" t="str">
-        <f>IF(OR(COUNTIF(C38:G38,"X")=0,COUNTIF(C38:G38,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K38" s="13" t="s">
@@ -2548,7 +2548,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>165</v>
       </c>
       <c r="H39" t="str">
-        <f>IF(OR(COUNTIF(C39:G39,"X")=0,COUNTIF(C39:G39,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="L39">
@@ -2578,7 +2578,7 @@
         <v>180</v>
       </c>
       <c r="H40" t="str">
-        <f>IF(OR(COUNTIF(C40:G40,"X")=0,COUNTIF(C40:G40,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I40" s="13" t="s">
@@ -2603,7 +2603,7 @@
         <v>180</v>
       </c>
       <c r="H41" t="str">
-        <f>IF(OR(COUNTIF(C41:G41,"X")=0,COUNTIF(C41:G41,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I41" s="13" t="s">
@@ -2617,7 +2617,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>180</v>
       </c>
       <c r="H42" t="str">
-        <f>IF(OR(COUNTIF(C42:G42,"X")=0,COUNTIF(C42:G42,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K42" s="13" t="s">
@@ -2639,7 +2639,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>180</v>
       </c>
       <c r="H43" t="str">
-        <f>IF(OR(COUNTIF(C43:G43,"X")=0,COUNTIF(C43:G43,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L43">
@@ -2658,7 +2658,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>180</v>
       </c>
       <c r="H44" t="str">
-        <f>IF(OR(COUNTIF(C44:G44,"X")=0,COUNTIF(C44:G44,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K44" s="13" t="s">
@@ -2680,7 +2680,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>123</v>
       </c>
       <c r="H45" t="str">
-        <f>IF(OR(COUNTIF(C45:G45,"X")=0,COUNTIF(C45:G45,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K45" s="13" t="s">
@@ -2699,7 +2699,7 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>180</v>
       </c>
       <c r="H46" t="str">
-        <f>IF(OR(COUNTIF(C46:G46,"X")=0,COUNTIF(C46:G46,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L46">
@@ -2718,7 +2718,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>174</v>
       </c>
       <c r="H47" t="str">
-        <f>IF(OR(COUNTIF(C47:G47,"X")=0,COUNTIF(C47:G47,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K47" s="13" t="s">
@@ -2737,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>180</v>
       </c>
       <c r="H48" t="str">
-        <f>IF(OR(COUNTIF(C48:G48,"X")=0,COUNTIF(C48:G48,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K48" s="13" t="s">
@@ -2762,7 +2762,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>80</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>169</v>
       </c>
       <c r="H49" t="str">
-        <f>IF(OR(COUNTIF(C49:G49,"X")=0,COUNTIF(C49:G49,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="L49">
@@ -2789,7 +2789,7 @@
         <v>180</v>
       </c>
       <c r="H50" t="str">
-        <f>IF(OR(COUNTIF(C50:G50,"X")=0,COUNTIF(C50:G50,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I50" s="13" t="s">
@@ -2806,7 +2806,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>180</v>
       </c>
       <c r="H51" t="str">
-        <f>IF(OR(COUNTIF(C51:G51,"X")=0,COUNTIF(C51:G51,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K51" s="13" t="s">
@@ -2836,7 +2836,7 @@
         <v>138</v>
       </c>
       <c r="H52" t="str">
-        <f>IF(OR(COUNTIF(C52:G52,"X")=0,COUNTIF(C52:G52,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="J52" t="s">
@@ -2847,7 +2847,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>171</v>
       </c>
       <c r="H53" t="str">
-        <f>IF(OR(COUNTIF(C53:G53,"X")=0,COUNTIF(C53:G53,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="L53">
@@ -2871,7 +2871,7 @@
         <v>139</v>
       </c>
       <c r="H54" t="str">
-        <f>IF(OR(COUNTIF(C54:G54,"X")=0,COUNTIF(C54:G54,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="J54" t="s">
@@ -2885,7 +2885,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>264</v>
       </c>
       <c r="H55" t="str">
-        <f>IF(OR(COUNTIF(C55:G55,"X")=0,COUNTIF(C55:G55,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="L55">
@@ -2904,7 +2904,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>180</v>
       </c>
       <c r="H56" t="str">
-        <f>IF(OR(COUNTIF(C56:G56,"X")=0,COUNTIF(C56:G56,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L56">
@@ -2923,7 +2923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>122</v>
       </c>
       <c r="H57" t="str">
-        <f>IF(OR(COUNTIF(C57:G57,"X")=0,COUNTIF(C57:G57,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K57" s="13" t="s">
@@ -2942,7 +2942,7 @@
         <v>17.12</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>180</v>
       </c>
       <c r="H58" t="str">
-        <f>IF(OR(COUNTIF(C58:G58,"X")=0,COUNTIF(C58:G58,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L58">
@@ -2964,7 +2964,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>180</v>
       </c>
       <c r="H59" t="str">
-        <f>IF(OR(COUNTIF(C59:G59,"X")=0,COUNTIF(C59:G59,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L59">
@@ -2986,7 +2986,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>180</v>
       </c>
       <c r="H60" t="str">
-        <f>IF(OR(COUNTIF(C60:G60,"X")=0,COUNTIF(C60:G60,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K60" s="13" t="s">
@@ -3019,7 +3019,7 @@
         <v>180</v>
       </c>
       <c r="H61" t="str">
-        <f>IF(OR(COUNTIF(C61:G61,"X")=0,COUNTIF(C61:G61,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J61" t="s">
@@ -3033,7 +3033,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>143</v>
       </c>
       <c r="H62" t="str">
-        <f>IF(OR(COUNTIF(C62:G62,"X")=0,COUNTIF(C62:G62,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K62" s="13" t="s">
@@ -3052,7 +3052,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>264</v>
       </c>
       <c r="H63" t="str">
-        <f>IF(OR(COUNTIF(C63:G63,"X")=0,COUNTIF(C63:G63,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="L63">
@@ -3082,7 +3082,7 @@
         <v>180</v>
       </c>
       <c r="H64" t="str">
-        <f>IF(OR(COUNTIF(C64:G64,"X")=0,COUNTIF(C64:G64,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J64" t="s">
@@ -3107,7 +3107,7 @@
         <v>180</v>
       </c>
       <c r="H65" t="str">
-        <f>IF(OR(COUNTIF(C65:G65,"X")=0,COUNTIF(C65:G65,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J65" t="s">
@@ -3121,7 +3121,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>180</v>
       </c>
       <c r="H66" t="str">
-        <f>IF(OR(COUNTIF(C66:G66,"X")=0,COUNTIF(C66:G66,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" ref="H66:H97" si="2">IF(OR(COUNTIF(C66:G66,"X")=0,COUNTIF(C66:G66,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
       <c r="K66" s="13" t="s">
@@ -3151,7 +3151,7 @@
         <v>115</v>
       </c>
       <c r="H67" t="str">
-        <f>IF(OR(COUNTIF(C67:G67,"X")=0,COUNTIF(C67:G67,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="J67" t="s">
@@ -3165,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>53</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>180</v>
       </c>
       <c r="H68" t="str">
-        <f>IF(OR(COUNTIF(C68:G68,"X")=0,COUNTIF(C68:G68,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K68" s="13" t="s">
@@ -3187,7 +3187,7 @@
         <v>2.82</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>134</v>
       </c>
       <c r="H69" t="str">
-        <f>IF(OR(COUNTIF(C69:G69,"X")=0,COUNTIF(C69:G69,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="K69" s="13" t="s">
@@ -3206,7 +3206,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>46</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>135</v>
       </c>
       <c r="H70" t="str">
-        <f>IF(OR(COUNTIF(C70:G70,"X")=0,COUNTIF(C70:G70,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="K70" s="13" t="s">
@@ -3239,7 +3239,7 @@
         <v>180</v>
       </c>
       <c r="H71" t="str">
-        <f>IF(OR(COUNTIF(C71:G71,"X")=0,COUNTIF(C71:G71,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I71" s="13" t="s">
@@ -3267,7 +3267,7 @@
         <v>180</v>
       </c>
       <c r="H72" t="str">
-        <f>IF(OR(COUNTIF(C72:G72,"X")=0,COUNTIF(C72:G72,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I72" s="13" t="s">
@@ -3284,7 +3284,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>59</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>180</v>
       </c>
       <c r="H73" t="str">
-        <f>IF(OR(COUNTIF(C73:G73,"X")=0,COUNTIF(C73:G73,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K73" s="13" t="s">
@@ -3320,7 +3320,7 @@
         <v>180</v>
       </c>
       <c r="H74" t="str">
-        <f>IF(OR(COUNTIF(C74:G74,"X")=0,COUNTIF(C74:G74,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I74" s="13" t="s">
@@ -3345,7 +3345,7 @@
         <v>105</v>
       </c>
       <c r="H75" t="str">
-        <f>IF(OR(COUNTIF(C75:G75,"X")=0,COUNTIF(C75:G75,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="J75" t="s">
@@ -3359,7 +3359,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>60</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>149</v>
       </c>
       <c r="H76" t="str">
-        <f>IF(OR(COUNTIF(C76:G76,"X")=0,COUNTIF(C76:G76,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="K76" s="13" t="s">
@@ -3389,7 +3389,7 @@
         <v>180</v>
       </c>
       <c r="H77" t="str">
-        <f>IF(OR(COUNTIF(C77:G77,"X")=0,COUNTIF(C77:G77,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I77" s="13" t="s">
@@ -3403,7 +3403,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>180</v>
       </c>
       <c r="H78" t="str">
-        <f>IF(OR(COUNTIF(C78:G78,"X")=0,COUNTIF(C78:G78,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K78" s="13" t="s">
@@ -3425,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>180</v>
       </c>
       <c r="H79" t="str">
-        <f>IF(OR(COUNTIF(C79:G79,"X")=0,COUNTIF(C79:G79,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K79" s="13" t="s">
@@ -3447,7 +3447,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>180</v>
       </c>
       <c r="H80" t="str">
-        <f>IF(OR(COUNTIF(C80:G80,"X")=0,COUNTIF(C80:G80,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K80" s="13" t="s">
@@ -3469,7 +3469,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>96</v>
       </c>
       <c r="H81" t="str">
-        <f>IF(OR(COUNTIF(C81:G81,"X")=0,COUNTIF(C81:G81,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="K81" s="13" t="s">
@@ -3488,7 +3488,7 @@
         <v>1.93</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>51</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>140</v>
       </c>
       <c r="H82" t="str">
-        <f>IF(OR(COUNTIF(C82:G82,"X")=0,COUNTIF(C82:G82,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="K82" s="13" t="s">
@@ -3507,7 +3507,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>180</v>
       </c>
       <c r="H83" t="str">
-        <f>IF(OR(COUNTIF(C83:G83,"X")=0,COUNTIF(C83:G83,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K83" s="13" t="s">
@@ -3529,7 +3529,7 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>43</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>132</v>
       </c>
       <c r="H84" t="str">
-        <f>IF(OR(COUNTIF(C84:G84,"X")=0,COUNTIF(C84:G84,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="K84" s="13" t="s">
@@ -3548,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>180</v>
       </c>
       <c r="H85" t="str">
-        <f>IF(OR(COUNTIF(C85:G85,"X")=0,COUNTIF(C85:G85,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K85" s="13" t="s">
@@ -3570,7 +3570,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>180</v>
       </c>
       <c r="H86" t="str">
-        <f>IF(OR(COUNTIF(C86:G86,"X")=0,COUNTIF(C86:G86,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K86" s="13" t="s">
@@ -3592,7 +3592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>83</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>180</v>
       </c>
       <c r="H87" t="str">
-        <f>IF(OR(COUNTIF(C87:G87,"X")=0,COUNTIF(C87:G87,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K87" s="13" t="s">
@@ -3614,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>84</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>173</v>
       </c>
       <c r="H88" t="str">
-        <f>IF(OR(COUNTIF(C88:G88,"X")=0,COUNTIF(C88:G88,"B")&lt;&gt;0),"X","")</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
       <c r="K88" s="13" t="s">
@@ -3634,7 +3634,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1">
+  <autoFilter ref="A1:K88">
+    <filterColumn colId="9">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <sortState ref="A2:K88">
       <sortCondition ref="A1"/>
     </sortState>

</xml_diff>

<commit_message>
ZooTuningRevisit_1 -Diet changes to zooplankton and some other fish spp.
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" tabRatio="853"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" tabRatio="853"/>
   </bookViews>
   <sheets>
     <sheet name="Group Condition" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Crash Diagnosis'!$A$1:$L$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Group Condition'!$A$1:$K$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Group Condition'!$A$1:$K$88</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Group Diagnostic'!$A$1:$P$88</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Init Scalar Revert'!$A$2:$J$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'mL-Log'!$A$1:$S$1</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="445">
   <si>
     <t>Too Low</t>
   </si>
@@ -1360,9 +1360,6 @@
   </si>
   <si>
     <t>New_Init_CatchTS_4 mQ2</t>
-  </si>
-  <si>
-    <t>invert</t>
   </si>
   <si>
     <t>New_Init_CatchTS_5</t>
@@ -9333,13 +9330,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E80" sqref="E80"/>
+      <selection pane="bottomRight" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9392,7 +9390,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9411,15 +9409,12 @@
         <f>IF(OR(COUNTIF(D2:G2,"X")=0,COUNTIF(D2:G2,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K2">
         <f>VLOOKUP(A2,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>3.4146443350000002</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -9442,14 +9437,14 @@
         <v/>
       </c>
       <c r="J3" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K3">
         <f>VLOOKUP(A3,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>6.4963754189999996</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -9460,16 +9455,13 @@
       <c r="C4" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H4" s="22" t="str">
         <f>VLOOKUP(A4,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I4" s="24" t="str">
         <f>IF(OR(COUNTIF(D4:G4,"X")=0,COUNTIF(D4:G4,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>429</v>
@@ -9479,7 +9471,7 @@
         <v>125.479276</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -9498,15 +9490,12 @@
         <f>IF(OR(COUNTIF(D5:G5,"X")=0,COUNTIF(D5:G5,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J5" s="13" t="s">
-        <v>429</v>
-      </c>
       <c r="K5">
         <f>VLOOKUP(A5,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -9533,7 +9522,7 @@
         <v>13.60138179</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9574,7 +9563,8 @@
       <c r="C8" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="29"/>
+      <c r="G8" s="24" t="s">
         <v>180</v>
       </c>
       <c r="H8" s="22" t="str">
@@ -9586,14 +9576,14 @@
         <v/>
       </c>
       <c r="J8" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K8">
         <f>VLOOKUP(A8,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>15.58729078</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -9616,14 +9606,14 @@
         <v/>
       </c>
       <c r="J9" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K9">
         <f>VLOOKUP(A9,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.120275307</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -9646,14 +9636,14 @@
         <v/>
       </c>
       <c r="J10" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K10">
         <f>VLOOKUP(A10,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>2.07701E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -9676,14 +9666,14 @@
         <v/>
       </c>
       <c r="J11" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K11">
         <f>VLOOKUP(A11,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.88352E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -9706,14 +9696,14 @@
         <v/>
       </c>
       <c r="J12" s="13" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K12">
         <f>VLOOKUP(A12,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -9737,7 +9727,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -9748,26 +9738,23 @@
       <c r="C14" t="s">
         <v>167</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H14" s="22" t="str">
         <f>VLOOKUP(A14,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I14" s="24" t="str">
         <f>IF(OR(COUNTIF(D14:G14,"X")=0,COUNTIF(D14:G14,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K14">
         <f>VLOOKUP(A14,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.41</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -9778,26 +9765,23 @@
       <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H15" s="22" t="str">
         <f>VLOOKUP(A15,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I15" s="24" t="str">
         <f>IF(OR(COUNTIF(D15:G15,"X")=0,COUNTIF(D15:G15,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K15">
         <f>VLOOKUP(A15,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.22</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -9816,15 +9800,12 @@
         <f>IF(OR(COUNTIF(D16:G16,"X")=0,COUNTIF(D16:G16,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J16" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K16">
         <f>VLOOKUP(A16,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>6.6672173600000004</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -9854,7 +9835,7 @@
         <v>36.832345089999997</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -9876,15 +9857,12 @@
         <f>IF(OR(COUNTIF(D18:G18,"X")=0,COUNTIF(D18:G18,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J18" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K18">
         <f>VLOOKUP(A18,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -9908,14 +9886,14 @@
         <v/>
       </c>
       <c r="J19" s="13" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K19">
         <f>VLOOKUP(A19,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>8.2990938990000007</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -9926,7 +9904,7 @@
       <c r="C20" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="D20" s="22" t="s">
         <v>180</v>
       </c>
       <c r="H20" s="22" t="str">
@@ -9938,14 +9916,14 @@
         <v/>
       </c>
       <c r="J20" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K20">
         <f>VLOOKUP(A20,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>72.318494520000002</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -9968,14 +9946,14 @@
         <v/>
       </c>
       <c r="J21" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K21">
         <f>VLOOKUP(A21,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -9986,26 +9964,23 @@
       <c r="C22" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H22" s="22" t="str">
         <f>VLOOKUP(A22,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I22" s="24" t="str">
         <f>IF(OR(COUNTIF(D22:G22,"X")=0,COUNTIF(D22:G22,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K22">
         <f>VLOOKUP(A22,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>4.8259999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -10029,7 +10004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -10048,15 +10023,12 @@
         <f>IF(OR(COUNTIF(D24:G24,"X")=0,COUNTIF(D24:G24,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J24" s="13" t="s">
-        <v>429</v>
-      </c>
       <c r="K24">
         <f>VLOOKUP(A24,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>7.84</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -10078,9 +10050,6 @@
         <f>IF(OR(COUNTIF(D25:G25,"X")=0,COUNTIF(D25:G25,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J25" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K25">
         <f>VLOOKUP(A25,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1712.1492270000001</v>
@@ -10097,16 +10066,19 @@
       <c r="C26" t="s">
         <v>100</v>
       </c>
+      <c r="D26" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H26" s="22" t="str">
         <f>VLOOKUP(A26,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I26" s="24" t="str">
         <f>IF(OR(COUNTIF(D26:G26,"X")=0,COUNTIF(D26:G26,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J26" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K26">
         <f>VLOOKUP(A26,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10124,7 +10096,7 @@
       <c r="C27" t="s">
         <v>168</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="D27" s="22" t="s">
         <v>180</v>
       </c>
       <c r="H27" s="22" t="str">
@@ -10136,7 +10108,7 @@
         <v/>
       </c>
       <c r="J27" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K27">
         <f>VLOOKUP(A27,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10154,16 +10126,14 @@
       <c r="C28" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="29" t="s">
-        <v>180</v>
-      </c>
+      <c r="E28" s="29"/>
       <c r="H28" s="22" t="str">
         <f>VLOOKUP(A28,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I28" s="24" t="str">
         <f>IF(OR(COUNTIF(D28:G28,"X")=0,COUNTIF(D28:G28,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J28" s="13" t="s">
         <v>431</v>
@@ -10173,7 +10143,7 @@
         <v>4.3494993800000001</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -10197,7 +10167,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -10208,13 +10178,16 @@
       <c r="C30" t="s">
         <v>150</v>
       </c>
+      <c r="D30" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H30" s="22" t="str">
         <f>VLOOKUP(A30,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I30" s="24" t="str">
         <f>IF(OR(COUNTIF(D30:G30,"X")=0,COUNTIF(D30:G30,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J30" s="13" t="s">
         <v>429</v>
@@ -10224,7 +10197,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -10259,26 +10232,23 @@
       <c r="C32" t="s">
         <v>141</v>
       </c>
-      <c r="E32" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H32" s="22" t="str">
         <f>VLOOKUP(A32,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I32" s="24" t="str">
         <f>IF(OR(COUNTIF(D32:G32,"X")=0,COUNTIF(D32:G32,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K32">
         <f>VLOOKUP(A32,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>8.3547796870000006</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -10301,14 +10271,14 @@
         <v/>
       </c>
       <c r="J33" s="13" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K33">
         <f>VLOOKUP(A33,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>3.5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -10332,7 +10302,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -10343,26 +10313,23 @@
       <c r="C35" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H35" s="22" t="str">
         <f>VLOOKUP(A35,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I35" s="24" t="str">
         <f>IF(OR(COUNTIF(D35:G35,"X")=0,COUNTIF(D35:G35,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K35">
         <f>VLOOKUP(A35,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>8.8772132989999992</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -10386,7 +10353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -10405,15 +10372,12 @@
         <f>IF(OR(COUNTIF(D37:G37,"X")=0,COUNTIF(D37:G37,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J37" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K37">
         <f>VLOOKUP(A37,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>30.058387249999999</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -10424,19 +10388,16 @@
       <c r="C38" t="s">
         <v>176</v>
       </c>
-      <c r="E38" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H38" s="22" t="str">
         <f>VLOOKUP(A38,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I38" s="24" t="str">
         <f>IF(OR(COUNTIF(D38:G38,"X")=0,COUNTIF(D38:G38,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K38">
         <f>VLOOKUP(A38,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10454,7 +10415,7 @@
       <c r="C39" t="s">
         <v>172</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="D39" s="22" t="s">
         <v>180</v>
       </c>
       <c r="H39" s="22" t="str">
@@ -10466,14 +10427,14 @@
         <v/>
       </c>
       <c r="J39" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K39">
         <f>VLOOKUP(A39,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -10484,26 +10445,24 @@
       <c r="C40" t="s">
         <v>173</v>
       </c>
-      <c r="E40" s="29" t="s">
-        <v>180</v>
-      </c>
+      <c r="E40" s="29"/>
       <c r="H40" s="22" t="str">
         <f>VLOOKUP(A40,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I40" s="24" t="str">
         <f>IF(OR(COUNTIF(D40:G40,"X")=0,COUNTIF(D40:G40,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K40">
         <f>VLOOKUP(A40,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -10514,19 +10473,16 @@
       <c r="C41" t="s">
         <v>107</v>
       </c>
-      <c r="E41" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H41" s="22" t="str">
         <f>VLOOKUP(A41,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I41" s="24" t="str">
         <f>IF(OR(COUNTIF(D41:G41,"X")=0,COUNTIF(D41:G41,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K41">
         <f>VLOOKUP(A41,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10544,13 +10500,16 @@
       <c r="C42" t="s">
         <v>130</v>
       </c>
+      <c r="D42" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H42" s="22" t="str">
         <f>VLOOKUP(A42,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I42" s="24" t="str">
         <f>IF(OR(COUNTIF(D42:G42,"X")=0,COUNTIF(D42:G42,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J42" s="13" t="s">
         <v>431</v>
@@ -10571,9 +10530,6 @@
       <c r="C43" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="G43" s="24" t="s">
         <v>180</v>
       </c>
@@ -10604,16 +10560,14 @@
       <c r="C44" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="29" t="s">
-        <v>180</v>
-      </c>
+      <c r="E44" s="29"/>
       <c r="H44" s="22" t="str">
         <f>VLOOKUP(A44,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I44" s="24" t="str">
         <f>IF(OR(COUNTIF(D44:G44,"X")=0,COUNTIF(D44:G44,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J44" s="13" t="s">
         <v>431</v>
@@ -10623,7 +10577,7 @@
         <v>2.6026244799999998</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -10647,7 +10601,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -10658,7 +10612,7 @@
       <c r="C46" t="s">
         <v>123</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="D46" s="22" t="s">
         <v>180</v>
       </c>
       <c r="H46" s="22" t="str">
@@ -10670,7 +10624,7 @@
         <v/>
       </c>
       <c r="J46" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K46">
         <f>VLOOKUP(A46,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10700,14 +10654,14 @@
         <v/>
       </c>
       <c r="J47" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K47">
         <f>VLOOKUP(A47,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.79</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -10731,14 +10685,14 @@
         <v/>
       </c>
       <c r="J48" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K48">
         <f>VLOOKUP(A48,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>15.580161759999999</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -10749,7 +10703,7 @@
       <c r="C49" t="s">
         <v>156</v>
       </c>
-      <c r="G49" s="24" t="s">
+      <c r="E49" s="23" t="s">
         <v>180</v>
       </c>
       <c r="H49" s="22" t="str">
@@ -10761,7 +10715,7 @@
         <v/>
       </c>
       <c r="J49" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K49">
         <f>VLOOKUP(A49,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10788,14 +10742,14 @@
         <v>X</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="K50">
         <f>VLOOKUP(A50,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.2528512570000001</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -10806,23 +10760,23 @@
       <c r="C51" t="s">
         <v>136</v>
       </c>
+      <c r="D51" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H51" s="22" t="str">
         <f>VLOOKUP(A51,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I51" s="24" t="str">
         <f>IF(OR(COUNTIF(D51:G51,"X")=0,COUNTIF(D51:G51,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="J51" s="13" t="s">
-        <v>431</v>
+        <v/>
       </c>
       <c r="K51">
         <f>VLOOKUP(A51,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.45343570100000002</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -10845,14 +10799,14 @@
         <v/>
       </c>
       <c r="J52" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K52">
         <f>VLOOKUP(A52,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.34674987200000001</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -10863,23 +10817,23 @@
       <c r="C53" t="s">
         <v>139</v>
       </c>
+      <c r="D53" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H53" s="22" t="str">
         <f>VLOOKUP(A53,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I53" s="24" t="str">
         <f>IF(OR(COUNTIF(D53:G53,"X")=0,COUNTIF(D53:G53,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="J53" s="13" t="s">
-        <v>431</v>
+        <v/>
       </c>
       <c r="K53">
         <f>VLOOKUP(A53,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>26.620192639999999</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -10903,7 +10857,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -10922,15 +10876,12 @@
         <f>IF(OR(COUNTIF(D55:G55,"X")=0,COUNTIF(D55:G55,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J55" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K55">
         <f>VLOOKUP(A55,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>5.6287183719999998</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -10941,23 +10892,26 @@
       <c r="C56" t="s">
         <v>174</v>
       </c>
+      <c r="E56" s="23" t="s">
+        <v>180</v>
+      </c>
       <c r="H56" s="22" t="str">
         <f>VLOOKUP(A56,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I56" s="24" t="str">
         <f>IF(OR(COUNTIF(D56:G56,"X")=0,COUNTIF(D56:G56,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J56" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K56">
         <f>VLOOKUP(A56,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -10981,7 +10935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -11005,7 +10959,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -11028,14 +10982,14 @@
         <v/>
       </c>
       <c r="J59" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K59">
         <f>VLOOKUP(A59,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>4.0453719340000003</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -11059,7 +11013,7 @@
         <v>9.1646354429999999</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -11070,7 +11024,7 @@
       <c r="C61" t="s">
         <v>159</v>
       </c>
-      <c r="G61" s="24" t="s">
+      <c r="D61" s="22" t="s">
         <v>180</v>
       </c>
       <c r="H61" s="22" t="str">
@@ -11089,7 +11043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>30</v>
       </c>
@@ -11100,26 +11054,20 @@
       <c r="C62" t="s">
         <v>118</v>
       </c>
-      <c r="E62" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H62" s="22" t="str">
         <f>VLOOKUP(A62,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I62" s="24" t="str">
         <f>IF(OR(COUNTIF(D62:G62,"X")=0,COUNTIF(D62:G62,"B")&lt;&gt;0),"X","")</f>
-        <v/>
-      </c>
-      <c r="J62" s="13" t="s">
-        <v>431</v>
+        <v>X</v>
       </c>
       <c r="K62">
         <f>VLOOKUP(A62,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>11.47346999</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -11138,12 +11086,15 @@
         <f>IF(OR(COUNTIF(D63:G63,"X")=0,COUNTIF(D63:G63,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
+      <c r="J63" s="13" t="s">
+        <v>430</v>
+      </c>
       <c r="K63">
         <f>VLOOKUP(A63,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -11167,7 +11118,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -11178,16 +11129,19 @@
       <c r="C65" t="s">
         <v>135</v>
       </c>
+      <c r="D65" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H65" s="22" t="str">
         <f>VLOOKUP(A65,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I65" s="24" t="str">
         <f>IF(OR(COUNTIF(D65:G65,"X")=0,COUNTIF(D65:G65,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J65" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K65">
         <f>VLOOKUP(A65,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11247,14 +11201,14 @@
         <v/>
       </c>
       <c r="J67" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K67">
         <f>VLOOKUP(A67,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.62</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>54</v>
       </c>
@@ -11273,15 +11227,12 @@
         <f>IF(OR(COUNTIF(D68:G68,"X")=0,COUNTIF(D68:G68,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J68" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K68">
         <f>VLOOKUP(A68,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>3.17</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -11308,7 +11259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -11328,7 +11279,7 @@
         <v>X</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K70">
         <f>VLOOKUP(A70,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11346,13 +11297,16 @@
       <c r="C71" t="s">
         <v>113</v>
       </c>
+      <c r="D71" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H71" s="22" t="str">
         <f>VLOOKUP(A71,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I71" s="24" t="str">
         <f>IF(OR(COUNTIF(D71:G71,"X")=0,COUNTIF(D71:G71,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J71" s="13" t="s">
         <v>431</v>
@@ -11362,7 +11316,7 @@
         <v>2.8553917279999999</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -11373,7 +11327,7 @@
       <c r="C72" t="s">
         <v>160</v>
       </c>
-      <c r="G72" s="24" t="s">
+      <c r="D72" s="22" t="s">
         <v>180</v>
       </c>
       <c r="H72" s="22" t="str">
@@ -11385,7 +11339,7 @@
         <v/>
       </c>
       <c r="J72" s="13" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="K72">
         <f>VLOOKUP(A72,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11403,16 +11357,13 @@
       <c r="C73" t="s">
         <v>115</v>
       </c>
-      <c r="E73" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H73" s="22" t="str">
         <f>VLOOKUP(A73,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I73" s="24" t="str">
         <f>IF(OR(COUNTIF(D73:G73,"X")=0,COUNTIF(D73:G73,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J73" s="13" t="s">
         <v>431</v>
@@ -11422,7 +11373,7 @@
         <v>4.5705284319999997</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -11476,7 +11427,7 @@
         <v>10.94402988</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>44</v>
       </c>
@@ -11499,14 +11450,14 @@
         <v/>
       </c>
       <c r="J76" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K76">
         <f>VLOOKUP(A76,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>25.449904530000001</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -11529,7 +11480,7 @@
         <v/>
       </c>
       <c r="J77" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K77">
         <f>VLOOKUP(A77,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11547,9 +11498,6 @@
       <c r="C78" t="s">
         <v>97</v>
       </c>
-      <c r="D78" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="G78" s="24" t="s">
         <v>180</v>
       </c>
@@ -11569,7 +11517,7 @@
         <v>26.855260869999999</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>38</v>
       </c>
@@ -11592,14 +11540,14 @@
         <v/>
       </c>
       <c r="J79" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K79">
         <f>VLOOKUP(A79,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>5.5777170800000002</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -11629,7 +11577,7 @@
         <v>13.99337553</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>60</v>
       </c>
@@ -11653,7 +11601,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -11676,7 +11624,7 @@
         <v/>
       </c>
       <c r="J82" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K82">
         <f>VLOOKUP(A82,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11713,7 +11661,7 @@
         <v>4.9696735710000004</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -11736,14 +11684,14 @@
         <v/>
       </c>
       <c r="J84" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K84">
         <f>VLOOKUP(A84,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>15.394965300000001</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>51</v>
       </c>
@@ -11766,14 +11714,14 @@
         <v/>
       </c>
       <c r="J85" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K85">
         <f>VLOOKUP(A85,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>15.126177269999999</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -11796,14 +11744,14 @@
         <v/>
       </c>
       <c r="J86" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K86">
         <f>VLOOKUP(A86,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>2.0841953969999998</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -11826,7 +11774,7 @@
         <v/>
       </c>
       <c r="J87" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K87">
         <f>VLOOKUP(A87,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11856,7 +11804,7 @@
         <v/>
       </c>
       <c r="J88" s="13" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K88">
         <f>VLOOKUP(A88,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11865,6 +11813,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K88">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="worse"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:K88">
       <sortCondition ref="C1:C88"/>
     </sortState>
@@ -13487,9 +13440,9 @@
       <c r="C8" t="s">
         <v>93</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="str">
         <f>VLOOKUP(A8,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>0</v>
+        <v>X</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -14258,9 +14211,9 @@
       <c r="C49" t="s">
         <v>156</v>
       </c>
-      <c r="E49" t="str">
+      <c r="E49">
         <f>VLOOKUP(A49,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
@@ -14402,9 +14355,9 @@
       <c r="C61" t="s">
         <v>159</v>
       </c>
-      <c r="E61" t="str">
+      <c r="E61">
         <f>VLOOKUP(A61,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="F61">
         <v>7</v>
@@ -14576,9 +14529,9 @@
       <c r="C72" t="s">
         <v>160</v>
       </c>
-      <c r="E72" t="str">
+      <c r="E72">
         <f>VLOOKUP(A72,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
@@ -14948,19 +14901,19 @@
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D9" si="0">IF(F2="X","H",IF(G2="X","L",IF(H2="X","C","G")))</f>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E2" s="34" t="str">
         <f>IF('Group Condition'!J40="","",'Group Condition'!J40)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F2" s="34">
         <f>'Group Condition'!D40</f>
         <v>0</v>
       </c>
-      <c r="G2" s="34" t="str">
+      <c r="G2" s="34">
         <f>'Group Condition'!E40</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H2" s="34">
         <f>'Group Condition'!G40</f>
@@ -14968,7 +14921,7 @@
       </c>
       <c r="I2" s="34" t="str">
         <f>'Group Condition'!I40</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>423</v>
@@ -14999,7 +14952,7 @@
       </c>
       <c r="E3" s="34" t="str">
         <f>IF('Group Condition'!J3="","",'Group Condition'!J3)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F3" s="34" t="str">
         <f>'Group Condition'!D3</f>
@@ -15036,7 +14989,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E4" s="34" t="str">
         <f>IF('Group Condition'!J4="","",'Group Condition'!J4)</f>
@@ -15046,9 +14999,9 @@
         <f>'Group Condition'!D4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="34" t="str">
+      <c r="G4" s="34">
         <f>'Group Condition'!E4</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H4" s="34">
         <f>'Group Condition'!G4</f>
@@ -15056,7 +15009,7 @@
       </c>
       <c r="I4" s="34" t="str">
         <f>'Group Condition'!I4</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="P4" t="s">
         <v>412</v>
@@ -15078,7 +15031,7 @@
       </c>
       <c r="E5" s="34" t="str">
         <f>IF('Group Condition'!J5="","",'Group Condition'!J5)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F5" s="34">
         <f>'Group Condition'!D5</f>
@@ -15160,7 +15113,7 @@
       </c>
       <c r="E7" s="34" t="str">
         <f>IF('Group Condition'!J33="","",'Group Condition'!J33)</f>
-        <v>invert</v>
+        <v>no change</v>
       </c>
       <c r="F7" s="34">
         <f>'Group Condition'!D33</f>
@@ -15200,23 +15153,23 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>L</v>
+        <v>C</v>
       </c>
       <c r="E8" s="34" t="str">
         <f>IF('Group Condition'!J8="","",'Group Condition'!J8)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F8" s="34">
         <f>'Group Condition'!D8</f>
         <v>0</v>
       </c>
-      <c r="G8" s="34" t="str">
+      <c r="G8" s="34">
         <f>'Group Condition'!E8</f>
-        <v>X</v>
-      </c>
-      <c r="H8" s="34">
+        <v>0</v>
+      </c>
+      <c r="H8" s="34" t="str">
         <f>'Group Condition'!G8</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="I8" s="34" t="str">
         <f>'Group Condition'!I8</f>
@@ -15242,7 +15195,7 @@
       </c>
       <c r="E9" s="34" t="str">
         <f>IF('Group Condition'!J9="","",'Group Condition'!J9)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F9" s="34">
         <f>'Group Condition'!D9</f>
@@ -15283,7 +15236,7 @@
       </c>
       <c r="E10" s="34" t="str">
         <f>IF('Group Condition'!J50="","",'Group Condition'!J50)</f>
-        <v>no change</v>
+        <v>worse</v>
       </c>
       <c r="F10" s="34">
         <f>'Group Condition'!D50</f>
@@ -15320,19 +15273,19 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E11" s="34" t="str">
         <f>IF('Group Condition'!J32="","",'Group Condition'!J32)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F11" s="34">
         <f>'Group Condition'!D32</f>
         <v>0</v>
       </c>
-      <c r="G11" s="34" t="str">
+      <c r="G11" s="34">
         <f>'Group Condition'!E32</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H11" s="34">
         <f>'Group Condition'!G32</f>
@@ -15340,7 +15293,7 @@
       </c>
       <c r="I11" s="34" t="str">
         <f>'Group Condition'!I32</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -15367,7 +15320,7 @@
       </c>
       <c r="E12" s="34" t="str">
         <f>IF('Group Condition'!J12="","",'Group Condition'!J12)</f>
-        <v>invert</v>
+        <v>no change</v>
       </c>
       <c r="F12" s="34">
         <f>'Group Condition'!D12</f>
@@ -15442,15 +15395,15 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="F14" s="34">
         <f>'Group Condition'!D14</f>
         <v>0</v>
       </c>
-      <c r="G14" s="34" t="str">
+      <c r="G14" s="34">
         <f>'Group Condition'!E14</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H14" s="34">
         <f>'Group Condition'!G14</f>
@@ -15458,7 +15411,7 @@
       </c>
       <c r="I14" s="34" t="str">
         <f>'Group Condition'!I14</f>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -15473,15 +15426,15 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E15" s="34" t="str">
         <f>IF('Group Condition'!J65="","",'Group Condition'!J65)</f>
-        <v>worse</v>
-      </c>
-      <c r="F15" s="34">
+        <v>better</v>
+      </c>
+      <c r="F15" s="34" t="str">
         <f>'Group Condition'!D65</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G15" s="34">
         <f>'Group Condition'!E65</f>
@@ -15493,7 +15446,7 @@
       </c>
       <c r="I15" s="34" t="str">
         <f>'Group Condition'!I65</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J15" s="13" t="s">
         <v>411</v>
@@ -15517,19 +15470,19 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E16" s="34" t="str">
         <f>IF('Group Condition'!J15="","",'Group Condition'!J15)</f>
-        <v>better</v>
+        <v>no change</v>
       </c>
       <c r="F16" s="34">
         <f>'Group Condition'!D15</f>
         <v>0</v>
       </c>
-      <c r="G16" s="34" t="str">
+      <c r="G16" s="34">
         <f>'Group Condition'!E15</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H16" s="34">
         <f>'Group Condition'!G15</f>
@@ -15537,7 +15490,7 @@
       </c>
       <c r="I16" s="34" t="str">
         <f>'Group Condition'!I15</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>411</v>
@@ -15597,7 +15550,7 @@
       </c>
       <c r="E18" s="34" t="str">
         <f>IF('Group Condition'!J18="","",'Group Condition'!J18)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F18" s="34" t="str">
         <f>'Group Condition'!D18</f>
@@ -15635,7 +15588,7 @@
       </c>
       <c r="E19" s="34" t="str">
         <f>IF('Group Condition'!J19="","",'Group Condition'!J19)</f>
-        <v>invert</v>
+        <v>no change</v>
       </c>
       <c r="F19" s="34" t="str">
         <f>'Group Condition'!D19</f>
@@ -15666,19 +15619,19 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>H</v>
       </c>
       <c r="E20" s="34" t="str">
         <f>IF('Group Condition'!J20="","",'Group Condition'!J20)</f>
-        <v>worse</v>
-      </c>
-      <c r="F20" s="34">
+        <v>better</v>
+      </c>
+      <c r="F20" s="34" t="str">
         <f>'Group Condition'!D20</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="34" t="str">
+        <v>X</v>
+      </c>
+      <c r="G20" s="34">
         <f>'Group Condition'!E20</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H20" s="34">
         <f>'Group Condition'!G20</f>
@@ -15711,7 +15664,7 @@
       </c>
       <c r="E21" s="34" t="str">
         <f>IF('Group Condition'!J21="","",'Group Condition'!J21)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F21" s="34">
         <f>'Group Condition'!D21</f>
@@ -15752,7 +15705,7 @@
       </c>
       <c r="E22" s="34" t="str">
         <f>IF('Group Condition'!J11="","",'Group Condition'!J11)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F22" s="34" t="str">
         <f>'Group Condition'!D11</f>
@@ -15876,7 +15829,7 @@
       </c>
       <c r="E25" s="34" t="str">
         <f>IF('Group Condition'!J25="","",'Group Condition'!J25)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F25" s="34" t="str">
         <f>'Group Condition'!D25</f>
@@ -15917,7 +15870,7 @@
       </c>
       <c r="E26" s="34" t="str">
         <f>IF('Group Condition'!J10="","",'Group Condition'!J10)</f>
-        <v>better</v>
+        <v>no change</v>
       </c>
       <c r="F26" s="34">
         <f>'Group Condition'!D10</f>
@@ -15960,19 +15913,19 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>H</v>
       </c>
       <c r="E27" s="34" t="str">
         <f>IF('Group Condition'!J27="","",'Group Condition'!J27)</f>
-        <v>better</v>
-      </c>
-      <c r="F27" s="34">
+        <v>worse</v>
+      </c>
+      <c r="F27" s="34" t="str">
         <f>'Group Condition'!D27</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="34" t="str">
+        <v>X</v>
+      </c>
+      <c r="G27" s="34">
         <f>'Group Condition'!E27</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H27" s="34">
         <f>'Group Condition'!G27</f>
@@ -16005,7 +15958,7 @@
       </c>
       <c r="E28" s="34" t="str">
         <f>IF('Group Condition'!J24="","",'Group Condition'!J24)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F28" s="34">
         <f>'Group Condition'!D24</f>
@@ -16045,15 +15998,15 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E29" s="34" t="str">
         <f>IF('Group Condition'!J30="","",'Group Condition'!J30)</f>
         <v>better</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="34" t="str">
         <f>'Group Condition'!D30</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G29" s="34">
         <f>'Group Condition'!E30</f>
@@ -16065,7 +16018,7 @@
       </c>
       <c r="I29" s="34" t="str">
         <f>'Group Condition'!I30</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="L29" s="13" t="s">
         <v>423</v>
@@ -16089,7 +16042,7 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E30" s="34" t="str">
         <f>IF('Group Condition'!J44="","",'Group Condition'!J44)</f>
@@ -16099,9 +16052,9 @@
         <f>'Group Condition'!D44</f>
         <v>0</v>
       </c>
-      <c r="G30" s="34" t="str">
+      <c r="G30" s="34">
         <f>'Group Condition'!E44</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H30" s="34">
         <f>'Group Condition'!G44</f>
@@ -16109,7 +16062,7 @@
       </c>
       <c r="I30" s="34" t="str">
         <f>'Group Condition'!I44</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J30"/>
       <c r="K30"/>
@@ -16170,15 +16123,15 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="1"/>
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E32" s="34" t="str">
         <f>IF('Group Condition'!J42="","",'Group Condition'!J42)</f>
         <v>worse</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="34" t="str">
         <f>'Group Condition'!D42</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G32" s="34">
         <f>'Group Condition'!E42</f>
@@ -16190,7 +16143,7 @@
       </c>
       <c r="I32" s="34" t="str">
         <f>'Group Condition'!I42</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J32" s="13" t="s">
         <v>410</v>
@@ -16221,7 +16174,7 @@
       </c>
       <c r="E33" s="34" t="str">
         <f>IF('Group Condition'!J16="","",'Group Condition'!J16)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F33" s="34">
         <f>'Group Condition'!D16</f>
@@ -16299,19 +16252,19 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E35" s="34" t="str">
         <f>IF('Group Condition'!J35="","",'Group Condition'!J35)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F35" s="34">
         <f>'Group Condition'!D35</f>
         <v>0</v>
       </c>
-      <c r="G35" s="34" t="str">
+      <c r="G35" s="34">
         <f>'Group Condition'!E35</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H35" s="34">
         <f>'Group Condition'!G35</f>
@@ -16319,7 +16272,7 @@
       </c>
       <c r="I35" s="34" t="str">
         <f>'Group Condition'!I35</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J35"/>
       <c r="K35"/>
@@ -16388,7 +16341,7 @@
       </c>
       <c r="E37" s="34" t="str">
         <f>IF('Group Condition'!J2="","",'Group Condition'!J2)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F37" s="34">
         <f>'Group Condition'!D2</f>
@@ -16428,19 +16381,19 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E38" s="34" t="str">
         <f>IF('Group Condition'!J38="","",'Group Condition'!J38)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F38" s="34">
         <f>'Group Condition'!D38</f>
         <v>0</v>
       </c>
-      <c r="G38" s="34" t="str">
+      <c r="G38" s="34">
         <f>'Group Condition'!E38</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H38" s="34">
         <f>'Group Condition'!G38</f>
@@ -16448,7 +16401,7 @@
       </c>
       <c r="I38" s="34" t="str">
         <f>'Group Condition'!I38</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J38"/>
       <c r="K38"/>
@@ -16469,19 +16422,19 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>H</v>
       </c>
       <c r="E39" s="34" t="str">
         <f>IF('Group Condition'!J39="","",'Group Condition'!J39)</f>
-        <v>better</v>
-      </c>
-      <c r="F39" s="34">
+        <v>worse</v>
+      </c>
+      <c r="F39" s="34" t="str">
         <f>'Group Condition'!D39</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="34" t="str">
+        <v>X</v>
+      </c>
+      <c r="G39" s="34">
         <f>'Group Condition'!E39</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H39" s="34">
         <f>'Group Condition'!G39</f>
@@ -16510,15 +16463,15 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="F40" s="34">
         <f>'Group Condition'!D28</f>
         <v>0</v>
       </c>
-      <c r="G40" s="34" t="str">
+      <c r="G40" s="34">
         <f>'Group Condition'!E28</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H40" s="34">
         <f>'Group Condition'!G28</f>
@@ -16526,7 +16479,7 @@
       </c>
       <c r="I40" s="34" t="str">
         <f>'Group Condition'!I28</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J40"/>
       <c r="K40"/>
@@ -16547,19 +16500,19 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E41" s="34" t="str">
         <f>IF('Group Condition'!J41="","",'Group Condition'!J41)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F41" s="34">
         <f>'Group Condition'!D41</f>
         <v>0</v>
       </c>
-      <c r="G41" s="34" t="str">
+      <c r="G41" s="34">
         <f>'Group Condition'!E41</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H41" s="34">
         <f>'Group Condition'!G41</f>
@@ -16567,7 +16520,7 @@
       </c>
       <c r="I41" s="34" t="str">
         <f>'Group Condition'!I41</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J41" s="13" t="s">
         <v>410</v>
@@ -16598,7 +16551,7 @@
       </c>
       <c r="E42" s="34" t="str">
         <f>IF('Group Condition'!J67="","",'Group Condition'!J67)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F42" s="34">
         <f>'Group Condition'!D67</f>
@@ -16639,15 +16592,15 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="2"/>
-        <v>H</v>
+        <v>C</v>
       </c>
       <c r="E43" s="34" t="str">
         <f>IF('Group Condition'!J43="","",'Group Condition'!J43)</f>
         <v>worse</v>
       </c>
-      <c r="F43" s="34" t="str">
+      <c r="F43" s="34">
         <f>'Group Condition'!D43</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G43" s="34">
         <f>'Group Condition'!E43</f>
@@ -16680,15 +16633,15 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" si="2"/>
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E44" s="34" t="str">
         <f>IF('Group Condition'!J51="","",'Group Condition'!J51)</f>
-        <v>worse</v>
-      </c>
-      <c r="F44" s="34">
+        <v/>
+      </c>
+      <c r="F44" s="34" t="str">
         <f>'Group Condition'!D51</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G44" s="34">
         <f>'Group Condition'!E51</f>
@@ -16700,7 +16653,7 @@
       </c>
       <c r="I44" s="34" t="str">
         <f>'Group Condition'!I51</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K44"/>
       <c r="L44"/>
@@ -16723,7 +16676,7 @@
       </c>
       <c r="E45" s="34" t="str">
         <f>IF('Group Condition'!J37="","",'Group Condition'!J37)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F45" s="34">
         <f>'Group Condition'!D37</f>
@@ -16757,19 +16710,19 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v>H</v>
       </c>
       <c r="E46" s="34" t="str">
         <f>IF('Group Condition'!J46="","",'Group Condition'!J46)</f>
-        <v>worse</v>
-      </c>
-      <c r="F46" s="34">
+        <v>no change</v>
+      </c>
+      <c r="F46" s="34" t="str">
         <f>'Group Condition'!D46</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="34" t="str">
+        <v>X</v>
+      </c>
+      <c r="G46" s="34">
         <f>'Group Condition'!E46</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H46" s="34">
         <f>'Group Condition'!G46</f>
@@ -16802,7 +16755,7 @@
       </c>
       <c r="E47" s="34" t="str">
         <f>IF('Group Condition'!J47="","",'Group Condition'!J47)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F47" s="34">
         <f>'Group Condition'!D47</f>
@@ -16843,7 +16796,7 @@
       </c>
       <c r="E48" s="34" t="str">
         <f>IF('Group Condition'!J48="","",'Group Condition'!J48)</f>
-        <v>worse</v>
+        <v>no change</v>
       </c>
       <c r="F48" s="34" t="str">
         <f>'Group Condition'!D48</f>
@@ -16874,23 +16827,23 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" si="2"/>
-        <v>C</v>
+        <v>L</v>
       </c>
       <c r="E49" s="34" t="str">
         <f>IF('Group Condition'!J49="","",'Group Condition'!J49)</f>
-        <v>better</v>
+        <v>no change</v>
       </c>
       <c r="F49" s="34">
         <f>'Group Condition'!D49</f>
         <v>0</v>
       </c>
-      <c r="G49" s="34">
+      <c r="G49" s="34" t="str">
         <f>'Group Condition'!E49</f>
-        <v>0</v>
-      </c>
-      <c r="H49" s="34" t="str">
+        <v>X</v>
+      </c>
+      <c r="H49" s="34">
         <f>'Group Condition'!G49</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="I49" s="34" t="str">
         <f>'Group Condition'!I49</f>
@@ -17007,7 +16960,7 @@
       </c>
       <c r="E52" s="34" t="str">
         <f>IF('Group Condition'!J52="","",'Group Condition'!J52)</f>
-        <v>worse</v>
+        <v>no change</v>
       </c>
       <c r="F52" s="34" t="str">
         <f>'Group Condition'!D52</f>
@@ -17044,15 +16997,15 @@
       </c>
       <c r="D53" t="str">
         <f t="shared" si="2"/>
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E53" s="34" t="str">
         <f>IF('Group Condition'!J53="","",'Group Condition'!J53)</f>
-        <v>worse</v>
-      </c>
-      <c r="F53" s="34">
+        <v/>
+      </c>
+      <c r="F53" s="34" t="str">
         <f>'Group Condition'!D53</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G53" s="34">
         <f>'Group Condition'!E53</f>
@@ -17064,7 +17017,7 @@
       </c>
       <c r="I53" s="34" t="str">
         <f>'Group Condition'!I53</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J53"/>
       <c r="K53"/>
@@ -17128,7 +17081,7 @@
       </c>
       <c r="E55" s="34" t="str">
         <f>IF('Group Condition'!J55="","",'Group Condition'!J55)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F55" s="34">
         <f>'Group Condition'!D55</f>
@@ -17162,19 +17115,19 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" si="2"/>
-        <v>G</v>
+        <v>L</v>
       </c>
       <c r="E56" s="34" t="str">
         <f>IF('Group Condition'!J56="","",'Group Condition'!J56)</f>
-        <v>worse</v>
+        <v>no change</v>
       </c>
       <c r="F56" s="34">
         <f>'Group Condition'!D56</f>
         <v>0</v>
       </c>
-      <c r="G56" s="34">
+      <c r="G56" s="34" t="str">
         <f>'Group Condition'!E56</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="H56" s="34">
         <f>'Group Condition'!G56</f>
@@ -17182,7 +17135,7 @@
       </c>
       <c r="I56" s="34" t="str">
         <f>'Group Condition'!I56</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J56"/>
       <c r="K56"/>
@@ -17292,7 +17245,7 @@
       </c>
       <c r="E59" s="34" t="str">
         <f>IF('Group Condition'!J59="","",'Group Condition'!J59)</f>
-        <v>worse</v>
+        <v>no change</v>
       </c>
       <c r="F59" s="34" t="str">
         <f>'Group Condition'!D59</f>
@@ -17370,19 +17323,19 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E61" s="34" t="str">
         <f>IF('Group Condition'!J22="","",'Group Condition'!J22)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F61" s="34">
         <f>'Group Condition'!D22</f>
         <v>0</v>
       </c>
-      <c r="G61" s="34" t="str">
+      <c r="G61" s="34">
         <f>'Group Condition'!E22</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H61" s="34">
         <f>'Group Condition'!G22</f>
@@ -17390,7 +17343,7 @@
       </c>
       <c r="I61" s="34" t="str">
         <f>'Group Condition'!I22</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J61"/>
       <c r="K61"/>
@@ -17411,19 +17364,19 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E62" s="34" t="str">
         <f>IF('Group Condition'!J62="","",'Group Condition'!J62)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F62" s="34">
         <f>'Group Condition'!D62</f>
         <v>0</v>
       </c>
-      <c r="G62" s="34" t="str">
+      <c r="G62" s="34">
         <f>'Group Condition'!E62</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H62" s="34">
         <f>'Group Condition'!G62</f>
@@ -17431,7 +17384,7 @@
       </c>
       <c r="I62" s="34" t="str">
         <f>'Group Condition'!I62</f>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
@@ -17450,7 +17403,7 @@
       </c>
       <c r="E63" s="34" t="str">
         <f>IF('Group Condition'!J63="","",'Group Condition'!J63)</f>
-        <v/>
+        <v>no change</v>
       </c>
       <c r="F63" s="34">
         <f>'Group Condition'!D63</f>
@@ -17484,23 +17437,23 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="2"/>
-        <v>C</v>
+        <v>H</v>
       </c>
       <c r="E64" s="34" t="str">
         <f>IF('Group Condition'!J61="","",'Group Condition'!J61)</f>
         <v>better</v>
       </c>
-      <c r="F64" s="34">
+      <c r="F64" s="34" t="str">
         <f>'Group Condition'!D61</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G64" s="34">
         <f>'Group Condition'!E61</f>
         <v>0</v>
       </c>
-      <c r="H64" s="34" t="str">
+      <c r="H64" s="34">
         <f>'Group Condition'!G61</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="I64" s="34" t="str">
         <f>'Group Condition'!I61</f>
@@ -17525,15 +17478,15 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="2"/>
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E65" s="34" t="str">
         <f>IF('Group Condition'!J71="","",'Group Condition'!J71)</f>
         <v>worse</v>
       </c>
-      <c r="F65" s="34">
+      <c r="F65" s="34" t="str">
         <f>'Group Condition'!D71</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G65" s="34">
         <f>'Group Condition'!E71</f>
@@ -17545,7 +17498,7 @@
       </c>
       <c r="I65" s="34" t="str">
         <f>'Group Condition'!I71</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="L65" s="13" t="s">
         <v>410</v>
@@ -17609,23 +17562,23 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" si="2"/>
-        <v>C</v>
+        <v>H</v>
       </c>
       <c r="E67" s="34" t="str">
         <f>IF('Group Condition'!J72="","",'Group Condition'!J72)</f>
-        <v>invert</v>
-      </c>
-      <c r="F67" s="34">
+        <v>better</v>
+      </c>
+      <c r="F67" s="34" t="str">
         <f>'Group Condition'!D72</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G67" s="34">
         <f>'Group Condition'!E72</f>
         <v>0</v>
       </c>
-      <c r="H67" s="34" t="str">
+      <c r="H67" s="34">
         <f>'Group Condition'!G72</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="I67" s="34" t="str">
         <f>'Group Condition'!I72</f>
@@ -17658,7 +17611,7 @@
       </c>
       <c r="E68" s="34" t="str">
         <f>IF('Group Condition'!J68="","",'Group Condition'!J68)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F68" s="34">
         <f>'Group Condition'!D68</f>
@@ -17743,7 +17696,7 @@
       </c>
       <c r="E70" s="34" t="str">
         <f>IF('Group Condition'!J70="","",'Group Condition'!J70)</f>
-        <v>worse</v>
+        <v>no change</v>
       </c>
       <c r="F70" s="34">
         <f>'Group Condition'!D70</f>
@@ -17784,7 +17737,7 @@
       </c>
       <c r="E71" s="34" t="str">
         <f>IF('Group Condition'!J77="","",'Group Condition'!J77)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F71" s="34" t="str">
         <f>'Group Condition'!D77</f>
@@ -17821,11 +17774,11 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="2"/>
-        <v>G</v>
-      </c>
-      <c r="F72" s="34">
+        <v>H</v>
+      </c>
+      <c r="F72" s="34" t="str">
         <f>'Group Condition'!D26</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G72" s="34">
         <f>'Group Condition'!E26</f>
@@ -17837,7 +17790,7 @@
       </c>
       <c r="I72" s="34" t="str">
         <f>'Group Condition'!I26</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J72" s="13" t="s">
         <v>410</v>
@@ -17895,15 +17848,15 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" ref="D74:D84" si="3">IF(F74="X","H",IF(G74="X","L",IF(H74="X","C","G")))</f>
-        <v>H</v>
+        <v>C</v>
       </c>
       <c r="E74" s="34" t="str">
         <f>IF('Group Condition'!J78="","",'Group Condition'!J78)</f>
         <v>worse</v>
       </c>
-      <c r="F74" s="34" t="str">
+      <c r="F74" s="34">
         <f>'Group Condition'!D78</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G74" s="34">
         <f>'Group Condition'!E78</f>
@@ -18058,7 +18011,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="3"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E78" s="34" t="str">
         <f>IF('Group Condition'!J73="","",'Group Condition'!J73)</f>
@@ -18068,9 +18021,9 @@
         <f>'Group Condition'!D73</f>
         <v>0</v>
       </c>
-      <c r="G78" s="34" t="str">
+      <c r="G78" s="34">
         <f>'Group Condition'!E73</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H78" s="34">
         <f>'Group Condition'!G73</f>
@@ -18078,7 +18031,7 @@
       </c>
       <c r="I78" s="34" t="str">
         <f>'Group Condition'!I73</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M78" s="13" t="s">
         <v>411</v>
@@ -18103,7 +18056,7 @@
       </c>
       <c r="E79" s="34" t="str">
         <f>IF('Group Condition'!J79="","",'Group Condition'!J79)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F79" s="34" t="str">
         <f>'Group Condition'!D79</f>
@@ -18138,7 +18091,7 @@
       </c>
       <c r="E80" s="34" t="str">
         <f>IF('Group Condition'!J82="","",'Group Condition'!J82)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F80" s="34" t="str">
         <f>'Group Condition'!D82</f>
@@ -18173,7 +18126,7 @@
       </c>
       <c r="E81" s="34" t="str">
         <f>IF('Group Condition'!J86="","",'Group Condition'!J86)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F81" s="34" t="str">
         <f>'Group Condition'!D86</f>
@@ -18290,7 +18243,7 @@
       </c>
       <c r="E84" s="34" t="str">
         <f>IF('Group Condition'!J84="","",'Group Condition'!J84)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F84" s="34" t="str">
         <f>'Group Condition'!D84</f>
@@ -18369,7 +18322,7 @@
       </c>
       <c r="E86" s="34" t="str">
         <f>IF('Group Condition'!J85="","",'Group Condition'!J85)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F86" s="34" t="str">
         <f>'Group Condition'!D85</f>
@@ -18410,7 +18363,7 @@
       </c>
       <c r="E87" s="34" t="str">
         <f>IF('Group Condition'!J87="","",'Group Condition'!J87)</f>
-        <v>worse</v>
+        <v>no change</v>
       </c>
       <c r="F87" s="34" t="str">
         <f>'Group Condition'!D87</f>
@@ -18451,7 +18404,7 @@
       </c>
       <c r="E88" s="34" t="str">
         <f>IF('Group Condition'!J88="","",'Group Condition'!J88)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F88" s="34" t="str">
         <f>'Group Condition'!D88</f>
@@ -18581,10 +18534,10 @@
         <v>432</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -18603,7 +18556,7 @@
       </c>
       <c r="E2" s="7" t="str">
         <f>VLOOKUP(A2,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F2" s="6">
         <v>532233758.39999998</v>
@@ -18954,7 +18907,7 @@
       </c>
       <c r="E10" s="7" t="str">
         <f>VLOOKUP(A10,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F10" s="6">
         <v>6500000</v>
@@ -19256,7 +19209,7 @@
       </c>
       <c r="E17" s="7" t="str">
         <f>VLOOKUP(A17,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F17" s="6">
         <v>4986608.142</v>
@@ -19400,7 +19353,7 @@
       </c>
       <c r="E20" s="7" t="str">
         <f>VLOOKUP(A20,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F20" s="6">
         <v>19030174.25</v>
@@ -19548,7 +19501,7 @@
       </c>
       <c r="E23" s="7" t="str">
         <f>VLOOKUP(A23,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F23" s="6">
         <v>4928995.608</v>
@@ -19649,7 +19602,7 @@
       </c>
       <c r="E25" s="7" t="str">
         <f>VLOOKUP(A25,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F25" s="6">
         <v>72230904</v>
@@ -19768,7 +19721,7 @@
       </c>
       <c r="E28" s="7" t="str">
         <f>VLOOKUP(A28,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F28" s="6">
         <v>3521063.9419999998</v>
@@ -20323,7 +20276,7 @@
       </c>
       <c r="E40" s="7" t="str">
         <f>VLOOKUP(A40,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F40" s="6">
         <v>7850000</v>
@@ -20359,7 +20312,7 @@
       </c>
       <c r="E41" s="7" t="str">
         <f>VLOOKUP(A41,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F41" s="6">
         <v>49700000</v>
@@ -20519,7 +20472,7 @@
       </c>
       <c r="E45" s="7" t="str">
         <f>VLOOKUP(A45,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F45" s="6">
         <v>75000</v>
@@ -20557,7 +20510,7 @@
       </c>
       <c r="E46" s="7" t="str">
         <f>VLOOKUP(A46,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F46" s="6">
         <v>110.9</v>
@@ -20662,7 +20615,7 @@
       </c>
       <c r="E49" s="7" t="str">
         <f>VLOOKUP(A49,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F49" s="6">
         <v>4273.9050960000004</v>
@@ -20740,7 +20693,7 @@
       </c>
       <c r="E51" s="7" t="str">
         <f>VLOOKUP(A51,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F51" s="6">
         <v>15150975.09</v>
@@ -20780,7 +20733,7 @@
       </c>
       <c r="E52" s="7" t="str">
         <f>VLOOKUP(A52,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F52" s="6">
         <v>328703</v>
@@ -21090,7 +21043,7 @@
       </c>
       <c r="E60" s="7" t="str">
         <f>VLOOKUP(A60,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F60" s="6">
         <v>197000</v>
@@ -21425,10 +21378,10 @@
         <v>434</v>
       </c>
       <c r="V1" t="s">
+        <v>438</v>
+      </c>
+      <c r="W1" t="s">
         <v>439</v>
-      </c>
-      <c r="W1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -21450,7 +21403,7 @@
       </c>
       <c r="F2" s="7" t="str">
         <f>VLOOKUP(A2,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K2">
         <f>VLOOKUP(A2,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -21792,7 +21745,7 @@
       </c>
       <c r="F10" s="7" t="str">
         <f>VLOOKUP(A10,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K10">
         <f>VLOOKUP(A10,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22154,7 +22107,7 @@
       </c>
       <c r="F17" s="7" t="str">
         <f>VLOOKUP(A17,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K17">
         <f>VLOOKUP(A17,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22292,7 +22245,7 @@
       </c>
       <c r="F20" s="7" t="str">
         <f>VLOOKUP(A20,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K20">
         <f>VLOOKUP(A20,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22440,7 +22393,7 @@
       </c>
       <c r="F23" s="7" t="str">
         <f>VLOOKUP(A23,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K23">
         <f>VLOOKUP(A23,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22540,7 +22493,7 @@
       </c>
       <c r="F25" s="7" t="str">
         <f>VLOOKUP(A25,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K25">
         <f>VLOOKUP(A25,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22666,7 +22619,7 @@
       </c>
       <c r="F28" s="7" t="str">
         <f>VLOOKUP(A28,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K28">
         <f>VLOOKUP(A28,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23170,7 +23123,7 @@
       </c>
       <c r="F40" s="7" t="str">
         <f>VLOOKUP(A40,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K40">
         <f>VLOOKUP(A40,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23212,7 +23165,7 @@
       </c>
       <c r="F41" s="7" t="str">
         <f>VLOOKUP(A41,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K41">
         <f>VLOOKUP(A41,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23380,7 +23333,7 @@
       </c>
       <c r="F45" s="7" t="str">
         <f>VLOOKUP(A45,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K45">
         <f>VLOOKUP(A45,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23422,7 +23375,7 @@
       </c>
       <c r="F46" s="7" t="str">
         <f>VLOOKUP(A46,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K46">
         <f>VLOOKUP(A46,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23548,7 +23501,7 @@
       </c>
       <c r="F49" s="7" t="str">
         <f>VLOOKUP(A49,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K49">
         <f>VLOOKUP(A49,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23632,7 +23585,7 @@
       </c>
       <c r="F51" s="7" t="str">
         <f>VLOOKUP(A51,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K51">
         <f>VLOOKUP(A51,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23680,7 +23633,7 @@
       </c>
       <c r="F52" s="7" t="str">
         <f>VLOOKUP(A52,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K52">
         <f>VLOOKUP(A52,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -24056,7 +24009,7 @@
       </c>
       <c r="F60" s="7" t="str">
         <f>VLOOKUP(A60,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K60">
         <f>VLOOKUP(A60,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -24374,16 +24327,16 @@
         <v>436</v>
       </c>
       <c r="AB1" t="s">
+        <v>440</v>
+      </c>
+      <c r="AC1" t="s">
         <v>441</v>
       </c>
-      <c r="AC1" t="s">
-        <v>442</v>
-      </c>
       <c r="AD1" t="s">
+        <v>443</v>
+      </c>
+      <c r="AE1" t="s">
         <v>444</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -24405,7 +24358,7 @@
       </c>
       <c r="F2" s="7" t="str">
         <f>VLOOKUP(A2,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G2">
         <f>D2*1.25</f>
@@ -24968,7 +24921,7 @@
       </c>
       <c r="F10" s="7" t="str">
         <f>VLOOKUP(A10,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="H10"/>
       <c r="Q10">
@@ -25425,7 +25378,7 @@
       </c>
       <c r="F17" s="7" t="str">
         <f>VLOOKUP(A17,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H17"/>
       <c r="Q17">
@@ -25609,7 +25562,7 @@
       </c>
       <c r="F20" s="7" t="str">
         <f>VLOOKUP(A20,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H20"/>
       <c r="Q20">
@@ -25809,7 +25762,7 @@
       </c>
       <c r="F23" s="7" t="str">
         <f>VLOOKUP(A23,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="H23"/>
       <c r="Q23">
@@ -25930,7 +25883,7 @@
       </c>
       <c r="F25" s="7" t="str">
         <f>VLOOKUP(A25,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H25"/>
       <c r="Q25">
@@ -26081,7 +26034,7 @@
       </c>
       <c r="F28" s="7" t="str">
         <f>VLOOKUP(A28,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H28"/>
       <c r="Q28">
@@ -26960,7 +26913,7 @@
       </c>
       <c r="F40" s="7" t="str">
         <f>VLOOKUP(A40,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="H40"/>
       <c r="Q40">
@@ -27009,7 +26962,7 @@
       </c>
       <c r="F41" s="7" t="str">
         <f>VLOOKUP(A41,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G41">
         <f>D41*0.75</f>
@@ -27258,7 +27211,7 @@
       </c>
       <c r="F45" s="7" t="str">
         <f>VLOOKUP(A45,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="G45">
         <f>D45*1.5</f>
@@ -27326,7 +27279,7 @@
       </c>
       <c r="F46" s="7" t="str">
         <f>VLOOKUP(A46,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="H46"/>
       <c r="M46" s="14">
@@ -27491,7 +27444,7 @@
       </c>
       <c r="F49" s="7" t="str">
         <f>VLOOKUP(A49,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="H49"/>
       <c r="Q49">
@@ -27599,7 +27552,7 @@
       </c>
       <c r="F51" s="7" t="str">
         <f>VLOOKUP(A51,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H51"/>
       <c r="Q51">
@@ -27650,7 +27603,7 @@
       </c>
       <c r="F52" s="7" t="str">
         <f>VLOOKUP(A52,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H52"/>
       <c r="Q52">
@@ -28114,7 +28067,7 @@
       </c>
       <c r="F60" s="7" t="str">
         <f>VLOOKUP(A60,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="G60">
         <f>D60*1.5</f>

</xml_diff>

<commit_message>
ZooTuningRevisit 10 - Dropped mum/C for ZL,ZG,ZM,ZS - Decreased predation on ZL by HER,MEN,MAK - Restored groups too high to RM mum/C - Standardized fish groups C = mum * 0.1
</commit_message>
<xml_diff>
--- a/diagnostics/Obs_Hindcast_Group_Progress.xlsx
+++ b/diagnostics/Obs_Hindcast_Group_Progress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15696" windowHeight="8748" tabRatio="853"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6492" windowHeight="6216" tabRatio="853"/>
   </bookViews>
   <sheets>
     <sheet name="Group Condition" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="446">
   <si>
     <t>Too Low</t>
   </si>
@@ -1341,9 +1341,6 @@
     <t>better</t>
   </si>
   <si>
-    <t>no change</t>
-  </si>
-  <si>
     <t>worse</t>
   </si>
   <si>
@@ -1384,6 +1381,12 @@
   </si>
   <si>
     <t>New_Init_CatchTS_6 mQ2</t>
+  </si>
+  <si>
+    <t>zero?</t>
+  </si>
+  <si>
+    <t>spike</t>
   </si>
 </sst>
 </file>
@@ -9337,7 +9340,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E47" sqref="E47"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9425,16 +9428,13 @@
       <c r="C3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="H3" s="22" t="str">
         <f>VLOOKUP(A3,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I3" s="24" t="str">
         <f>IF(OR(COUNTIF(D3:G3,"X")=0,COUNTIF(D3:G3,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>429</v>
@@ -9463,9 +9463,6 @@
         <f>IF(OR(COUNTIF(D4:G4,"X")=0,COUNTIF(D4:G4,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J4" s="13" t="s">
-        <v>429</v>
-      </c>
       <c r="K4">
         <f>VLOOKUP(A4,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>125.479276</v>
@@ -9514,15 +9511,12 @@
         <f>IF(OR(COUNTIF(D6:G6,"X")=0,COUNTIF(D6:G6,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J6" s="13" t="s">
-        <v>429</v>
-      </c>
       <c r="K6">
         <f>VLOOKUP(A6,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>13.60138179</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9563,10 +9557,10 @@
       <c r="C8" t="s">
         <v>93</v>
       </c>
+      <c r="D8" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="E8" s="29"/>
-      <c r="G8" s="24" t="s">
-        <v>180</v>
-      </c>
       <c r="H8" s="22" t="str">
         <f>VLOOKUP(A8,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
@@ -9576,7 +9570,7 @@
         <v/>
       </c>
       <c r="J8" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K8">
         <f>VLOOKUP(A8,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -9594,19 +9588,17 @@
       <c r="C9" t="s">
         <v>112</v>
       </c>
-      <c r="G9" s="24" t="s">
-        <v>180</v>
-      </c>
+      <c r="E9" s="29"/>
       <c r="H9" s="22" t="str">
         <f>VLOOKUP(A9,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I9" s="24" t="str">
         <f>IF(OR(COUNTIF(D9:G9,"X")=0,COUNTIF(D9:G9,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K9">
         <f>VLOOKUP(A9,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -9624,26 +9616,20 @@
       <c r="C10" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="H10" s="22" t="str">
         <f>VLOOKUP(A10,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I10" s="24" t="str">
         <f>IF(OR(COUNTIF(D10:G10,"X")=0,COUNTIF(D10:G10,"B")&lt;&gt;0),"X","")</f>
-        <v/>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>430</v>
+        <v>X</v>
       </c>
       <c r="K10">
         <f>VLOOKUP(A10,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>2.07701E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -9673,7 +9659,7 @@
         <v>1.88352E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -9696,7 +9682,7 @@
         <v/>
       </c>
       <c r="J12" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K12">
         <f>VLOOKUP(A12,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -9746,9 +9732,6 @@
         <f>IF(OR(COUNTIF(D14:G14,"X")=0,COUNTIF(D14:G14,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K14">
         <f>VLOOKUP(A14,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.41</v>
@@ -9773,9 +9756,6 @@
         <f>IF(OR(COUNTIF(D15:G15,"X")=0,COUNTIF(D15:G15,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K15">
         <f>VLOOKUP(A15,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.22</v>
@@ -9805,7 +9785,7 @@
         <v>6.6672173600000004</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -9828,14 +9808,14 @@
         <v/>
       </c>
       <c r="J17" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K17">
         <f>VLOOKUP(A17,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>36.832345089999997</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -9862,7 +9842,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -9885,9 +9865,6 @@
         <f>IF(OR(COUNTIF(D19:G19,"X")=0,COUNTIF(D19:G19,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J19" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K19">
         <f>VLOOKUP(A19,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>8.2990938990000007</v>
@@ -9904,26 +9881,20 @@
       <c r="C20" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="H20" s="22" t="str">
         <f>VLOOKUP(A20,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I20" s="24" t="str">
         <f>IF(OR(COUNTIF(D20:G20,"X")=0,COUNTIF(D20:G20,"B")&lt;&gt;0),"X","")</f>
-        <v/>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>429</v>
+        <v>X</v>
       </c>
       <c r="K20">
         <f>VLOOKUP(A20,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>72.318494520000002</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -9934,6 +9905,9 @@
       <c r="C21" t="s">
         <v>163</v>
       </c>
+      <c r="D21" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="E21" s="23" t="s">
         <v>180</v>
       </c>
@@ -9946,7 +9920,7 @@
         <v/>
       </c>
       <c r="J21" s="13" t="s">
-        <v>429</v>
+        <v>445</v>
       </c>
       <c r="K21">
         <f>VLOOKUP(A21,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -9972,9 +9946,6 @@
         <f>IF(OR(COUNTIF(D22:G22,"X")=0,COUNTIF(D22:G22,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J22" s="13" t="s">
-        <v>429</v>
-      </c>
       <c r="K22">
         <f>VLOOKUP(A22,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>4.8259999999999996</v>
@@ -10028,7 +9999,7 @@
         <v>7.84</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -10050,6 +10021,9 @@
         <f>IF(OR(COUNTIF(D25:G25,"X")=0,COUNTIF(D25:G25,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
+      <c r="J25" s="13" t="s">
+        <v>429</v>
+      </c>
       <c r="K25">
         <f>VLOOKUP(A25,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1712.1492270000001</v>
@@ -10077,9 +10051,6 @@
         <f>IF(OR(COUNTIF(D26:G26,"X")=0,COUNTIF(D26:G26,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K26">
         <f>VLOOKUP(A26,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>3.9979082419999998</v>
@@ -10096,7 +10067,7 @@
       <c r="C27" t="s">
         <v>168</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="E27" s="23" t="s">
         <v>180</v>
       </c>
       <c r="H27" s="22" t="str">
@@ -10108,14 +10079,14 @@
         <v/>
       </c>
       <c r="J27" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K27">
         <f>VLOOKUP(A27,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.61</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -10135,9 +10106,6 @@
         <f>IF(OR(COUNTIF(D28:G28,"X")=0,COUNTIF(D28:G28,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J28" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K28">
         <f>VLOOKUP(A28,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>4.3494993800000001</v>
@@ -10167,7 +10135,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -10221,7 +10189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -10240,15 +10208,12 @@
         <f>IF(OR(COUNTIF(D32:G32,"X")=0,COUNTIF(D32:G32,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J32" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K32">
         <f>VLOOKUP(A32,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>8.3547796870000006</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -10271,7 +10236,7 @@
         <v/>
       </c>
       <c r="J33" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K33">
         <f>VLOOKUP(A33,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10302,7 +10267,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -10313,16 +10278,19 @@
       <c r="C35" t="s">
         <v>92</v>
       </c>
+      <c r="G35" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="H35" s="22" t="str">
         <f>VLOOKUP(A35,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I35" s="24" t="str">
         <f>IF(OR(COUNTIF(D35:G35,"X")=0,COUNTIF(D35:G35,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J35" s="13" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="K35">
         <f>VLOOKUP(A35,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10397,7 +10365,7 @@
         <v>X</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K38">
         <f>VLOOKUP(A38,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -10415,7 +10383,7 @@
       <c r="C39" t="s">
         <v>172</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="E39" s="23" t="s">
         <v>180</v>
       </c>
       <c r="H39" s="22" t="str">
@@ -10427,14 +10395,14 @@
         <v/>
       </c>
       <c r="J39" s="13" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="K39">
         <f>VLOOKUP(A39,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -10445,24 +10413,23 @@
       <c r="C40" t="s">
         <v>173</v>
       </c>
-      <c r="E40" s="29"/>
+      <c r="E40" s="29" t="s">
+        <v>180</v>
+      </c>
       <c r="H40" s="22" t="str">
         <f>VLOOKUP(A40,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I40" s="24" t="str">
         <f>IF(OR(COUNTIF(D40:G40,"X")=0,COUNTIF(D40:G40,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>429</v>
+        <v/>
       </c>
       <c r="K40">
         <f>VLOOKUP(A40,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -10473,13 +10440,16 @@
       <c r="C41" t="s">
         <v>107</v>
       </c>
+      <c r="D41" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="H41" s="22" t="str">
         <f>VLOOKUP(A41,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I41" s="24" t="str">
         <f>IF(OR(COUNTIF(D41:G41,"X")=0,COUNTIF(D41:G41,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J41" s="13" t="s">
         <v>429</v>
@@ -10512,14 +10482,14 @@
         <v/>
       </c>
       <c r="J42" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K42">
         <f>VLOOKUP(A42,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.844462681</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -10530,26 +10500,20 @@
       <c r="C43" t="s">
         <v>111</v>
       </c>
-      <c r="G43" s="24" t="s">
-        <v>180</v>
-      </c>
       <c r="H43" s="22" t="str">
         <f>VLOOKUP(A43,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I43" s="24" t="str">
         <f>IF(OR(COUNTIF(D43:G43,"X")=0,COUNTIF(D43:G43,"B")&lt;&gt;0),"X","")</f>
-        <v/>
-      </c>
-      <c r="J43" s="13" t="s">
-        <v>431</v>
+        <v>X</v>
       </c>
       <c r="K43">
         <f>VLOOKUP(A43,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.8621823959999999</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -10569,15 +10533,12 @@
         <f>IF(OR(COUNTIF(D44:G44,"X")=0,COUNTIF(D44:G44,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J44" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K44">
         <f>VLOOKUP(A44,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>2.6026244799999998</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -10588,20 +10549,23 @@
       <c r="C45" t="s">
         <v>161</v>
       </c>
+      <c r="E45" s="23" t="s">
+        <v>180</v>
+      </c>
       <c r="H45" s="22" t="str">
         <f>VLOOKUP(A45,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v/>
       </c>
       <c r="I45" s="24" t="str">
         <f>IF(OR(COUNTIF(D45:G45,"X")=0,COUNTIF(D45:G45,"B")&lt;&gt;0),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K45">
         <f>VLOOKUP(A45,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>2.19</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -10623,9 +10587,6 @@
         <f>IF(OR(COUNTIF(D46:G46,"X")=0,COUNTIF(D46:G46,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J46" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K46">
         <f>VLOOKUP(A46,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.3995842030000001</v>
@@ -10654,14 +10615,14 @@
         <v/>
       </c>
       <c r="J47" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K47">
         <f>VLOOKUP(A47,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.79</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -10685,14 +10646,14 @@
         <v/>
       </c>
       <c r="J48" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K48">
         <f>VLOOKUP(A48,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>15.580161759999999</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -10715,14 +10676,14 @@
         <v/>
       </c>
       <c r="J49" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K49">
         <f>VLOOKUP(A49,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.16</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -10741,15 +10702,12 @@
         <f>IF(OR(COUNTIF(D50:G50,"X")=0,COUNTIF(D50:G50,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J50" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K50">
         <f>VLOOKUP(A50,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1.2528512570000001</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -10771,6 +10729,9 @@
         <f>IF(OR(COUNTIF(D51:G51,"X")=0,COUNTIF(D51:G51,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
+      <c r="J51" s="13" t="s">
+        <v>430</v>
+      </c>
       <c r="K51">
         <f>VLOOKUP(A51,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.45343570100000002</v>
@@ -10787,26 +10748,20 @@
       <c r="C52" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="H52" s="22" t="str">
         <f>VLOOKUP(A52,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I52" s="24" t="str">
         <f>IF(OR(COUNTIF(D52:G52,"X")=0,COUNTIF(D52:G52,"B")&lt;&gt;0),"X","")</f>
-        <v/>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>430</v>
+        <v>X</v>
       </c>
       <c r="K52">
         <f>VLOOKUP(A52,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.34674987200000001</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -10828,6 +10783,9 @@
         <f>IF(OR(COUNTIF(D53:G53,"X")=0,COUNTIF(D53:G53,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
+      <c r="J53" s="13" t="s">
+        <v>429</v>
+      </c>
       <c r="K53">
         <f>VLOOKUP(A53,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>26.620192639999999</v>
@@ -10881,7 +10839,7 @@
         <v>5.6287183719999998</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -10959,7 +10917,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -10981,9 +10939,6 @@
         <f>IF(OR(COUNTIF(D59:G59,"X")=0,COUNTIF(D59:G59,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J59" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K59">
         <f>VLOOKUP(A59,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>4.0453719340000003</v>
@@ -11008,12 +10963,15 @@
         <f>IF(OR(COUNTIF(D60:G60,"X")=0,COUNTIF(D60:G60,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
+      <c r="J60" s="13" t="s">
+        <v>429</v>
+      </c>
       <c r="K60">
         <f>VLOOKUP(A60,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>9.1646354429999999</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -11024,7 +10982,7 @@
       <c r="C61" t="s">
         <v>159</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="E61" s="29" t="s">
         <v>180</v>
       </c>
       <c r="H61" s="22" t="str">
@@ -11086,9 +11044,6 @@
         <f>IF(OR(COUNTIF(D63:G63,"X")=0,COUNTIF(D63:G63,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J63" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K63">
         <f>VLOOKUP(A63,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1</v>
@@ -11118,7 +11073,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -11141,7 +11096,7 @@
         <v/>
       </c>
       <c r="J65" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K65">
         <f>VLOOKUP(A65,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11171,7 +11126,7 @@
         <v/>
       </c>
       <c r="J66" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K66">
         <f>VLOOKUP(A66,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11200,9 +11155,6 @@
         <f>IF(OR(COUNTIF(D67:G67,"X")=0,COUNTIF(D67:G67,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J67" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K67">
         <f>VLOOKUP(A67,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.62</v>
@@ -11232,7 +11184,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -11278,9 +11230,6 @@
         <f>IF(OR(COUNTIF(D70:G70,"X")=0,COUNTIF(D70:G70,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J70" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K70">
         <f>VLOOKUP(A70,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>1000.68</v>
@@ -11309,14 +11258,14 @@
         <v/>
       </c>
       <c r="J71" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K71">
         <f>VLOOKUP(A71,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>2.8553917279999999</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -11339,14 +11288,14 @@
         <v/>
       </c>
       <c r="J72" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K72">
         <f>VLOOKUP(A72,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>27</v>
       </c>
@@ -11365,9 +11314,6 @@
         <f>IF(OR(COUNTIF(D73:G73,"X")=0,COUNTIF(D73:G73,"B")&lt;&gt;0),"X","")</f>
         <v>X</v>
       </c>
-      <c r="J73" s="13" t="s">
-        <v>431</v>
-      </c>
       <c r="K73">
         <f>VLOOKUP(A73,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>4.5705284319999997</v>
@@ -11397,7 +11343,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>45</v>
       </c>
@@ -11408,19 +11354,16 @@
       <c r="C75" t="s">
         <v>134</v>
       </c>
-      <c r="D75" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="H75" s="22" t="str">
         <f>VLOOKUP(A75,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I75" s="24" t="str">
         <f>IF(OR(COUNTIF(D75:G75,"X")=0,COUNTIF(D75:G75,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J75" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K75">
         <f>VLOOKUP(A75,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11438,26 +11381,20 @@
       <c r="C76" t="s">
         <v>133</v>
       </c>
-      <c r="D76" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="H76" s="22" t="str">
         <f>VLOOKUP(A76,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I76" s="24" t="str">
         <f>IF(OR(COUNTIF(D76:G76,"X")=0,COUNTIF(D76:G76,"B")&lt;&gt;0),"X","")</f>
-        <v/>
-      </c>
-      <c r="J76" s="13" t="s">
-        <v>430</v>
+        <v>X</v>
       </c>
       <c r="K76">
         <f>VLOOKUP(A76,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>25.449904530000001</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -11480,7 +11417,7 @@
         <v/>
       </c>
       <c r="J77" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K77">
         <f>VLOOKUP(A77,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11510,14 +11447,14 @@
         <v/>
       </c>
       <c r="J78" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K78">
         <f>VLOOKUP(A78,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>26.855260869999999</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>38</v>
       </c>
@@ -11539,15 +11476,12 @@
         <f>IF(OR(COUNTIF(D79:G79,"X")=0,COUNTIF(D79:G79,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J79" s="13" t="s">
-        <v>429</v>
-      </c>
       <c r="K79">
         <f>VLOOKUP(A79,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>5.5777170800000002</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -11570,7 +11504,7 @@
         <v/>
       </c>
       <c r="J80" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K80">
         <f>VLOOKUP(A80,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11601,7 +11535,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -11645,6 +11579,7 @@
       <c r="D83" s="22" t="s">
         <v>180</v>
       </c>
+      <c r="E83" s="29"/>
       <c r="H83" s="22" t="str">
         <f>VLOOKUP(A83,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
@@ -11654,7 +11589,7 @@
         <v/>
       </c>
       <c r="J83" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K83">
         <f>VLOOKUP(A83,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11672,16 +11607,13 @@
       <c r="C84" t="s">
         <v>98</v>
       </c>
-      <c r="D84" s="22" t="s">
-        <v>180</v>
-      </c>
       <c r="H84" s="22" t="str">
         <f>VLOOKUP(A84,'Init Scalar '!$A$2:$H$90,7,FALSE)</f>
         <v>X</v>
       </c>
       <c r="I84" s="24" t="str">
         <f>IF(OR(COUNTIF(D84:G84,"X")=0,COUNTIF(D84:G84,"B")&lt;&gt;0),"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J84" s="13" t="s">
         <v>429</v>
@@ -11691,7 +11623,7 @@
         <v>15.394965300000001</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>51</v>
       </c>
@@ -11721,7 +11653,7 @@
         <v>15.126177269999999</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -11743,15 +11675,12 @@
         <f>IF(OR(COUNTIF(D86:G86,"X")=0,COUNTIF(D86:G86,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J86" s="13" t="s">
-        <v>429</v>
-      </c>
       <c r="K86">
         <f>VLOOKUP(A86,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>2.0841953969999998</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -11773,9 +11702,6 @@
         <f>IF(OR(COUNTIF(D87:G87,"X")=0,COUNTIF(D87:G87,"B")&lt;&gt;0),"X","")</f>
         <v/>
       </c>
-      <c r="J87" s="13" t="s">
-        <v>430</v>
-      </c>
       <c r="K87">
         <f>VLOOKUP(A87,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
         <v>3.05</v>
@@ -11804,7 +11730,7 @@
         <v/>
       </c>
       <c r="J88" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K88">
         <f>VLOOKUP(A88,'Init Scalar '!$A$2:$H$90,6,FALSE)</f>
@@ -11813,10 +11739,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K88">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="worse"/>
-      </filters>
+    <filterColumn colId="8">
+      <filters blank="1"/>
     </filterColumn>
     <sortState ref="A2:K88">
       <sortCondition ref="C1:C88"/>
@@ -13440,9 +13364,9 @@
       <c r="C8" t="s">
         <v>93</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8">
         <f>VLOOKUP(A8,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -13452,9 +13376,9 @@
       <c r="C9" t="s">
         <v>112</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9">
         <f>VLOOKUP(A9,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -13962,9 +13886,9 @@
       <c r="C35" t="s">
         <v>92</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="str">
         <f>VLOOKUP(A35,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="F35">
         <v>28</v>
@@ -14115,9 +14039,9 @@
       <c r="C43" t="s">
         <v>111</v>
       </c>
-      <c r="E43" t="str">
+      <c r="E43">
         <f>VLOOKUP(A43,'Group Condition'!$A$2:$I$88,7,FALSE)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>10</v>
@@ -14901,19 +14825,19 @@
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D9" si="0">IF(F2="X","H",IF(G2="X","L",IF(H2="X","C","G")))</f>
-        <v>G</v>
+        <v>L</v>
       </c>
       <c r="E2" s="34" t="str">
         <f>IF('Group Condition'!J40="","",'Group Condition'!J40)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F2" s="34">
         <f>'Group Condition'!D40</f>
         <v>0</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="34" t="str">
         <f>'Group Condition'!E40</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="H2" s="34">
         <f>'Group Condition'!G40</f>
@@ -14921,7 +14845,7 @@
       </c>
       <c r="I2" s="34" t="str">
         <f>'Group Condition'!I40</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="L2" s="13" t="s">
         <v>423</v>
@@ -14948,15 +14872,15 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="E3" s="34" t="str">
         <f>IF('Group Condition'!J3="","",'Group Condition'!J3)</f>
         <v>better</v>
       </c>
-      <c r="F3" s="34" t="str">
+      <c r="F3" s="34">
         <f>'Group Condition'!D3</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G3" s="34">
         <f>'Group Condition'!E3</f>
@@ -14968,7 +14892,7 @@
       </c>
       <c r="I3" s="34" t="str">
         <f>'Group Condition'!I3</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J3"/>
       <c r="K3"/>
@@ -14993,7 +14917,7 @@
       </c>
       <c r="E4" s="34" t="str">
         <f>IF('Group Condition'!J4="","",'Group Condition'!J4)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F4" s="34">
         <f>'Group Condition'!D4</f>
@@ -15075,7 +14999,7 @@
       </c>
       <c r="E6" s="34" t="str">
         <f>IF('Group Condition'!J6="","",'Group Condition'!J6)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F6" s="34">
         <f>'Group Condition'!D6</f>
@@ -15113,7 +15037,7 @@
       </c>
       <c r="E7" s="34" t="str">
         <f>IF('Group Condition'!J33="","",'Group Condition'!J33)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F7" s="34">
         <f>'Group Condition'!D33</f>
@@ -15153,23 +15077,23 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>H</v>
       </c>
       <c r="E8" s="34" t="str">
         <f>IF('Group Condition'!J8="","",'Group Condition'!J8)</f>
         <v>worse</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="34" t="str">
         <f>'Group Condition'!D8</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G8" s="34">
         <f>'Group Condition'!E8</f>
         <v>0</v>
       </c>
-      <c r="H8" s="34" t="str">
+      <c r="H8" s="34">
         <f>'Group Condition'!G8</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="I8" s="34" t="str">
         <f>'Group Condition'!I8</f>
@@ -15191,11 +15115,11 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>G</v>
       </c>
       <c r="E9" s="34" t="str">
         <f>IF('Group Condition'!J9="","",'Group Condition'!J9)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F9" s="34">
         <f>'Group Condition'!D9</f>
@@ -15205,13 +15129,13 @@
         <f>'Group Condition'!E9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="34" t="str">
+      <c r="H9" s="34">
         <f>'Group Condition'!G9</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="I9" s="34" t="str">
         <f>'Group Condition'!I9</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -15236,7 +15160,7 @@
       </c>
       <c r="E10" s="34" t="str">
         <f>IF('Group Condition'!J50="","",'Group Condition'!J50)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F10" s="34">
         <f>'Group Condition'!D50</f>
@@ -15277,7 +15201,7 @@
       </c>
       <c r="E11" s="34" t="str">
         <f>IF('Group Condition'!J32="","",'Group Condition'!J32)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F11" s="34">
         <f>'Group Condition'!D32</f>
@@ -15320,7 +15244,7 @@
       </c>
       <c r="E12" s="34" t="str">
         <f>IF('Group Condition'!J12="","",'Group Condition'!J12)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F12" s="34">
         <f>'Group Condition'!D12</f>
@@ -15430,7 +15354,7 @@
       </c>
       <c r="E15" s="34" t="str">
         <f>IF('Group Condition'!J65="","",'Group Condition'!J65)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F15" s="34" t="str">
         <f>'Group Condition'!D65</f>
@@ -15474,7 +15398,7 @@
       </c>
       <c r="E16" s="34" t="str">
         <f>IF('Group Condition'!J15="","",'Group Condition'!J15)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F16" s="34">
         <f>'Group Condition'!D15</f>
@@ -15515,7 +15439,7 @@
       </c>
       <c r="E17" s="34" t="str">
         <f>IF('Group Condition'!J17="","",'Group Condition'!J17)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F17" s="34" t="str">
         <f>'Group Condition'!D17</f>
@@ -15588,7 +15512,7 @@
       </c>
       <c r="E19" s="34" t="str">
         <f>IF('Group Condition'!J19="","",'Group Condition'!J19)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F19" s="34" t="str">
         <f>'Group Condition'!D19</f>
@@ -15619,15 +15543,15 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="E20" s="34" t="str">
         <f>IF('Group Condition'!J20="","",'Group Condition'!J20)</f>
-        <v>better</v>
-      </c>
-      <c r="F20" s="34" t="str">
+        <v/>
+      </c>
+      <c r="F20" s="34">
         <f>'Group Condition'!D20</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G20" s="34">
         <f>'Group Condition'!E20</f>
@@ -15639,7 +15563,7 @@
       </c>
       <c r="I20" s="34" t="str">
         <f>'Group Condition'!I20</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
@@ -15660,15 +15584,15 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>H</v>
       </c>
       <c r="E21" s="34" t="str">
         <f>IF('Group Condition'!J21="","",'Group Condition'!J21)</f>
-        <v>better</v>
-      </c>
-      <c r="F21" s="34">
+        <v>spike</v>
+      </c>
+      <c r="F21" s="34" t="str">
         <f>'Group Condition'!D21</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G21" s="34" t="str">
         <f>'Group Condition'!E21</f>
@@ -15829,7 +15753,7 @@
       </c>
       <c r="E25" s="34" t="str">
         <f>IF('Group Condition'!J25="","",'Group Condition'!J25)</f>
-        <v/>
+        <v>better</v>
       </c>
       <c r="F25" s="34" t="str">
         <f>'Group Condition'!D25</f>
@@ -15866,19 +15790,19 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
-        <v>L</v>
+        <v>G</v>
       </c>
       <c r="E26" s="34" t="str">
         <f>IF('Group Condition'!J10="","",'Group Condition'!J10)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F26" s="34">
         <f>'Group Condition'!D10</f>
         <v>0</v>
       </c>
-      <c r="G26" s="34" t="str">
+      <c r="G26" s="34">
         <f>'Group Condition'!E10</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="H26" s="34">
         <f>'Group Condition'!G10</f>
@@ -15886,7 +15810,7 @@
       </c>
       <c r="I26" s="34" t="str">
         <f>'Group Condition'!I10</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>410</v>
@@ -15913,19 +15837,19 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
-        <v>H</v>
+        <v>L</v>
       </c>
       <c r="E27" s="34" t="str">
         <f>IF('Group Condition'!J27="","",'Group Condition'!J27)</f>
         <v>worse</v>
       </c>
-      <c r="F27" s="34" t="str">
+      <c r="F27" s="34">
         <f>'Group Condition'!D27</f>
-        <v>X</v>
-      </c>
-      <c r="G27" s="34">
+        <v>0</v>
+      </c>
+      <c r="G27" s="34" t="str">
         <f>'Group Condition'!E27</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="H27" s="34">
         <f>'Group Condition'!G27</f>
@@ -16046,7 +15970,7 @@
       </c>
       <c r="E30" s="34" t="str">
         <f>IF('Group Condition'!J44="","",'Group Condition'!J44)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F30" s="34">
         <f>'Group Condition'!D44</f>
@@ -16127,7 +16051,7 @@
       </c>
       <c r="E32" s="34" t="str">
         <f>IF('Group Condition'!J42="","",'Group Condition'!J42)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F32" s="34" t="str">
         <f>'Group Condition'!D42</f>
@@ -16252,11 +16176,11 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="1"/>
-        <v>G</v>
+        <v>C</v>
       </c>
       <c r="E35" s="34" t="str">
         <f>IF('Group Condition'!J35="","",'Group Condition'!J35)</f>
-        <v>better</v>
+        <v>zero?</v>
       </c>
       <c r="F35" s="34">
         <f>'Group Condition'!D35</f>
@@ -16266,13 +16190,13 @@
         <f>'Group Condition'!E35</f>
         <v>0</v>
       </c>
-      <c r="H35" s="34">
+      <c r="H35" s="34" t="str">
         <f>'Group Condition'!G35</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="I35" s="34" t="str">
         <f>'Group Condition'!I35</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J35"/>
       <c r="K35"/>
@@ -16385,7 +16309,7 @@
       </c>
       <c r="E38" s="34" t="str">
         <f>IF('Group Condition'!J38="","",'Group Condition'!J38)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F38" s="34">
         <f>'Group Condition'!D38</f>
@@ -16422,19 +16346,19 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
-        <v>H</v>
+        <v>L</v>
       </c>
       <c r="E39" s="34" t="str">
         <f>IF('Group Condition'!J39="","",'Group Condition'!J39)</f>
-        <v>worse</v>
-      </c>
-      <c r="F39" s="34" t="str">
+        <v>zero?</v>
+      </c>
+      <c r="F39" s="34">
         <f>'Group Condition'!D39</f>
-        <v>X</v>
-      </c>
-      <c r="G39" s="34">
+        <v>0</v>
+      </c>
+      <c r="G39" s="34" t="str">
         <f>'Group Condition'!E39</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="H39" s="34">
         <f>'Group Condition'!G39</f>
@@ -16500,15 +16424,15 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E41" s="34" t="str">
         <f>IF('Group Condition'!J41="","",'Group Condition'!J41)</f>
         <v>better</v>
       </c>
-      <c r="F41" s="34">
+      <c r="F41" s="34" t="str">
         <f>'Group Condition'!D41</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="G41" s="34">
         <f>'Group Condition'!E41</f>
@@ -16520,7 +16444,7 @@
       </c>
       <c r="I41" s="34" t="str">
         <f>'Group Condition'!I41</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J41" s="13" t="s">
         <v>410</v>
@@ -16551,7 +16475,7 @@
       </c>
       <c r="E42" s="34" t="str">
         <f>IF('Group Condition'!J67="","",'Group Condition'!J67)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F42" s="34">
         <f>'Group Condition'!D67</f>
@@ -16592,11 +16516,11 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="2"/>
-        <v>C</v>
+        <v>G</v>
       </c>
       <c r="E43" s="34" t="str">
         <f>IF('Group Condition'!J43="","",'Group Condition'!J43)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F43" s="34">
         <f>'Group Condition'!D43</f>
@@ -16606,13 +16530,13 @@
         <f>'Group Condition'!E43</f>
         <v>0</v>
       </c>
-      <c r="H43" s="34" t="str">
+      <c r="H43" s="34">
         <f>'Group Condition'!G43</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="I43" s="34" t="str">
         <f>'Group Condition'!I43</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J43"/>
       <c r="K43"/>
@@ -16637,7 +16561,7 @@
       </c>
       <c r="E44" s="34" t="str">
         <f>IF('Group Condition'!J51="","",'Group Condition'!J51)</f>
-        <v/>
+        <v>worse</v>
       </c>
       <c r="F44" s="34" t="str">
         <f>'Group Condition'!D51</f>
@@ -16714,7 +16638,7 @@
       </c>
       <c r="E46" s="34" t="str">
         <f>IF('Group Condition'!J46="","",'Group Condition'!J46)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F46" s="34" t="str">
         <f>'Group Condition'!D46</f>
@@ -16755,7 +16679,7 @@
       </c>
       <c r="E47" s="34" t="str">
         <f>IF('Group Condition'!J47="","",'Group Condition'!J47)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F47" s="34">
         <f>'Group Condition'!D47</f>
@@ -16796,7 +16720,7 @@
       </c>
       <c r="E48" s="34" t="str">
         <f>IF('Group Condition'!J48="","",'Group Condition'!J48)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F48" s="34" t="str">
         <f>'Group Condition'!D48</f>
@@ -16831,7 +16755,7 @@
       </c>
       <c r="E49" s="34" t="str">
         <f>IF('Group Condition'!J49="","",'Group Condition'!J49)</f>
-        <v>no change</v>
+        <v>better</v>
       </c>
       <c r="F49" s="34">
         <f>'Group Condition'!D49</f>
@@ -16956,15 +16880,15 @@
       </c>
       <c r="D52" t="str">
         <f t="shared" si="2"/>
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="E52" s="34" t="str">
         <f>IF('Group Condition'!J52="","",'Group Condition'!J52)</f>
-        <v>no change</v>
-      </c>
-      <c r="F52" s="34" t="str">
+        <v/>
+      </c>
+      <c r="F52" s="34">
         <f>'Group Condition'!D52</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G52" s="34">
         <f>'Group Condition'!E52</f>
@@ -16976,7 +16900,7 @@
       </c>
       <c r="I52" s="34" t="str">
         <f>'Group Condition'!I52</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J52"/>
       <c r="K52"/>
@@ -17001,7 +16925,7 @@
       </c>
       <c r="E53" s="34" t="str">
         <f>IF('Group Condition'!J53="","",'Group Condition'!J53)</f>
-        <v/>
+        <v>better</v>
       </c>
       <c r="F53" s="34" t="str">
         <f>'Group Condition'!D53</f>
@@ -17119,7 +17043,7 @@
       </c>
       <c r="E56" s="34" t="str">
         <f>IF('Group Condition'!J56="","",'Group Condition'!J56)</f>
-        <v>no change</v>
+        <v>worse</v>
       </c>
       <c r="F56" s="34">
         <f>'Group Condition'!D56</f>
@@ -17245,7 +17169,7 @@
       </c>
       <c r="E59" s="34" t="str">
         <f>IF('Group Condition'!J59="","",'Group Condition'!J59)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F59" s="34" t="str">
         <f>'Group Condition'!D59</f>
@@ -17286,7 +17210,7 @@
       </c>
       <c r="E60" s="34" t="str">
         <f>IF('Group Condition'!J60="","",'Group Condition'!J60)</f>
-        <v/>
+        <v>better</v>
       </c>
       <c r="F60" s="34">
         <f>'Group Condition'!D60</f>
@@ -17327,7 +17251,7 @@
       </c>
       <c r="E61" s="34" t="str">
         <f>IF('Group Condition'!J22="","",'Group Condition'!J22)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F61" s="34">
         <f>'Group Condition'!D22</f>
@@ -17403,7 +17327,7 @@
       </c>
       <c r="E63" s="34" t="str">
         <f>IF('Group Condition'!J63="","",'Group Condition'!J63)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F63" s="34">
         <f>'Group Condition'!D63</f>
@@ -17437,19 +17361,19 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="2"/>
-        <v>H</v>
+        <v>L</v>
       </c>
       <c r="E64" s="34" t="str">
         <f>IF('Group Condition'!J61="","",'Group Condition'!J61)</f>
         <v>better</v>
       </c>
-      <c r="F64" s="34" t="str">
+      <c r="F64" s="34">
         <f>'Group Condition'!D61</f>
-        <v>X</v>
-      </c>
-      <c r="G64" s="34">
+        <v>0</v>
+      </c>
+      <c r="G64" s="34" t="str">
         <f>'Group Condition'!E61</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="H64" s="34">
         <f>'Group Condition'!G61</f>
@@ -17482,7 +17406,7 @@
       </c>
       <c r="E65" s="34" t="str">
         <f>IF('Group Condition'!J71="","",'Group Condition'!J71)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F65" s="34" t="str">
         <f>'Group Condition'!D71</f>
@@ -17519,7 +17443,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="2"/>
-        <v>G</v>
+        <v>L</v>
       </c>
       <c r="E66" s="34" t="str">
         <f>IF('Group Condition'!J45="","",'Group Condition'!J45)</f>
@@ -17529,9 +17453,9 @@
         <f>'Group Condition'!D45</f>
         <v>0</v>
       </c>
-      <c r="G66" s="34">
+      <c r="G66" s="34" t="str">
         <f>'Group Condition'!E45</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="H66" s="34">
         <f>'Group Condition'!G45</f>
@@ -17539,7 +17463,7 @@
       </c>
       <c r="I66" s="34" t="str">
         <f>'Group Condition'!I45</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J66"/>
       <c r="K66"/>
@@ -17566,7 +17490,7 @@
       </c>
       <c r="E67" s="34" t="str">
         <f>IF('Group Condition'!J72="","",'Group Condition'!J72)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F67" s="34" t="str">
         <f>'Group Condition'!D72</f>
@@ -17696,7 +17620,7 @@
       </c>
       <c r="E70" s="34" t="str">
         <f>IF('Group Condition'!J70="","",'Group Condition'!J70)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F70" s="34">
         <f>'Group Condition'!D70</f>
@@ -17737,7 +17661,7 @@
       </c>
       <c r="E71" s="34" t="str">
         <f>IF('Group Condition'!J77="","",'Group Condition'!J77)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F71" s="34" t="str">
         <f>'Group Condition'!D77</f>
@@ -17852,7 +17776,7 @@
       </c>
       <c r="E74" s="34" t="str">
         <f>IF('Group Condition'!J78="","",'Group Condition'!J78)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F74" s="34">
         <f>'Group Condition'!D78</f>
@@ -17889,15 +17813,15 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="3"/>
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="E75" s="34" t="str">
         <f>IF('Group Condition'!J75="","",'Group Condition'!J75)</f>
         <v>worse</v>
       </c>
-      <c r="F75" s="34" t="str">
+      <c r="F75" s="34">
         <f>'Group Condition'!D75</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G75" s="34">
         <f>'Group Condition'!E75</f>
@@ -17909,7 +17833,7 @@
       </c>
       <c r="I75" s="34" t="str">
         <f>'Group Condition'!I75</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J75"/>
       <c r="K75"/>
@@ -17930,11 +17854,11 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="3"/>
-        <v>H</v>
-      </c>
-      <c r="F76" s="34" t="str">
+        <v>G</v>
+      </c>
+      <c r="F76" s="34">
         <f>'Group Condition'!D76</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G76" s="34">
         <f>'Group Condition'!E76</f>
@@ -17946,7 +17870,7 @@
       </c>
       <c r="I76" s="34" t="str">
         <f>'Group Condition'!I76</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J76"/>
       <c r="K76"/>
@@ -18015,7 +17939,7 @@
       </c>
       <c r="E78" s="34" t="str">
         <f>IF('Group Condition'!J73="","",'Group Condition'!J73)</f>
-        <v>worse</v>
+        <v/>
       </c>
       <c r="F78" s="34">
         <f>'Group Condition'!D73</f>
@@ -18056,7 +17980,7 @@
       </c>
       <c r="E79" s="34" t="str">
         <f>IF('Group Condition'!J79="","",'Group Condition'!J79)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F79" s="34" t="str">
         <f>'Group Condition'!D79</f>
@@ -18126,7 +18050,7 @@
       </c>
       <c r="E81" s="34" t="str">
         <f>IF('Group Condition'!J86="","",'Group Condition'!J86)</f>
-        <v>better</v>
+        <v/>
       </c>
       <c r="F81" s="34" t="str">
         <f>'Group Condition'!D86</f>
@@ -18167,7 +18091,7 @@
       </c>
       <c r="E82" s="34" t="str">
         <f>IF('Group Condition'!J83="","",'Group Condition'!J83)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F82" s="34" t="str">
         <f>'Group Condition'!D83</f>
@@ -18202,7 +18126,7 @@
       </c>
       <c r="E83" s="34" t="str">
         <f>IF('Group Condition'!J80="","",'Group Condition'!J80)</f>
-        <v>better</v>
+        <v>worse</v>
       </c>
       <c r="F83" s="34" t="str">
         <f>'Group Condition'!D80</f>
@@ -18239,15 +18163,15 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" si="3"/>
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="E84" s="34" t="str">
         <f>IF('Group Condition'!J84="","",'Group Condition'!J84)</f>
         <v>better</v>
       </c>
-      <c r="F84" s="34" t="str">
+      <c r="F84" s="34">
         <f>'Group Condition'!D84</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="G84" s="34">
         <f>'Group Condition'!E84</f>
@@ -18259,7 +18183,7 @@
       </c>
       <c r="I84" s="34" t="str">
         <f>'Group Condition'!I84</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J84"/>
       <c r="K84"/>
@@ -18284,7 +18208,7 @@
       </c>
       <c r="E85" s="34" t="str">
         <f>IF('Group Condition'!J66="","",'Group Condition'!J66)</f>
-        <v>worse</v>
+        <v>better</v>
       </c>
       <c r="F85" s="34" t="str">
         <f>'Group Condition'!D66</f>
@@ -18363,7 +18287,7 @@
       </c>
       <c r="E87" s="34" t="str">
         <f>IF('Group Condition'!J87="","",'Group Condition'!J87)</f>
-        <v>no change</v>
+        <v/>
       </c>
       <c r="F87" s="34" t="str">
         <f>'Group Condition'!D87</f>
@@ -18531,13 +18455,13 @@
         <v>424</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -18556,7 +18480,7 @@
       </c>
       <c r="E2" s="7" t="str">
         <f>VLOOKUP(A2,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F2" s="6">
         <v>532233758.39999998</v>
@@ -18830,7 +18754,7 @@
       </c>
       <c r="E8" s="7" t="str">
         <f>VLOOKUP(A8,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F8" s="6">
         <v>1080000</v>
@@ -18999,7 +18923,7 @@
       </c>
       <c r="E12" s="7" t="str">
         <f>VLOOKUP(A12,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F12" s="6">
         <v>6384375</v>
@@ -19052,7 +18976,7 @@
       </c>
       <c r="E13" s="7" t="str">
         <f>VLOOKUP(A13,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F13" s="6">
         <v>8500000</v>
@@ -19209,7 +19133,7 @@
       </c>
       <c r="E17" s="7" t="str">
         <f>VLOOKUP(A17,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F17" s="6">
         <v>4986608.142</v>
@@ -19264,7 +19188,7 @@
       </c>
       <c r="E18" s="7" t="str">
         <f>VLOOKUP(A18,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F18" s="6">
         <v>4000000</v>
@@ -19408,7 +19332,7 @@
       </c>
       <c r="E21" s="7" t="str">
         <f>VLOOKUP(A21,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F21" s="6">
         <v>2430000</v>
@@ -19451,7 +19375,7 @@
       </c>
       <c r="E22" s="7" t="str">
         <f>VLOOKUP(A22,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F22" s="6">
         <v>321227180.55000001</v>
@@ -19992,7 +19916,7 @@
       </c>
       <c r="E34" s="7" t="str">
         <f>VLOOKUP(A34,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F34" s="6">
         <v>2123.8950410000002</v>
@@ -20392,7 +20316,7 @@
       </c>
       <c r="E43" s="7" t="str">
         <f>VLOOKUP(A43,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F43" s="6">
         <v>176000000</v>
@@ -20432,7 +20356,7 @@
       </c>
       <c r="E44" s="7" t="str">
         <f>VLOOKUP(A44,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F44" s="6">
         <v>250000</v>
@@ -21166,7 +21090,7 @@
       </c>
       <c r="E63" s="7" t="str">
         <f>VLOOKUP(A63,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F63" s="6">
         <v>1.2500000000000001E-2</v>
@@ -21372,16 +21296,16 @@
         <v>426</v>
       </c>
       <c r="T1" t="s">
+        <v>432</v>
+      </c>
+      <c r="U1" t="s">
         <v>433</v>
       </c>
-      <c r="U1" t="s">
-        <v>434</v>
-      </c>
       <c r="V1" t="s">
+        <v>437</v>
+      </c>
+      <c r="W1" t="s">
         <v>438</v>
-      </c>
-      <c r="W1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -21403,7 +21327,7 @@
       </c>
       <c r="F2" s="7" t="str">
         <f>VLOOKUP(A2,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K2">
         <f>VLOOKUP(A2,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -21661,7 +21585,7 @@
       </c>
       <c r="F8" s="7" t="str">
         <f>VLOOKUP(A8,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K8">
         <f>VLOOKUP(A8,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -21829,7 +21753,7 @@
       </c>
       <c r="F12" s="7" t="str">
         <f>VLOOKUP(A12,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K12">
         <f>VLOOKUP(A12,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -21871,7 +21795,7 @@
       </c>
       <c r="F13" s="7" t="str">
         <f>VLOOKUP(A13,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K13">
         <f>VLOOKUP(A13,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22107,7 +22031,7 @@
       </c>
       <c r="F17" s="7" t="str">
         <f>VLOOKUP(A17,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K17">
         <f>VLOOKUP(A17,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22155,7 +22079,7 @@
       </c>
       <c r="F18" s="7" t="str">
         <f>VLOOKUP(A18,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K18">
         <f>VLOOKUP(A18,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22293,7 +22217,7 @@
       </c>
       <c r="F21" s="7" t="str">
         <f>VLOOKUP(A21,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K21">
         <f>VLOOKUP(A21,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -22335,7 +22259,7 @@
       </c>
       <c r="F22" s="7" t="str">
         <f>VLOOKUP(A22,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G22" s="14">
         <v>1.0000000000000001E-15</v>
@@ -22871,7 +22795,7 @@
       </c>
       <c r="F34" s="7" t="str">
         <f>VLOOKUP(A34,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K34">
         <f>VLOOKUP(A34,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23249,7 +23173,7 @@
       </c>
       <c r="F43" s="7" t="str">
         <f>VLOOKUP(A43,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K43">
         <f>VLOOKUP(A43,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -23291,7 +23215,7 @@
       </c>
       <c r="F44" s="7" t="str">
         <f>VLOOKUP(A44,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K44">
         <f>VLOOKUP(A44,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -24135,7 +24059,7 @@
       </c>
       <c r="F63" s="7" t="str">
         <f>VLOOKUP(A63,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K63">
         <f>VLOOKUP(A63,[3]mL!$A$2:$C$87,3,FALSE)</f>
@@ -24321,22 +24245,22 @@
         <v>428</v>
       </c>
       <c r="Z1" t="s">
+        <v>434</v>
+      </c>
+      <c r="AA1" t="s">
         <v>435</v>
       </c>
-      <c r="AA1" t="s">
-        <v>436</v>
-      </c>
       <c r="AB1" t="s">
+        <v>439</v>
+      </c>
+      <c r="AC1" t="s">
         <v>440</v>
       </c>
-      <c r="AC1" t="s">
-        <v>441</v>
-      </c>
       <c r="AD1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AE1" t="s">
         <v>443</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -24358,7 +24282,7 @@
       </c>
       <c r="F2" s="7" t="str">
         <f>VLOOKUP(A2,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="G2">
         <f>D2*1.25</f>
@@ -24787,7 +24711,7 @@
       </c>
       <c r="F8" s="7" t="str">
         <f>VLOOKUP(A8,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G8">
         <f>D8*0.5</f>
@@ -25054,7 +24978,7 @@
       </c>
       <c r="F12" s="7" t="str">
         <f>VLOOKUP(A12,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H12"/>
       <c r="Q12">
@@ -25105,7 +25029,7 @@
       </c>
       <c r="F13" s="7" t="str">
         <f>VLOOKUP(A13,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G13">
         <f>D13*1.25</f>
@@ -25378,7 +25302,7 @@
       </c>
       <c r="F17" s="7" t="str">
         <f>VLOOKUP(A17,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="H17"/>
       <c r="Q17">
@@ -25449,7 +25373,7 @@
       </c>
       <c r="F18" s="7" t="str">
         <f>VLOOKUP(A18,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G18">
         <f>D18*0.5</f>
@@ -25627,7 +25551,7 @@
       </c>
       <c r="F21" s="7" t="str">
         <f>VLOOKUP(A21,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G21">
         <f>D21*0.5</f>
@@ -25705,7 +25629,7 @@
       </c>
       <c r="F22" s="7" t="str">
         <f>VLOOKUP(A22,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G22" s="14">
         <v>1.4999999999999999E-14</v>
@@ -26445,7 +26369,7 @@
       </c>
       <c r="F34" s="7" t="str">
         <f>VLOOKUP(A34,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="H34"/>
       <c r="Q34">
@@ -27083,7 +27007,7 @@
       </c>
       <c r="F43" s="7" t="str">
         <f>VLOOKUP(A43,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G43" s="14">
         <v>1E-13</v>
@@ -27149,7 +27073,7 @@
       </c>
       <c r="F44" s="7" t="str">
         <f>VLOOKUP(A44,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="G44">
         <f>D44*1.5</f>
@@ -28215,7 +28139,7 @@
       </c>
       <c r="F63" s="7" t="str">
         <f>VLOOKUP(A63,'Group Condition'!$A$2:$K$88,9,FALSE)</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="H63"/>
       <c r="Q63">

</xml_diff>